<commit_message>
changes to the extraction process
</commit_message>
<xml_diff>
--- a/QALD9-Plus-testing/CoT-entity-aligned/CoT-dbpedia-wikidata/comparison_results_llama_CoT_dbpedia_wikidata.xlsx
+++ b/QALD9-Plus-testing/CoT-entity-aligned/CoT-dbpedia-wikidata/comparison_results_llama_CoT_dbpedia_wikidata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,17 +458,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Who developed Skype?</t>
+          <t>Who is the founder of Penguin Books?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q246125']</t>
+          <t>['http://www.wikidata.org/entity/Q1263483']</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q246125']</t>
+          <t>['http://www.wikidata.org/entity/Q1263483']</t>
         </is>
       </c>
       <c r="D2" t="b">
@@ -478,37 +478,37 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Give me all actors starring in movies directed by William Shatner.</t>
+          <t>Which films did Stanley Kubrick direct?</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q110154', 'http://www.wikidata.org/entity/Q1209826', 'http://www.wikidata.org/entity/Q1396278', 'http://www.wikidata.org/entity/Q152773', 'http://www.wikidata.org/entity/Q16296', 'http://www.wikidata.org/entity/Q16297', 'http://www.wikidata.org/entity/Q16345', 'http://www.wikidata.org/entity/Q16349', 'http://www.wikidata.org/entity/Q190523', 'http://www.wikidata.org/entity/Q2263306', 'http://www.wikidata.org/entity/Q230038', 'http://www.wikidata.org/entity/Q231576', 'http://www.wikidata.org/entity/Q23466', 'http://www.wikidata.org/entity/Q2451563', 'http://www.wikidata.org/entity/Q254038', 'http://www.wikidata.org/entity/Q266391', 'http://www.wikidata.org/entity/Q2667506', 'http://www.wikidata.org/entity/Q272214', 'http://www.wikidata.org/entity/Q2805350', 'http://www.wikidata.org/entity/Q311699', 'http://www.wikidata.org/entity/Q313789', 'http://www.wikidata.org/entity/Q318412', 'http://www.wikidata.org/entity/Q346595', 'http://www.wikidata.org/entity/Q348445', 'http://www.wikidata.org/entity/Q356846', 'http://www.wikidata.org/entity/Q363271', 'http://www.wikidata.org/entity/Q366012', 'http://www.wikidata.org/entity/Q376176', 'http://www.wikidata.org/entity/Q444217', 'http://www.wikidata.org/entity/Q461794', 'http://www.wikidata.org/entity/Q5115837', 'http://www.wikidata.org/entity/Q5213941', 'http://www.wikidata.org/entity/Q550778', 'http://www.wikidata.org/entity/Q552103', 'http://www.wikidata.org/entity/Q6066272']</t>
+          <t>['http://www.wikidata.org/entity/Q103474', 'http://www.wikidata.org/entity/Q105702', 'http://www.wikidata.org/entity/Q108297', 'http://www.wikidata.org/entity/Q110624336', 'http://www.wikidata.org/entity/Q1434632', 'http://www.wikidata.org/entity/Q181086', 'http://www.wikidata.org/entity/Q186341', 'http://www.wikidata.org/entity/Q209481', 'http://www.wikidata.org/entity/Q2164458', 'http://www.wikidata.org/entity/Q243439', 'http://www.wikidata.org/entity/Q426628', 'http://www.wikidata.org/entity/Q471716', 'http://www.wikidata.org/entity/Q536560', 'http://www.wikidata.org/entity/Q592072', 'http://www.wikidata.org/entity/Q747936', 'http://www.wikidata.org/entity/Q929157', 'http://www.wikidata.org/entity/Q936477']</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q110154', 'http://www.wikidata.org/entity/Q16297', 'http://www.wikidata.org/entity/Q16345', 'http://www.wikidata.org/entity/Q16349', 'http://www.wikidata.org/entity/Q254038', 'http://www.wikidata.org/entity/Q2667506', 'http://www.wikidata.org/entity/Q318412', 'http://www.wikidata.org/entity/Q356846', 'http://www.wikidata.org/entity/Q363271', 'http://www.wikidata.org/entity/Q376176', 'http://www.wikidata.org/entity/Q1209826', 'http://www.wikidata.org/entity/Q152773', 'http://www.wikidata.org/entity/Q16297', 'http://www.wikidata.org/entity/Q2263306', 'http://www.wikidata.org/entity/Q2451563', 'http://www.wikidata.org/entity/Q2805350', 'http://www.wikidata.org/entity/Q444217', 'http://www.wikidata.org/entity/Q461794', 'http://www.wikidata.org/entity/Q5115837', 'http://www.wikidata.org/entity/Q5213941', 'http://www.wikidata.org/entity/Q116281', 'http://www.wikidata.org/entity/Q1320797', 'http://www.wikidata.org/entity/Q1338682', 'http://www.wikidata.org/entity/Q16297', 'http://www.wikidata.org/entity/Q1720634', 'http://www.wikidata.org/entity/Q18211660', 'http://www.wikidata.org/entity/Q234114', 'http://www.wikidata.org/entity/Q238168', 'http://www.wikidata.org/entity/Q2439878', 'http://www.wikidata.org/entity/Q2933924', 'http://www.wikidata.org/entity/Q2965115', 'http://www.wikidata.org/entity/Q3177047', 'http://www.wikidata.org/entity/Q3300864', 'http://www.wikidata.org/entity/Q3441429', 'http://www.wikidata.org/entity/Q3559413', 'http://www.wikidata.org/entity/Q378538', 'http://www.wikidata.org/entity/Q3852420', 'http://www.wikidata.org/entity/Q3877584', 'http://www.wikidata.org/entity/Q42329064', 'http://www.wikidata.org/entity/Q442025', 'http://www.wikidata.org/entity/Q504028', 'http://www.wikidata.org/entity/Q5407123', 'http://www.wikidata.org/entity/Q6308308', 'http://www.wikidata.org/entity/Q6811353', 'http://www.wikidata.org/entity/Q1396278', 'http://www.wikidata.org/entity/Q16296', 'http://www.wikidata.org/entity/Q16297', 'http://www.wikidata.org/entity/Q16345', 'http://www.wikidata.org/entity/Q16349', 'http://www.wikidata.org/entity/Q190523', 'http://www.wikidata.org/entity/Q230038', 'http://www.wikidata.org/entity/Q231576', 'http://www.wikidata.org/entity/Q23466', 'http://www.wikidata.org/entity/Q266391', 'http://www.wikidata.org/entity/Q272214', 'http://www.wikidata.org/entity/Q311699', 'http://www.wikidata.org/entity/Q313789', 'http://www.wikidata.org/entity/Q346595', 'http://www.wikidata.org/entity/Q348445', 'http://www.wikidata.org/entity/Q366012', 'http://www.wikidata.org/entity/Q376176', 'http://www.wikidata.org/entity/Q550778', 'http://www.wikidata.org/entity/Q552103', 'http://www.wikidata.org/entity/Q6066272']</t>
+          <t>['http://www.wikidata.org/entity/Q103474', 'http://www.wikidata.org/entity/Q105702', 'http://www.wikidata.org/entity/Q108297', 'http://www.wikidata.org/entity/Q110624336', 'http://www.wikidata.org/entity/Q1434632', 'http://www.wikidata.org/entity/Q181086', 'http://www.wikidata.org/entity/Q186341', 'http://www.wikidata.org/entity/Q209481', 'http://www.wikidata.org/entity/Q2164458', 'http://www.wikidata.org/entity/Q243439', 'http://www.wikidata.org/entity/Q426628', 'http://www.wikidata.org/entity/Q471716', 'http://www.wikidata.org/entity/Q536560', 'http://www.wikidata.org/entity/Q592072', 'http://www.wikidata.org/entity/Q747936', 'http://www.wikidata.org/entity/Q929157', 'http://www.wikidata.org/entity/Q936477']</t>
         </is>
       </c>
       <c r="D3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Which movies star both Liz Taylor and Richard Burton?</t>
+          <t>Who developed Skype?</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q1198059', 'http://www.wikidata.org/entity/Q1235065', 'http://www.wikidata.org/entity/Q1527877', 'http://www.wikidata.org/entity/Q1630930', 'http://www.wikidata.org/entity/Q2497114', 'http://www.wikidata.org/entity/Q325643', 'http://www.wikidata.org/entity/Q426314', 'http://www.wikidata.org/entity/Q4430', 'http://www.wikidata.org/entity/Q568696', 'http://www.wikidata.org/entity/Q634049', 'http://www.wikidata.org/entity/Q668569', 'http://www.wikidata.org/entity/Q910226']</t>
+          <t>['http://www.wikidata.org/entity/Q246125']</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q1198059', 'http://www.wikidata.org/entity/Q1235065', 'http://www.wikidata.org/entity/Q1527877', 'http://www.wikidata.org/entity/Q1630930', 'http://www.wikidata.org/entity/Q2497114', 'http://www.wikidata.org/entity/Q325643', 'http://www.wikidata.org/entity/Q426314', 'http://www.wikidata.org/entity/Q4430', 'http://www.wikidata.org/entity/Q568696', 'http://www.wikidata.org/entity/Q634049', 'http://www.wikidata.org/entity/Q668569', 'http://www.wikidata.org/entity/Q910226']</t>
+          <t>['http://www.wikidata.org/entity/Q246125']</t>
         </is>
       </c>
       <c r="D4" t="b">
@@ -518,17 +518,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Give me the runtime of Toy Story.</t>
+          <t>Which movies star both Liz Taylor and Richard Burton?</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>['81']</t>
+          <t>['http://www.wikidata.org/entity/Q1198059', 'http://www.wikidata.org/entity/Q1235065', 'http://www.wikidata.org/entity/Q1527877', 'http://www.wikidata.org/entity/Q1630930', 'http://www.wikidata.org/entity/Q2497114', 'http://www.wikidata.org/entity/Q325643', 'http://www.wikidata.org/entity/Q426314', 'http://www.wikidata.org/entity/Q4430', 'http://www.wikidata.org/entity/Q568696', 'http://www.wikidata.org/entity/Q634049', 'http://www.wikidata.org/entity/Q668569', 'http://www.wikidata.org/entity/Q910226']</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['81']</t>
+          <t>['http://www.wikidata.org/entity/Q1198059', 'http://www.wikidata.org/entity/Q1235065', 'http://www.wikidata.org/entity/Q1527877', 'http://www.wikidata.org/entity/Q1630930', 'http://www.wikidata.org/entity/Q2497114', 'http://www.wikidata.org/entity/Q325643', 'http://www.wikidata.org/entity/Q426314', 'http://www.wikidata.org/entity/Q4430', 'http://www.wikidata.org/entity/Q568696', 'http://www.wikidata.org/entity/Q634049', 'http://www.wikidata.org/entity/Q668569', 'http://www.wikidata.org/entity/Q910226']</t>
         </is>
       </c>
       <c r="D5" t="b">
@@ -538,17 +538,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Who was the doctoral supervisor of Albert Einstein?</t>
+          <t>Who developed Minecraft?</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q116635', 'http://www.wikidata.org/entity/Q4175282', 'http://www.wikidata.org/entity/Q97154']</t>
+          <t>['http://www.wikidata.org/entity/Q1129295', 'http://www.wikidata.org/entity/Q2283']</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q116635', 'http://www.wikidata.org/entity/Q4175282', 'http://www.wikidata.org/entity/Q97154']</t>
+          <t>['http://www.wikidata.org/entity/Q1129295', 'http://www.wikidata.org/entity/Q2283']</t>
         </is>
       </c>
       <c r="D6" t="b">
@@ -558,37 +558,37 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Who is the author of the interpretation of dreams?</t>
+          <t>What is the most frequent cause of death?</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q9215']</t>
+          <t>['http://www.wikidata.org/entity/Q12152']</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q9215']</t>
+          <t>['http://www.wikidata.org/entity/Q1324130']</t>
         </is>
       </c>
       <c r="D7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Which holidays are celebrated around the world?</t>
+          <t>What is the highest mountain in Italy?</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q103987830', 'http://www.wikidata.org/entity/Q104013369', 'http://www.wikidata.org/entity/Q116978631', 'http://www.wikidata.org/entity/Q21163268', 'http://www.wikidata.org/entity/Q10283187', 'http://www.wikidata.org/entity/Q111738564', 'http://www.wikidata.org/entity/Q112127159', 'http://www.wikidata.org/entity/Q124422802', 'http://www.wikidata.org/entity/Q18465013', 'http://www.wikidata.org/entity/Q125856465', 'http://www.wikidata.org/entity/Q1361434', 'http://www.wikidata.org/entity/Q1651570', 'http://www.wikidata.org/entity/Q2564633', 'http://www.wikidata.org/entity/Q333016', 'http://www.wikidata.org/entity/Q61359735', 'http://www.wikidata.org/entity/Q72318', 'http://www.wikidata.org/entity/Q744159', 'http://www.wikidata.org/entity/Q751738', 'http://www.wikidata.org/entity/Q110707177', 'http://www.wikidata.org/entity/Q45922130', 'http://www.wikidata.org/entity/Q57350935', 'http://www.wikidata.org/entity/Q57397044', 'http://www.wikidata.org/entity/Q116978568', 'http://www.wikidata.org/entity/Q2859605', 'http://www.wikidata.org/entity/Q113090457', 'http://www.wikidata.org/entity/Q115181793', 'http://www.wikidata.org/entity/Q115369110', 'http://www.wikidata.org/entity/Q115369980', 'http://www.wikidata.org/entity/Q115377287', 'http://www.wikidata.org/entity/Q21697589', 'http://www.wikidata.org/entity/Q122069654', 'http://www.wikidata.org/entity/Q1145566', 'http://www.wikidata.org/entity/Q11406184', 'http://www.wikidata.org/entity/Q11643728', 'http://www.wikidata.org/entity/Q20044441', 'http://www.wikidata.org/entity/Q28685931', 'http://www.wikidata.org/entity/Q11255045', 'http://www.wikidata.org/entity/Q11387821', 'http://www.wikidata.org/entity/Q11436695', 'http://www.wikidata.org/entity/Q11501518', 'http://www.wikidata.org/entity/Q11502138', 'http://www.wikidata.org/entity/Q11512398', 'http://www.wikidata.org/entity/Q11590440', 'http://www.wikidata.org/entity/Q11604982', 'http://www.wikidata.org/entity/Q6455253', 'http://www.wikidata.org/entity/Q111162467', 'http://www.wikidata.org/entity/Q124005660', 'http://www.wikidata.org/entity/Q130611902', 'http://www.wikidata.org/entity/Q13258770', 'http://www.wikidata.org/entity/Q2838743', 'http://www.wikidata.org/entity/Q3092925', 'http://www.wikidata.org/entity/Q123004384', 'http://www.wikidata.org/entity/Q4546230', 'http://www.wikidata.org/entity/Q1009535', 'http://www.wikidata.org/entity/Q1049141', 'http://www.wikidata.org/entity/Q1059995', 'http://www.wikidata.org/entity/Q1137351', 'http://www.wikidata.org/entity/Q1145630', 'http://www.wikidata.org/entity/Q1186410', 'http://www.wikidata.org/entity/Q1355051', 'http://www.wikidata.org/entity/Q1355833', 'http://www.wikidata.org/entity/Q1359602', 'http://www.wikidata.org/entity/Q1361434', 'http://www.wikidata.org/entity/Q1361489', 'http://www.wikidata.org/entity/Q17218111', 'http://www.wikidata.org/entity/Q483226', 'http://www.wikidata.org/entity/Q82405', 'http://www.wikidata.org/entity/Q101706322', 'http://www.wikidata.org/entity/Q10265921', 'http://www.wikidata.org/entity/Q10274', 'http://www.wikidata.org/entity/Q10281751', 'http://www.wikidata.org/entity/Q10313072', 'http://www.wikidata.org/entity/Q1034573', 'http://www.wikidata.org/entity/Q10379695', 'http://www.wikidata.org/entity/Q1038328', 'http://www.wikidata.org/entity/Q104842151', 'http://www.wikidata.org/entity/Q104842171', 'http://www.wikidata.org/entity/Q104844735', 'http://www.wikidata.org/entity/Q104853673', 'http://www.wikidata.org/entity/Q104861126', 'http://www.wikidata.org/entity/Q10488275', 'http://www.wikidata.org/entity/Q105047091', 'http://www.wikidata.org/entity/Q105047582', 'http://www.wikidata.org/entity/Q105047587', 'http://www.wikidata.org/entity/Q105271464', 'http://www.wikidata.org/entity/Q105393636', 'http://www.wikidata.org/entity/Q10560877', 'http://www.wikidata.org/entity/Q105742385', 'http://www.wikidata.org/entity/Q105742388', 'http://www.wikidata.org/entity/Q1058840', 'http://www.wikidata.org/entity/Q106010', 'http://www.wikidata.org/entity/Q106290028', 'http://www.wikidata.org/entity/Q106307776', 'http://www.wikidata.org/entity/Q106806190', 'http://www.wikidata.org/entity/Q106855753', 'http://www.wikidata.org/entity/Q1070437', 'http://www.wikidata.org/entity/Q107139413', 'http://www.wikidata.org/entity/Q10726425', 'http://www.wikidata.org/entity/Q107486932', 'http://www.wikidata.org/entity/Q107643630', 'http://www.wikidata.org/entity/Q108120675', 'http://www.wikidata.org/entity/Q108265918', 'http://www.wikidata.org/entity/Q108305674', 'http://www.wikidata.org/entity/Q108456662', 'http://www.wikidata.org/entity/Q108540687', 'http://www.wikidata.org/entity/Q10862448', 'http://www.wikidata.org/entity/Q108745010', 'http://www.wikidata.org/entity/Q10881633', 'http://www.wikidata.org/entity/Q108936865', 'http://www.wikidata.org/entity/Q10901070', 'http://www.wikidata.org/entity/Q109040869', 'http://www.wikidata.org/entity/Q10921475', 'http://www.wikidata.org/entity/Q109356066', 'http://www.wikidata.org/entity/Q109609391', 'http://www.wikidata.org/entity/Q109796906', 'http://www.wikidata.org/entity/Q110239836', 'http://www.wikidata.org/entity/Q1105149', 'http://www.wikidata.org/entity/Q110712627', 'http://www.wikidata.org/entity/Q110738072', 'http://www.wikidata.org/entity/Q110804043', 'http://www.wikidata.org/entity/Q11095193', 'http://www.wikidata.org/entity/Q11156396', 'http://www.wikidata.org/entity/Q11156590', 'http://www.wikidata.org/entity/Q11156602', 'http://www.wikidata.org/entity/Q111585601', 'http://www.wikidata.org/entity/Q111586257', 'http://www.wikidata.org/entity/Q111588212', 'http://www.wikidata.org/entity/Q111588631', 'http://www.wikidata.org/entity/Q111591927', 'http://www.wikidata.org/entity/Q111592030', 'http://www.wikidata.org/entity/Q111592221', 'http://www.wikidata.org/entity/Q111592231', 'http://www.wikidata.org/entity/Q111592392', 'http://www.wikidata.org/entity/Q111593121', 'http://www.wikidata.org/entity/Q111599061', 'http://www.wikidata.org/entity/Q111605534', 'http://www.wikidata.org/entity/Q111605672', 'http://www.wikidata.org/entity/Q111605780', 'http://www.wikidata.org/entity/Q111619857', 'http://www.wikidata.org/entity/Q111621136', 'http://www.wikidata.org/entity/Q111639188', 'http://www.wikidata.org/entity/Q111639464', 'http://www.wikidata.org/entity/Q111639796', 'http://www.wikidata.org/entity/Q111640394', 'http://www.wikidata.org/entity/Q111644691', 'http://www.wikidata.org/entity/Q111644855', 'http://www.wikidata.org/entity/Q111646483', 'http://www.wikidata.org/entity/Q111646603', 'http://www.wikidata.org/entity/Q111646902', 'http://www.wikidata.org/entity/Q111646942', 'http://www.wikidata.org/entity/Q111647178', 'http://www.wikidata.org/entity/Q111647244', 'http://www.wikidata.org/entity/Q111648147', 'http://www.wikidata.org/entity/Q111648327', 'http://www.wikidata.org/entity/Q111648357', 'http://www.wikidata.org/entity/Q111649590', 'http://www.wikidata.org/entity/Q111649647', 'http://www.wikidata.org/entity/Q111649691', 'http://www.wikidata.org/entity/Q111649919', 'http://www.wikidata.org/entity/Q111653594', 'http://www.wikidata.org/entity/Q111653613', 'http://www.wikidata.org/entity/Q111653631', 'http://www.wikidata.org/entity/Q111653637', 'http://www.wikidata.org/entity/Q111653675', 'http://www.wikidata.org/entity/Q111653779', 'http://www.wikidata.org/entity/Q111653938', 'http://www.wikidata.org/entity/Q111653958', 'http://www.wikidata.org/entity/Q111653969', 'http://www.wikidata.org/entity/Q111654007', 'http://www.wikidata.org/entity/Q111654040', 'http://www.wikidata.org/entity/Q111654093', 'http://www.wikidata.org/entity/Q111654098', 'http://www.wikidata.org/entity/Q111654121', 'http://www.wikidata.org/entity/Q111654136', 'http://www.wikidata.org/entity/Q111654241', 'http://www.wikidata.org/entity/Q111654346', 'http://www.wikidata.org/entity/Q111654469', 'http://www.wikidata.org/entity/Q111654484', 'http://www.wikidata.org/entity/Q111658731', 'http://www.wikidata.org/entity/Q111658801', 'http://www.wikidata.org/entity/Q111658833', 'http://www.wikidata.org/entity/Q111658927', 'http://www.wikidata.org/entity/Q111661297', 'http://www.wikidata.org/entity/Q111661840', 'http://www.wikidata.org/entity/Q111661872', 'http://www.wikidata.org/entity/Q111661886', 'http://www.wikidata.org/entity/Q111662034', 'http://www.wikidata.org/entity/Q111662035', 'http://www.wikidata.org/entity/Q111662040', 'http://www.wikidata.org/entity/Q111662133', 'http://www.wikidata.org/entity/Q111663221', 'http://www.wikidata.org/entity/Q111665328', 'http://www.wikidata.org/entity/Q111665519', 'http://www.wikidata.org/entity/Q111666301', 'http://www.wikidata.org/entity/Q111670117', 'http://www.wikidata.org/entity/Q111670231', 'http://www.wikidata.org/entity/Q111670397', 'http://www.wikidata.org/entity/Q111670481', 'http://www.wikidata.org/entity/Q111670617', 'http://www.wikidata.org/entity/Q111670624', 'http://www.wikidata.org/entity/Q111670628', 'http://www.wikidata.org/entity/Q111671698', 'http://www.wikidata.org/entity/Q111671968', 'http://www.wikidata.org/entity/Q111672442', 'http://www.wikidata.org/entity/Q111675204', 'http://www.wikidata.org/entity/Q111675217', 'http://www.wikidata.org/entity/Q111675293', 'http://www.wikidata.org/entity/Q111675405', 'http://www.wikidata.org/entity/Q111675518', 'http://www.wikidata.org/entity/Q111675816', 'http://www.wikidata.org/entity/Q111676530', 'http://www.wikidata.org/entity/Q111676789', 'http://www.wikidata.org/entity/Q111676828', 'http://www.wikidata.org/entity/Q111676959', 'http://www.wikidata.org/entity/Q111679720', 'http://www.wikidata.org/entity/Q111679753', 'http://www.wikidata.org/entity/Q111679830', 'http://www.wikidata.org/entity/Q111679840', 'http://www.wikidata.org/entity/Q111679871', 'http://www.wikidata.org/entity/Q111679978', 'http://www.wikidata.org/entity/Q111680097', 'http://www.wikidata.org/entity/Q111680142', 'http://www.wikidata.org/entity/Q111680149', 'http://www.wikidata.org/entity/Q111680197', 'http://www.wikidata.org/entity/Q111680221', 'http://www.wikidata.org/entity/Q111680229', 'http://www.wikidata.org/entity/Q111693657', 'http://www.wikidata.org/entity/Q111693675', 'http://www.wikidata.org/entity/Q111693696', 'http://www.wikidata.org/entity/Q111693773', 'http://www.wikidata.org/entity/Q111693781', 'http://www.wikidata.org/entity/Q111693947', 'http://www.wikidata.org/entity/Q111694017', 'http://www.wikidata.org/entity/Q111695525', 'http://www.wikidata.org/entity/Q111702011', 'http://www.wikidata.org/entity/Q111702051', 'http://www.wikidata.org/entity/Q111702063', 'http://www.wikidata.org/entity/Q111705727', 'http://www.wikidata.org/entity/Q111708136', 'http://www.wikidata.org/entity/Q111711151', 'http://www.wikidata.org/entity/Q111711160', 'http://www.wikidata.org/entity/Q111711162', 'http://www.wikidata.org/entity/Q111711184', 'http://www.wikidata.org/entity/Q111711264', 'http://www.wikidata.org/entity/Q111711268', 'http://www.wikidata.org/entity/Q111711270', 'http://www.wikidata.org/entity/Q111711273', 'http://www.wikidata.org/entity/Q111711278', 'http://www.wikidata.org/entity/Q111711311', 'http://www.wikidata.org/entity/Q111711342', 'http://www.wikidata.org/entity/Q111711421', 'http://www.wikidata.org/entity/Q111711540', 'http://www.wikidata.org/entity/Q111711547', 'http://www.wikidata.org/entity/Q111711661', 'http://www.wikidata.org/entity/Q111711757', 'http://www.wikidata.org/entity/Q111711903', 'http://www.wikidata.org/entity/Q111711907', 'http://www.wikidata.org/entity/Q111712005', 'http://www.wikidata.org/entity/Q111712010', 'http://www.wikidata.org/entity/Q111712059', 'http://www.wikidata.org/entity/Q111712123', 'http://www.wikidata.org/entity/Q111716408', 'http://www.wikidata.org/entity/Q111719293', 'http://www.wikidata.org/entity/Q111725575', 'http://www.wikidata.org/entity/Q111725911', 'http://www.wikidata.org/entity/Q111726390', 'http://www.wikidata.org/entity/Q111726615', 'http://www.wikidata.org/entity/Q111726617', 'http://www.wikidata.org/entity/Q111726635', 'http://www.wikidata.org/entity/Q111726669', 'http://www.wikidata.org/entity/Q111726714', 'http://www.wikidata.org/entity/Q111726768', 'http://www.wikidata.org/entity/Q111726774', 'http://www.wikidata.org/entity/Q111726793', 'http://www.wikidata.org/entity/Q111726805', 'http://www.wikidata.org/entity/Q111734330', 'http://www.wikidata.org/entity/Q111734453', 'http://www.wikidata.org/entity/Q111734646', 'http://www.wikidata.org/entity/Q111734661', 'http://www.wikidata.org/entity/Q111734681', 'http://www.wikidata.org/entity/Q111734708', 'http://www.wikidata.org/entity/Q111734879', 'http://www.wikidata.org/entity/Q111734906', 'http://www.wikidata.org/entity/Q111734910', 'http://www.wikidata.org/entity/Q111734978', 'http://www.wikidata.org/entity/Q111735009', 'http://www.wikidata.org/entity/Q111735146', 'http://www.wikidata.org/entity/Q111735183', 'http://www.wikidata.org/entity/Q111735311', 'http://www.wikidata.org/entity/Q111738073', 'http://www.wikidata.org/entity/Q111738552', 'http://www.wikidata.org/entity/Q111738762', 'http://www.wikidata.org/entity/Q111738881', 'http://www.wikidata.org/entity/Q111743473', 'http://www.wikidata.org/entity/Q111743614', 'http://www.wikidata.org/entity/Q111743635', 'http://www.wikidata.org/entity/Q111743658', 'http://www.wikidata.org/entity/Q111743894', 'http://www.wikidata.org/entity/Q111743903', 'http://www.wikidata.org/entity/Q111743905', 'http://www.wikidata.org/entity/Q111743922', 'http://www.wikidata.org/entity/Q111744105', 'http://www.wikidata.org/entity/Q111744185', 'http://www.wikidata.org/entity/Q111744196', 'http://www.wikidata.org/entity/Q111744206', 'http://www.wikidata.org/entity/Q111744231', 'http://www.wikidata.org/entity/Q111744233', 'http://www.wikidata.org/entity/Q111744287', 'http://www.wikidata.org/entity/Q111750057', 'http://www.wikidata.org/entity/Q111750098', 'http://www.wikidata.org/entity/Q111750104', 'http://www.wikidata.org/entity/Q111750108', 'http://www.wikidata.org/entity/Q111750391', 'http://www.wikidata.org/entity/Q111750396', 'http://www.wikidata.org/entity/Q111750414', 'http://www.wikidata.org/entity/Q111750482', 'http://www.wikidata.org/entity/Q111750486', 'http://www.wikidata.org/entity/Q111750538', 'http://www.wikidata.org/entity/Q111750619', 'http://www.wikidata.org/entity/Q111750632', 'http://www.wikidata.org/entity/Q111750636', 'http://www.wikidata.org/entity/Q111750803', 'http://www.wikidata.org/entity/Q111772339', 'http://www.wikidata.org/entity/Q111772429', 'http://www.wikidata.org/entity/Q111772455', 'http://www.wikidata.org/entity/Q111772465', 'http://www.wikidata.org/entity/Q111772467', 'http://www.wikidata.org/entity/Q111772470', 'http://www.wikidata.org/entity/Q111772479', 'http://www.wikidata.org/entity/Q111772481', 'http://www.wikidata.org/entity/Q111772492', 'http://www.wikidata.org/entity/Q111772538', 'http://www.wikidata.org/entity/Q111772542', 'http://www.wikidata.org/entity/Q111772579', 'http://www.wikidata.org/entity/Q111772903', 'http://www.wikidata.org/entity/Q111774488', 'http://www.wikidata.org/entity/Q111774855', 'http://www.wikidata.org/entity/Q111775976', 'http://www.wikidata.org/entity/Q111781307', 'http://www.wikidata.org/entity/Q111781313', 'http://www.wikidata.org/entity/Q111781415', 'http://www.wikidata.org/entity/Q111782305', 'http://www.wikidata.org/entity/Q111782406', 'http://www.wikidata.org/entity/Q111792237', 'http://www.wikidata.org/entity/Q111792287', 'http://www.wikidata.org/entity/Q111792297', 'http://www.wikidata.org/entity/Q111792422', 'http://www.wikidata.org/entity/Q111792427', 'http://www.wikidata.org/entity/Q111792455', 'http://www.wikidata.org/entity/Q111792652', 'http://www.wikidata.org/entity/Q111792657', 'http://www.wikidata.org/entity/Q111792669', 'http://www.wikidata.org/entity/Q111795166', 'http://www.wikidata.org/entity/Q111795170', 'http://www.wikidata.org/entity/Q111795181', 'http://www.wikidata.org/entity/Q111795190', 'http://www.wikidata.org/entity/Q111795208', 'http://www.wikidata.org/entity/Q111795217', 'http://www.wikidata.org/entity/Q111795226', 'http://www.wikidata.org/entity/Q111795230', 'http://www.wikidata.org/entity/Q111795234', 'http://www.wikidata.org/entity/Q111795238', 'http://www.wikidata.org/entity/Q111798789', 'http://www.wikidata.org/entity/Q111799191', 'http://www.wikidata.org/entity/Q111799265', 'http://www.wikidata.org/entity/Q111799326', 'http://www.wikidata.org/entity/Q111799364', 'http://www.wikidata.org/entity/Q111799715', 'http://www.wikidata.org/entity/Q111800151', 'http://www.wikidata.org/entity/Q111800560', 'http://www.wikidata.org/entity/Q111800590', 'http://www.wikidata.org/entity/Q111800661', 'http://www.wikidata.org/entity/Q111800678', 'http://www.wikidata.org/entity/Q111800735', 'http://www.wikidata.org/entity/Q111800758', 'http://www.wikidata.org/entity/Q111801201', 'http://www.wikidata.org/entity/Q111801219', 'http://www.wikidata.org/entity/Q111801257', 'http://www.wikidata.org/entity/Q111801366', 'http://www.wikidata.org/entity/Q111801395', 'http://www.wikidata.org/entity/Q111801411', 'http://www.wikidata.org/entity/Q111801450', 'http://www.wikidata.org/entity/Q111801507', 'http://www.wikidata.org/entity/Q111801550', 'http://www.wikidata.org/entity/Q111810594', 'http://www.wikidata.org/entity/Q111810721', 'http://www.wikidata.org/entity/Q111811564', 'http://www.wikidata.org/entity/Q111811624', 'http://www.wikidata.org/entity/Q111811681', 'http://www.wikidata.org/entity/Q111812563', 'http://www.wikidata.org/entity/Q111812584', 'http://www.wikidata.org/entity/Q111812855', 'http://www.wikidata.org/entity/Q111816790', 'http://www.wikidata.org/entity/Q111817714', 'http://www.wikidata.org/entity/Q111817744', 'http://www.wikidata.org/entity/Q111817829', 'http://www.wikidata.org/entity/Q111817846', 'http://www.wikidata.org/entity/Q111817920', 'http://www.wikidata.org/entity/Q111818123', 'http://www.wikidata.org/entity/Q111824276', 'http://www.wikidata.org/entity/Q111824296', 'http://www.wikidata.org/entity/Q111824414', 'http://www.wikidata.org/entity/Q111824439', 'http://www.wikidata.org/entity/Q111824771', 'http://www.wikidata.org/entity/Q111824800', 'http://www.wikidata.org/entity/Q111824823', 'http://www.wikidata.org/entity/Q111824918', 'http://www.wikidata.org/entity/Q111825400', 'http://www.wikidata.org/entity/Q111825424', 'http://www.wikidata.org/entity/Q111825449', 'http://www.wikidata.org/entity/Q111825554', 'http://www.wikidata.org/entity/Q111825613', 'http://www.wikidata.org/entity/Q111825677', 'http://www.wikidata.org/entity/Q111825713', 'http://www.wikidata.org/entity/Q111825832', 'http://www.wikidata.org/entity/Q111826063', 'http://www.wikidata.org/entity/Q111826089', 'http://www.wikidata.org/entity/Q111830034', 'http://www.wikidata.org/entity/Q111830188', 'http://www.wikidata.org/entity/Q111837290', 'http://www.wikidata.org/entity/Q111837438', 'http://www.wikidata.org/entity/Q111837464', 'http://www.wikidata.org/entity/Q111837474', 'http://www.wikidata.org/entity/Q111837785', 'http://www.wikidata.org/entity/Q111837834', 'http://www.wikidata.org/entity/Q111837845', 'http://www.wikidata.org/entity/Q111837855', 'http://www.wikidata.org/entity/Q111837912', 'http://www.wikidata.org/entity/Q111837991', 'http://www.wikidata.org/entity/Q111848069', 'http://www.wikidata.org/entity/Q111848409', 'http://www.wikidata.org/entity/Q111848456', 'http://www.wikidata.org/entity/Q111848558', 'http://www.wikidata.org/entity/Q111848588', 'http://www.wikidata.org/entity/Q111848721', 'http://www.wikidata.org/entity/Q111848749', 'http://www.wikidata.org/entity/Q111848889', 'http://www.wikidata.org/entity/Q111903596', 'http://www.wikidata.org/entity/Q111903847', 'http://www.wikidata.org/entity/Q111903850', 'http://www.wikidata.org/entity/Q111903876', 'http://www.wikidata.org/entity/Q111903878', 'http://www.wikidata.org/entity/Q111903929', 'http://www.wikidata.org/entity/Q111903935', 'http://www.wikidata.org/entity/Q111903958', 'http://www.wikidata.org/entity/Q111904025', 'http://www.wikidata.org/entity/Q111904053', 'http://www.wikidata.org/entity/Q111904059', 'http://www.wikidata.org/entity/Q111904155', 'http://www.wikidata.org/entity/Q111905212', 'http://www.wikidata.org/entity/Q111905225', 'http://www.wikidata.org/entity/Q111905272', 'http://www.wikidata.org/entity/Q111906585', 'http://www.wikidata.org/entity/Q111906632', 'http://www.wikidata.org/entity/Q111906707', 'http://www.wikidata.org/entity/Q111907290', 'http://www.wikidata.org/entity/Q111907317', 'http://www.wikidata.org/entity/Q111908878', 'http://www.wikidata.org/entity/Q111908880', 'http://www.wikidata.org/entity/Q111908884', 'http://www.wikidata.org/entity/Q111908910', 'http://www.wikidata.org/entity/Q111909231', 'http://www.wikidata.org/entity/Q111909314', 'http://www.wikidata.org/entity/Q111909357', 'http://www.wikidata.org/entity/Q111909361', 'http://www.wikidata.org/entity/Q111909369', 'http://www.wikidata.org/entity/Q111909483', 'http://www.wikidata.org/entity/Q111909520', 'http://www.wikidata.org/entity/Q111909557', 'http://www.wikidata.org/entity/Q111909632', 'http://www.wikidata.org/entity/Q111909656', 'http://www.wikidata.org/entity/Q111909659', 'http://www.wikidata.org/entity/Q111909665', 'http://www.wikidata.org/entity/Q111909679', 'http://www.wikidata.org/entity/Q111909683', 'http://www.wikidata.org/entity/Q111909686', 'http://www.wikidata.org/entity/Q111918622', 'http://www.wikidata.org/entity/Q111972328', 'http://www.wikidata.org/entity/Q111972588', 'http://www.wikidata.org/entity/Q111972596', 'http://www.wikidata.org/entity/Q111972626', 'http://www.wikidata.org/entity/Q111972641', 'http://www.wikidata.org/entity/Q111972655', 'http://www.wikidata.org/entity/Q111972667', 'http://www.wikidata.org/entity/Q111972760', 'http://www.wikidata.org/entity/Q111972775', 'http://www.wikidata.org/entity/Q111981575', 'http://www.wikidata.org/entity/Q111981578', 'http://www.wikidata.org/entity/Q111981586', 'http://www.wikidata.org/entity/Q111981600', 'http://www.wikidata.org/entity/Q111981655', 'http://www.wikidata.org/entity/Q111981806', 'http://www.wikidata.org/entity/Q111984435', 'http://www.wikidata.org/entity/Q111993442', 'http://www.wikidata.org/entity/Q111993561', 'http://www.wikidata.org/entity/Q112028016', 'http://www.wikidata.org/entity/Q112028058', 'http://www.wikidata.org/entity/Q112030707', 'http://www.wikidata.org/entity/Q112037464', 'http://www.wikidata.org/entity/Q112038287', 'http://www.wikidata.org/entity/Q112040430', 'http://www.wikidata.org/entity/Q112053302', 'http://www.wikidata.org/entity/Q112059989', 'http://www.wikidata.org/entity/Q112063713', 'http://www.wikidata.org/entity/Q112087493', 'http://www.wikidata.org/entity/Q112127176', 'http://www.wikidata.org/entity/Q112183753', 'http://www.wikidata.org/entity/Q112190885', 'http://www.wikidata.org/entity/Q112263083', 'http://www.wikidata.org/entity/Q112667083', 'http://www.wikidata.org/entity/Q112667550', 'http://www.wikidata.org/entity/Q112669313', 'http://www.wikidata.org/entity/Q112669383', 'http://www.wikidata.org/entity/Q112681996', 'http://www.wikidata.org/entity/Q112746421', 'http://www.wikidata.org/entity/Q112747808', 'http://www.wikidata.org/entity/Q112894949', 'http://www.wikidata.org/entity/Q112894986', 'http://www.wikidata.org/entity/Q113015050', 'http://www.wikidata.org/entity/Q113072738', 'http://www.wikidata.org/entity/Q1131707', 'http://www.wikidata.org/entity/Q113272299', 'http://www.wikidata.org/entity/Q113272409', 'http://www.wikidata.org/entity/Q113272932', 'http://www.wikidata.org/entity/Q113499373', 'http://www.wikidata.org/entity/Q113499494', 'http://www.wikidata.org/entity/Q113650760', 'http://www.wikidata.org/entity/Q11368765', 'http://www.wikidata.org/entity/Q113811579', 'http://www.wikidata.org/entity/Q113813231', 'http://www.wikidata.org/entity/Q113828978', 'http://www.wikidata.org/entity/Q113830063', 'http://www.wikidata.org/entity/Q113841626', 'http://www.wikidata.org/entity/Q113849016', 'http://www.wikidata.org/entity/Q113860611', 'http://www.wikidata.org/entity/Q113860644', 'http://www.wikidata.org/entity/Q113861194', 'http://www.wikidata.org/entity/Q113882354', 'http://www.wikidata.org/entity/Q113884368', 'http://www.wikidata.org/entity/Q113901976', 'http://www.wikidata.org/entity/Q113904662', 'http://www.wikidata.org/entity/Q1139536', 'http://www.wikidata.org/entity/Q113955599', 'http://www.wikidata.org/entity/Q113955616', 'http://www.wikidata.org/entity/Q113955620', 'http://www.wikidata.org/entity/Q113955692', 'http://www.wikidata.org/entity/Q113961851', 'http://www.wikidata.org/entity/Q113961888', 'http://www.wikidata.org/entity/Q113961932', 'http://www.wikidata.org/entity/Q114028189', 'http://www.wikidata.org/entity/Q114046091', 'http://www.wikidata.org/entity/Q114056617', 'http://www.wikidata.org/entity/Q114057278', 'http://www.wikidata.org/entity/Q114059225', 'http://www.wikidata.org/entity/Q114243677', 'http://www.wikidata.org/entity/Q114454471', 'http://www.wikidata.org/entity/Q1145566', 'http://www.wikidata.org/entity/Q1145630', 'http://www.wikidata.org/entity/Q114582556', 'http://www.wikidata.org/entity/Q114588676', 'http://www.wikidata.org/entity/Q114604', 'http://www.wikidata.org/entity/Q114947458', 'http://www.wikidata.org/entity/Q114948159', 'http://www.wikidata.org/entity/Q114996688', 'http://www.wikidata.org/entity/Q114997174', 'http://www.wikidata.org/entity/Q115341348', 'http://www.wikidata.org/entity/Q115367992', 'http://www.wikidata.org/entity/Q115397386', 'http://www.wikidata.org/entity/Q115517924', 'http://www.wikidata.org/entity/Q115764515', 'http://www.wikidata.org/entity/Q115801523', 'http://www.wikidata.org/entity/Q115912774', 'http://www.wikidata.org/entity/Q115990472', 'http://www.wikidata.org/entity/Q116414186', 'http://www.wikidata.org/entity/Q116690653', 'http://www.wikidata.org/entity/Q117421915', 'http://www.wikidata.org/entity/Q117695225', 'http://www.wikidata.org/entity/Q117751349', 'http://www.wikidata.org/entity/Q117795094', 'http://www.wikidata.org/entity/Q11789705', 'http://www.wikidata.org/entity/Q118128483', 'http://www.wikidata.org/entity/Q11921906', 'http://www.wikidata.org/entity/Q11938851', 'http://www.wikidata.org/entity/Q119496586', 'http://www.wikidata.org/entity/Q11993043', 'http://www.wikidata.org/entity/Q1207931', 'http://www.wikidata.org/entity/Q1207932', 'http://www.wikidata.org/entity/Q120837533', 'http://www.wikidata.org/entity/Q121886956', 'http://www.wikidata.org/entity/Q122068698', 'http://www.wikidata.org/entity/Q122188018', 'http://www.wikidata.org/entity/Q12228863', 'http://www.wikidata.org/entity/Q12228866', 'http://www.wikidata.org/entity/Q12228868', 'http://www.wikidata.org/entity/Q12228876', 'http://www.wikidata.org/entity/Q12228884', 'http://www.wikidata.org/entity/Q12252186', 'http://www.wikidata.org/entity/Q12277858', 'http://www.wikidata.org/entity/Q122832546', 'http://www.wikidata.org/entity/Q12314502', 'http://www.wikidata.org/entity/Q123337193', 'http://www.wikidata.org/entity/Q123592992', 'http://www.wikidata.org/entity/Q12361577', 'http://www.wikidata.org/entity/Q123746478', 'http://www.wikidata.org/entity/Q12376028', 'http://www.wikidata.org/entity/Q12378350', 'http://www.wikidata.org/entity/Q124036138', 'http://www.wikidata.org/entity/Q12407929', 'http://www.wikidata.org/entity/Q12411505', 'http://www.wikidata.org/entity/Q124367042', 'http://www.wikidata.org/entity/Q124504910', 'http://www.wikidata.org/entity/Q124564384', 'http://www.wikidata.org/entity/Q124612831', 'http://www.wikidata.org/entity/Q124615758', 'http://www.wikidata.org/entity/Q124619352', 'http://www.wikidata.org/entity/Q124620804', 'http://www.wikidata.org/entity/Q124620822', 'http://www.wikidata.org/entity/Q124707699', 'http://www.wikidata.org/entity/Q124820083', 'http://www.wikidata.org/entity/Q124830280', 'http://www.wikidata.org/entity/Q124857570', 'http://www.wikidata.org/entity/Q124858688', 'http://www.wikidata.org/entity/Q124858953', 'http://www.wikidata.org/entity/Q125149734', 'http://www.wikidata.org/entity/Q125205121', 'http://www.wikidata.org/entity/Q1254268', 'http://www.wikidata.org/entity/Q125510673', 'http://www.wikidata.org/entity/Q125511630', 'http://www.wikidata.org/entity/Q125521675', 'http://www.wikidata.org/entity/Q125521758', 'http://www.wikidata.org/entity/Q125555445', 'http://www.wikidata.org/entity/Q125566609', 'http://www.wikidata.org/entity/Q125577561', 'http://www.wikidata.org/entity/Q125592462', 'http://www.wikidata.org/entity/Q12560060', 'http://www.wikidata.org/entity/Q125688458', 'http://www.wikidata.org/entity/Q125688603', 'http://www.wikidata.org/entity/Q125700972', 'http://www.wikidata.org/entity/Q125704427', 'http://www.wikidata.org/entity/Q125747483', 'http://www.wikidata.org/entity/Q125749644', 'http://www.wikidata.org/entity/Q125758800', 'http://www.wikidata.org/entity/Q125759229', 'http://www.wikidata.org/entity/Q125845551', 'http://www.wikidata.org/entity/Q12584835', 'http://www.wikidata.org/entity/Q125856465', 'http://www.wikidata.org/entity/Q125867175', 'http://www.wikidata.org/entity/Q125867458', 'http://www.wikidata.org/entity/Q125867756', 'http://www.wikidata.org/entity/Q125867888', 'http://www.wikidata.org/entity/Q125869488', 'http://www.wikidata.org/entity/Q125879646', 'http://www.wikidata.org/entity/Q125879891', 'http://www.wikidata.org/entity/Q125883649', 'http://www.wikidata.org/entity/Q125883847', 'http://www.wikidata.org/entity/Q125890530', 'http://www.wikidata.org/entity/Q125890753', 'http://www.wikidata.org/entity/Q125891443', 'http://www.wikidata.org/entity/Q125891720', 'http://www.wikidata.org/entity/Q125895110', 'http://www.wikidata.org/entity/Q125895155', 'http://www.wikidata.org/entity/Q125899181', 'http://www.wikidata.org/entity/Q125899513', 'http://www.wikidata.org/entity/Q125901134', 'http://www.wikidata.org/entity/Q125903138', 'http://www.wikidata.org/entity/Q125910729', 'http://www.wikidata.org/entity/Q125910806', 'http://www.wikidata.org/entity/Q125911055', 'http://www.wikidata.org/entity/Q125911072', 'http://www.wikidata.org/entity/Q125914666', 'http://www.wikidata.org/entity/Q125914885', 'http://www.wikidata.org/entity/Q125921693', 'http://www.wikidata.org/entity/Q125922831', 'http://www.wikidata.org/entity/Q125922882', 'http://www.wikidata.org/entity/Q125926636', 'http://www.wikidata.org/entity/Q125932740', 'http://www.wikidata.org/entity/Q125936101', 'http://www.wikidata.org/entity/Q125936683', 'http://www.wikidata.org/entity/Q125956876', 'http://www.wikidata.org/entity/Q125959131', 'http://www.wikidata.org/entity/Q125965703', 'http://www.wikidata.org/entity/Q125966437', 'http://www.wikidata.org/entity/Q125966992', 'http://www.wikidata.org/entity/Q125968806', 'http://www.wikidata.org/entity/Q125969610', 'http://www.wikidata.org/entity/Q125970539', 'http://www.wikidata.org/entity/Q125984409', 'http://www.wikidata.org/entity/Q125984492', 'http://www.wikidata.org/entity/Q125994583', 'http://www.wikidata.org/entity/Q125997034', 'http://www.wikidata.org/entity/Q125998688', 'http://www.wikidata.org/entity/Q125998803', 'http://www.wikidata.org/entity/Q125998897', 'http://www.wikidata.org/entity/Q125999072', 'http://www.wikidata.org/entity/Q12599950', 'http://www.wikidata.org/entity/Q126010095', 'http://www.wikidata.org/entity/Q126010128', 'http://www.wikidata.org/entity/Q126028447', 'http://www.wikidata.org/entity/Q126028546', 'http://www.wikidata.org/entity/Q126032653', 'http://www.wikidata.org/entity/Q126126323', 'http://www.wikidata.org/entity/Q126126778', 'http://www.wikidata.org/entity/Q12613371', 'http://www.wikidata.org/entity/Q12629515', 'http://www.wikidata.org/entity/Q126325524', 'http://www.wikidata.org/entity/Q126361854', 'http://www.wikidata.org/entity/Q126362969', 'http://www.wikidata.org/entity/Q126371412', 'http://www.wikidata.org/entity/Q126371457', 'http://www.wikidata.org/entity/Q126371864', 'http://www.wikidata.org/entity/Q126371886', 'http://www.wikidata.org/entity/Q126372368', 'http://www.wikidata.org/entity/Q126372458', 'http://www.wikidata.org/entity/Q126372576', 'http://www.wikidata.org/entity/Q126415038', 'http://www.wikidata.org/entity/Q126456102', 'http://www.wikidata.org/entity/Q126477003', 'http://www.wikidata.org/entity/Q126477086', 'http://www.wikidata.org/entity/Q126477151', 'http://www.wikidata.org/entity/Q126477162', 'http://www.wikidata.org/entity/Q126478091', 'http://www.wikidata.org/entity/Q126478228', 'http://www.wikidata.org/entity/Q126511431', 'http://www.wikidata.org/entity/Q126513767', 'http://www.wikidata.org/entity/Q126593634', 'http://www.wikidata.org/entity/Q12663413', 'http://www.wikidata.org/entity/Q126666887', 'http://www.wikidata.org/entity/Q126709387', 'http://www.wikidata.org/entity/Q126721902', 'http://www.wikidata.org/entity/Q126726117', 'http://www.wikidata.org/entity/Q126811008', 'http://www.wikidata.org/e</t>
+          <t>['http://www.wikidata.org/entity/Q102174232']</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q100329955', 'http://www.wikidata.org/entity/Q100597341', 'http://www.wikidata.org/entity/Q100860934', 'http://www.wikidata.org/entity/Q101026979', 'http://www.wikidata.org/entity/Q101545880', 'http://www.wikidata.org/entity/Q101627559', 'http://www.wikidata.org/entity/Q1016833', 'http://www.wikidata.org/entity/Q101706322', 'http://www.wikidata.org/entity/Q102276948', 'http://www.wikidata.org/entity/Q102398478', 'http://www.wikidata.org/entity/Q10244', 'http://www.wikidata.org/entity/Q10253', 'http://www.wikidata.org/entity/Q1025481', 'http://www.wikidata.org/entity/Q10259922', 'http://www.wikidata.org/entity/Q10265947', 'http://www.wikidata.org/entity/Q10281787', 'http://www.wikidata.org/entity/Q10329424', 'http://www.wikidata.org/entity/Q103821550', 'http://www.wikidata.org/entity/Q1038328', 'http://www.wikidata.org/entity/Q103956800', 'http://www.wikidata.org/entity/Q10398273', 'http://www.wikidata.org/entity/Q104051143', 'http://www.wikidata.org/entity/Q10412386', 'http://www.wikidata.org/entity/Q10416096', 'http://www.wikidata.org/entity/Q10418897', 'http://www.wikidata.org/entity/Q104224166', 'http://www.wikidata.org/entity/Q1043596', 'http://www.wikidata.org/entity/Q104601590', 'http://www.wikidata.org/entity/Q104625773', 'http://www.wikidata.org/entity/Q104758920', 'http://www.wikidata.org/entity/Q10481350', 'http://www.wikidata.org/entity/Q104920297', 'http://www.wikidata.org/entity/Q10494624', 'http://www.wikidata.org/entity/Q10495964', 'http://www.wikidata.org/entity/Q10496086', 'http://www.wikidata.org/entity/Q10501512', 'http://www.wikidata.org/entity/Q1050292', 'http://www.wikidata.org/entity/Q105043914', 'http://www.wikidata.org/entity/Q105121443', 'http://www.wikidata.org/entity/Q105360445', 'http://www.wikidata.org/entity/Q105393711', 'http://www.wikidata.org/entity/Q105394069', 'http://www.wikidata.org/entity/Q10541207', 'http://www.wikidata.org/entity/Q1054558', 'http://www.wikidata.org/entity/Q105663779', 'http://www.wikidata.org/entity/Q10586365', 'http://www.wikidata.org/entity/Q10601007', 'http://www.wikidata.org/entity/Q10601355', 'http://www.wikidata.org/entity/Q106019359', 'http://www.wikidata.org/entity/Q106043577', 'http://www.wikidata.org/entity/Q106078232', 'http://www.wikidata.org/entity/Q106200291', 'http://www.wikidata.org/entity/Q106240773', 'http://www.wikidata.org/entity/Q106290028', 'http://www.wikidata.org/entity/Q106307776', 'http://www.wikidata.org/entity/Q10631904', 'http://www.wikidata.org/entity/Q106331005', 'http://www.wikidata.org/entity/Q106349026', 'http://www.wikidata.org/entity/Q106369745', 'http://www.wikidata.org/entity/Q106436015', 'http://www.wikidata.org/entity/Q106505905', 'http://www.wikidata.org/entity/Q10666884', 'http://www.wikidata.org/entity/Q106675733', 'http://www.wikidata.org/entity/Q106689897', 'http://www.wikidata.org/entity/Q10669318', 'http://www.wikidata.org/entity/Q10669370', 'http://www.wikidata.org/entity/Q10669371', 'http://www.wikidata.org/entity/Q10685840', 'http://www.wikidata.org/entity/Q10689144', 'http://www.wikidata.org/entity/Q10689145', 'http://www.wikidata.org/entity/Q10689146', 'http://www.wikidata.org/entity/Q106899527', 'http://www.wikidata.org/entity/Q10698576', 'http://www.wikidata.org/entity/Q10698931', 'http://www.wikidata.org/entity/Q10698932', 'http://www.wikidata.org/entity/Q10698935', 'http://www.wikidata.org/entity/Q10698936', 'http://www.wikidata.org/entity/Q10698937', 'http://www.wikidata.org/entity/Q10699347', 'http://www.wikidata.org/entity/Q107015910', 'http://www.wikidata.org/entity/Q10701677', 'http://www.wikidata.org/entity/Q10701968', 'http://www.wikidata.org/entity/Q1070318', 'http://www.wikidata.org/entity/Q10714715', 'http://www.wikidata.org/entity/Q10726998', 'http://www.wikidata.org/entity/Q107309593', 'http://www.wikidata.org/entity/Q107718805', 'http://www.wikidata.org/entity/Q107739995', 'http://www.wikidata.org/entity/Q108010714', 'http://www.wikidata.org/entity/Q108101493', 'http://www.wikidata.org/entity/Q108131371', 'http://www.wikidata.org/entity/Q108219988', 'http://www.wikidata.org/entity/Q108315106', 'http://www.wikidata.org/entity/Q108392466', 'http://www.wikidata.org/entity/Q108424805', 'http://www.wikidata.org/entity/Q10854401', 'http://www.wikidata.org/entity/Q10855559', 'http://www.wikidata.org/entity/Q108660772', 'http://www.wikidata.org/entity/Q10868404', 'http://www.wikidata.org/entity/Q108730127', 'http://www.wikidata.org/entity/Q108749396', 'http://www.wikidata.org/entity/Q108749484', 'http://www.wikidata.org/entity/Q108814176', 'http://www.wikidata.org/entity/Q108936669', 'http://www.wikidata.org/entity/Q10909572', 'http://www.wikidata.org/entity/Q109121006', 'http://www.wikidata.org/entity/Q1091428', 'http://www.wikidata.org/entity/Q10921477', 'http://www.wikidata.org/entity/Q109285268', 'http://www.wikidata.org/entity/Q109329448', 'http://www.wikidata.org/entity/Q109329455', 'http://www.wikidata.org/entity/Q109356066', 'http://www.wikidata.org/entity/Q109381834', 'http://www.wikidata.org/entity/Q109381883', 'http://www.wikidata.org/entity/Q109440429', 'http://www.wikidata.org/entity/Q109455204', 'http://www.wikidata.org/entity/Q10955171', 'http://www.wikidata.org/entity/Q109558468', 'http://www.wikidata.org/entity/Q109609391', 'http://www.wikidata.org/entity/Q10964022', 'http://www.wikidata.org/entity/Q109827527', 'http://www.wikidata.org/entity/Q109838056', 'http://www.wikidata.org/entity/Q109908577', 'http://www.wikidata.org/entity/Q11002663', 'http://www.wikidata.org/entity/Q110091424', 'http://www.wikidata.org/entity/Q110128398', 'http://www.wikidata.org/entity/Q110206440', 'http://www.wikidata.org/entity/Q110239836', 'http://www.wikidata.org/entity/Q110639888', 'http://www.wikidata.org/entity/Q110962934', 'http://www.wikidata.org/entity/Q111149458', 'http://www.wikidata.org/entity/Q111202983', 'http://www.wikidata.org/entity/Q111333928', 'http://www.wikidata.org/entity/Q111574867', 'http://www.wikidata.org/entity/Q111605537', 'http://www.wikidata.org/entity/Q111649462', 'http://www.wikidata.org/entity/Q111649876', 'http://www.wikidata.org/entity/Q111655654', 'http://www.wikidata.org/entity/Q111711222', 'http://www.wikidata.org/entity/Q111732603', 'http://www.wikidata.org/entity/Q111811564', 'http://www.wikidata.org/entity/Q111846538', 'http://www.wikidata.org/entity/Q111914764', 'http://www.wikidata.org/entity/Q112055', 'http://www.wikidata.org/entity/Q112059989', 'http://www.wikidata.org/entity/Q112075710', 'http://www.wikidata.org/entity/Q11219195', 'http://www.wikidata.org/entity/Q112292803', 'http://www.wikidata.org/entity/Q11237670', 'http://www.wikidata.org/entity/Q11244589', 'http://www.wikidata.org/entity/Q112613424', 'http://www.wikidata.org/entity/Q11269', 'http://www.wikidata.org/entity/Q112748137', 'http://www.wikidata.org/entity/Q11277431', 'http://www.wikidata.org/entity/Q112971391', 'http://www.wikidata.org/entity/Q112971396', 'http://www.wikidata.org/entity/Q112971410', 'http://www.wikidata.org/entity/Q112971413', 'http://www.wikidata.org/entity/Q113040064', 'http://www.wikidata.org/entity/Q113114857', 'http://www.wikidata.org/entity/Q113232600', 'http://www.wikidata.org/entity/Q113383597', 'http://www.wikidata.org/entity/Q113470219', 'http://www.wikidata.org/entity/Q113470532', 'http://www.wikidata.org/entity/Q113485231', 'http://www.wikidata.org/entity/Q113499420', 'http://www.wikidata.org/entity/Q113499458', 'http://www.wikidata.org/entity/Q1135034', 'http://www.wikidata.org/entity/Q11354348', 'http://www.wikidata.org/entity/Q113549137', 'http://www.wikidata.org/entity/Q113576165', 'http://www.wikidata.org/entity/Q113581609', 'http://www.wikidata.org/entity/Q113627236', 'http://www.wikidata.org/entity/Q113631347', 'http://www.wikidata.org/entity/Q113631375', 'http://www.wikidata.org/entity/Q113631508', 'http://www.wikidata.org/entity/Q113631563', 'http://www.wikidata.org/entity/Q113631569', 'http://www.wikidata.org/entity/Q113674106', 'http://www.wikidata.org/entity/Q11371391', 'http://www.wikidata.org/entity/Q113714633', 'http://www.wikidata.org/entity/Q11387117', 'http://www.wikidata.org/entity/Q113903854', 'http://www.wikidata.org/entity/Q11391277', 'http://www.wikidata.org/entity/Q1139591', 'http://www.wikidata.org/entity/Q11409712', 'http://www.wikidata.org/entity/Q114315605', 'http://www.wikidata.org/entity/Q114658295', 'http://www.wikidata.org/entity/Q1147008', 'http://www.wikidata.org/entity/Q114779611', 'http://www.wikidata.org/entity/Q114780741', 'http://www.wikidata.org/entity/Q114781351', 'http://www.wikidata.org/entity/Q114840373', 'http://www.wikidata.org/entity/Q114863314', 'http://www.wikidata.org/entity/Q115152362', 'http://www.wikidata.org/entity/Q115209188', 'http://www.wikidata.org/entity/Q115214299', 'http://www.wikidata.org/entity/Q115259173', 'http://www.wikidata.org/entity/Q115294651', 'http://www.wikidata.org/entity/Q115327380', 'http://www.wikidata.org/entity/Q1153848', 'http://www.wikidata.org/entity/Q11545488', 'http://www.wikidata.org/entity/Q115516436', 'http://www.wikidata.org/entity/Q115526578', 'http://www.wikidata.org/entity/Q115624997', 'http://www.wikidata.org/entity/Q115628690', 'http://www.wikidata.org/entity/Q11567159', 'http://www.wikidata.org/entity/Q11590237', 'http://www.wikidata.org/entity/Q115937074', 'http://www.wikidata.org/entity/Q11606287', 'http://www.wikidata.org/entity/Q116113833', 'http://www.wikidata.org/entity/Q116349234', 'http://www.wikidata.org/entity/Q116767714', 'http://www.wikidata.org/entity/Q116790237', 'http://www.wikidata.org/entity/Q116846825', 'http://www.wikidata.org/entity/Q116858640', 'http://www.wikidata.org/entity/Q116938985', 'http://www.wikidata.org/entity/Q11695705', 'http://www.wikidata.org/entity/Q11695707', 'http://www.wikidata.org/entity/Q11695708', 'http://www.wikidata.org/entity/Q11695711', 'http://www.wikidata.org/entity/Q11695713', 'http://www.wikidata.org/entity/Q11695714', 'http://www.wikidata.org/entity/Q11695716', 'http://www.wikidata.org/entity/Q11695717', 'http://www.wikidata.org/entity/Q11695718', 'http://www.wikidata.org/entity/Q11695721', 'http://www.wikidata.org/entity/Q11695722', 'http://www.wikidata.org/entity/Q11695723', 'http://www.wikidata.org/entity/Q116973585', 'http://www.wikidata.org/entity/Q116980492', 'http://www.wikidata.org/entity/Q117035968', 'http://www.wikidata.org/entity/Q11703716', 'http://www.wikidata.org/entity/Q117040282', 'http://www.wikidata.org/entity/Q11706236', 'http://www.wikidata.org/entity/Q1170632', 'http://www.wikidata.org/entity/Q117361394', 'http://www.wikidata.org/entity/Q117421915', 'http://www.wikidata.org/entity/Q117455751', 'http://www.wikidata.org/entity/Q117587270', 'http://www.wikidata.org/entity/Q117711867', 'http://www.wikidata.org/entity/Q11783773', 'http://www.wikidata.org/entity/Q11783808', 'http://www.wikidata.org/entity/Q117844480', 'http://www.wikidata.org/entity/Q11789695', 'http://www.wikidata.org/entity/Q11789705', 'http://www.wikidata.org/entity/Q11789707', 'http://www.wikidata.org/entity/Q11802972', 'http://www.wikidata.org/entity/Q118224784', 'http://www.wikidata.org/entity/Q118288532', 'http://www.wikidata.org/entity/Q118314773', 'http://www.wikidata.org/entity/Q118330188', 'http://www.wikidata.org/entity/Q118369207', 'http://www.wikidata.org/entity/Q118744251', 'http://www.wikidata.org/entity/Q118842681', 'http://www.wikidata.org/entity/Q118849459', 'http://www.wikidata.org/entity/Q118947258', 'http://www.wikidata.org/entity/Q119105010', 'http://www.wikidata.org/entity/Q11919090', 'http://www.wikidata.org/entity/Q119241124', 'http://www.wikidata.org/entity/Q119243817', 'http://www.wikidata.org/entity/Q119285617', 'http://www.wikidata.org/entity/Q119348301', 'http://www.wikidata.org/entity/Q119397277', 'http://www.wikidata.org/entity/Q1194059', 'http://www.wikidata.org/entity/Q11977920', 'http://www.wikidata.org/entity/Q119806244', 'http://www.wikidata.org/entity/Q119853995', 'http://www.wikidata.org/entity/Q120068971', 'http://www.wikidata.org/entity/Q120146391', 'http://www.wikidata.org/entity/Q120403912', 'http://www.wikidata.org/entity/Q120486552', 'http://www.wikidata.org/entity/Q12060958', 'http://www.wikidata.org/entity/Q120823815', 'http://www.wikidata.org/entity/Q120837533', 'http://www.wikidata.org/entity/Q12090941', 'http://www.wikidata.org/entity/Q1209940', 'http://www.wikidata.org/entity/Q12100125', 'http://www.wikidata.org/entity/Q12100126', 'http://www.wikidata.org/entity/Q12100128', 'http://www.wikidata.org/entity/Q12100132', 'http://www.wikidata.org/entity/Q12100138', 'http://www.wikidata.org/entity/Q12100141', 'http://www.wikidata.org/entity/Q12100152', 'http://www.wikidata.org/entity/Q12100160', 'http://www.wikidata.org/entity/Q12131090', 'http://www.wikidata.org/entity/Q121322780', 'http://www.wikidata.org/entity/Q121393', 'http://www.wikidata.org/entity/Q12149731', 'http://www.wikidata.org/entity/Q12174361', 'http://www.wikidata.org/entity/Q121759535', 'http://www.wikidata.org/entity/Q121852183', 'http://www.wikidata.org/entity/Q121864546', 'http://www.wikidata.org/entity/Q121991381', 'http://www.wikidata.org/entity/Q122057715', 'http://www.wikidata.org/entity/Q122058042', 'http://www.wikidata.org/entity/Q122144115', 'http://www.wikidata.org/entity/Q122199376', 'http://www.wikidata.org/entity/Q122341064', 'http://www.wikidata.org/entity/Q122460010', 'http://www.wikidata.org/entity/Q122495885', 'http://www.wikidata.org/entity/Q1226845', 'http://www.wikidata.org/entity/Q122767100', 'http://www.wikidata.org/entity/Q12284238', 'http://www.wikidata.org/entity/Q12286265', 'http://www.wikidata.org/entity/Q12286390', 'http://www.wikidata.org/entity/Q12289674', 'http://www.wikidata.org/entity/Q12292151', 'http://www.wikidata.org/entity/Q12293119', 'http://www.wikidata.org/entity/Q12293243', 'http://www.wikidata.org/entity/Q12299913', 'http://www.wikidata.org/entity/Q123111964', 'http://www.wikidata.org/entity/Q1231872', 'http://www.wikidata.org/entity/Q123253535', 'http://www.wikidata.org/entity/Q123265528', 'http://www.wikidata.org/entity/Q123450314', 'http://www.wikidata.org/entity/Q123515600', 'http://www.wikidata.org/entity/Q12353618', 'http://www.wikidata.org/entity/Q123746478', 'http://www.wikidata.org/entity/Q123757853', 'http://www.wikidata.org/entity/Q1239437', 'http://www.wikidata.org/entity/Q12407917', 'http://www.wikidata.org/entity/Q12407923', 'http://www.wikidata.org/entity/Q1241858', 'http://www.wikidata.org/entity/Q12422844', 'http://www.wikidata.org/entity/Q124250314', 'http://www.wikidata.org/entity/Q124250951', 'http://www.wikidata.org/entity/Q124255532', 'http://www.wikidata.org/entity/Q124318023', 'http://www.wikidata.org/entity/Q124352953', 'http://www.wikidata.org/entity/Q124367000', 'http://www.wikidata.org/entity/Q12438967', 'http://www.wikidata.org/entity/Q124408550', 'http://www.wikidata.org/entity/Q12441237', 'http://www.wikidata.org/entity/Q124498473', 'http://www.wikidata.org/entity/Q124498859', 'http://www.wikidata.org/entity/Q124568688', 'http://www.wikidata.org/entity/Q124747000', 'http://www.wikidata.org/entity/Q124799998', 'http://www.wikidata.org/entity/Q124830290', 'http://www.wikidata.org/entity/Q124854084', 'http://www.wikidata.org/entity/Q12513670', 'http://www.wikidata.org/entity/Q12525597', 'http://www.wikidata.org/entity/Q1252585', 'http://www.wikidata.org/entity/Q1252596', 'http://www.wikidata.org/entity/Q125505711', 'http://www.wikidata.org/entity/Q1255099', 'http://www.wikidata.org/entity/Q125524227', 'http://www.wikidata.org/entity/Q125613295', 'http://www.wikidata.org/entity/Q125912847', 'http://www.wikidata.org/entity/Q125928736', 'http://www.wikidata.org/entity/Q12601109', 'http://www.wikidata.org/entity/Q12602481', 'http://www.wikidata.org/entity/Q126083299', 'http://www.wikidata.org/entity/Q126083373', 'http://www.wikidata.org/entity/Q126113071', 'http://www.wikidata.org/entity/Q12614307', 'http://www.wikidata.org/entity/Q12614875', 'http://www.wikidata.org/entity/Q126192995', 'http://www.wikidata.org/entity/Q126260200', 'http://www.wikidata.org/entity/Q12650252', 'http://www.wikidata.org/entity/Q12663498', 'http://www.wikidata.org/entity/Q126708915', 'http://www.wikidata.org/entity/Q126902823', 'http://www.wikidata.org/entity/Q126903060', 'http://www.wikidata.org/entity/Q126910647', 'http://www.wikidata.org/entity/Q126948133', 'http://www.wikidata.org/entity/Q126949840', 'http://www.wikidata.org/entity/Q1270782', 'http://www.wikidata.org/entity/Q12713841', 'http://www.wikidata.org/entity/Q12716026', 'http://www.wikidata.org/entity/Q12719109', 'http://www.wikidata.org/entity/Q127393146', 'http://www.wikidata.org/entity/Q127502506', 'http://www.wikidata.org/entity/Q12750635', 'http://www.wikidata.org/entity/Q127597840', 'http://www.wikidata.org/entity/Q127798249', 'http://www.wikidata.org/entity/Q12787253', 'http://www.wikidata.org/entity/Q12787255', 'http://www.wikidata.org/entity/Q127922454', 'http://www.wikidata.org/entity/Q12803843', 'http://www.wikidata.org/entity/Q12836659', 'http://www.wikidata.org/entity/Q12859165', 'http://www.wikidata.org/entity/Q12864158', 'http://www.wikidata.org/entity/Q1290276', 'http://www.wikidata.org/entity/Q12927731', 'http://www.wikidata.org/entity/Q129726', 'http://www.wikidata.org/entity/Q12986877', 'http://www.wikidata.org/entity/Q129876847', 'http://www.wikidata.org/entity/Q129876849', 'http://www.wikidata.org/entity/Q129876851', 'http://www.wikidata.org/entity/Q129876853', 'http://www.wikidata.org/entity/Q129876855', 'http://www.wikidata.org/entity/Q129876857', 'http://www.wikidata.org/entity/Q12989464', 'http://www.wikidata.org/entity/Q13020973', 'http://www.wikidata.org/entity/Q130215597', 'http://www.wikidata.org/entity/Q130237269', 'http://www.wikidata.org/entity/Q130237270', 'http://www.wikidata.org/entity/Q130237271', 'http://www.wikidata.org/entity/Q130237272', 'http://www.wikidata.org/entity/Q130237273', 'http://www.wikidata.org/entity/Q130237274', 'http://www.wikidata.org/entity/Q130237276', 'http://www.wikidata.org/entity/Q130237277', 'http://www.wikidata.org/entity/Q130237278', 'http://www.wikidata.org/entity/Q130237279', 'http://www.wikidata.org/entity/Q130237280', 'http://www.wikidata.org/entity/Q130237281', 'http://www.wikidata.org/entity/Q130237282', 'http://www.wikidata.org/entity/Q130237283', 'http://www.wikidata.org/entity/Q130237284', 'http://www.wikidata.org/entity/Q130237285', 'http://www.wikidata.org/entity/Q130237286', 'http://www.wikidata.org/entity/Q130237287', 'http://www.wikidata.org/entity/Q130237288', 'http://www.wikidata.org/entity/Q130237289', 'http://www.wikidata.org/entity/Q130237290', 'http://www.wikidata.org/entity/Q130237291', 'http://www.wikidata.org/entity/Q130237292', 'http://www.wikidata.org/entity/Q130237293', 'http://www.wikidata.org/entity/Q130237294', 'http://www.wikidata.org/entity/Q130237295', 'http://www.wikidata.org/entity/Q130237296', 'http://www.wikidata.org/entity/Q130237297', 'http://www.wikidata.org/entity/Q130237298', 'http://www.wikidata.org/entity/Q130237299', 'http://www.wikidata.org/entity/Q130237300', 'http://www.wikidata.org/entity/Q130237301', 'http://www.wikidata.org/entity/Q130237302', 'http://www.wikidata.org/entity/Q130237303', 'http://www.wikidata.org/entity/Q130237304', 'http://www.wikidata.org/entity/Q130237305', 'http://www.wikidata.org/entity/Q130237306', 'http://www.wikidata.org/entity/Q130237307', 'http://www.wikidata.org/entity/Q130237308', 'http://www.wikidata.org/entity/Q130237309', 'http://www.wikidata.org/entity/Q130237310', 'http://www.wikidata.org/entity/Q130237311', 'http://www.wikidata.org/entity/Q130237312', 'http://www.wikidata.org/entity/Q130237314', 'http://www.wikidata.org/entity/Q130237315', 'http://www.wikidata.org/entity/Q130237316', 'http://www.wikidata.org/entity/Q130237317', 'http://www.wikidata.org/entity/Q130237318', 'http://www.wikidata.org/entity/Q130237319', 'http://www.wikidata.org/entity/Q130237320', 'http://www.wikidata.org/entity/Q130237321', 'http://www.wikidata.org/entity/Q130237322', 'http://www.wikidata.org/entity/Q130237323', 'http://www.wikidata.org/entity/Q130237324', 'http://www.wikidata.org/entity/Q130237325', 'http://www.wikidata.org/entity/Q130237326', 'http://www.wikidata.org/entity/Q130237327', 'http://www.wikidata.org/entity/Q130237328', 'http://www.wikidata.org/entity/Q130237329', 'http://www.wikidata.org/entity/Q130237330', 'http://www.wikidata.org/entity/Q130237331', 'http://www.wikidata.org/entity/Q130237332', 'http://www.wikidata.org/entity/Q130237333', 'http://www.wikidata.org/entity/Q130237334', 'http://www.wikidata.org/entity/Q130237335', 'http://www.wikidata.org/entity/Q130237336', 'http://www.wikidata.org/entity/Q130237337', 'http://www.wikidata.org/entity/Q130237338', 'http://www.wikidata.org/entity/Q130237339', 'http://www.wikidata.org/entity/Q130237340', 'http://www.wikidata.org/entity/Q130237341', 'http://www.wikidata.org/entity/Q130237342', 'http://www.wikidata.org/entity/Q130237343', 'http://www.wikidata.org/entity/Q130237344', 'http://www.wikidata.org/entity/Q130237345', 'http://www.wikidata.org/entity/Q130237346', 'http://www.wikidata.org/entity/Q130237347', 'http://www.wikidata.org/entity/Q130237348', 'http://www.wikidata.org/entity/Q130237349', 'http://www.wikidata.org/entity/Q130237350', 'http://www.wikidata.org/entity/Q130237351', 'http://www.wikidata.org/entity/Q130237353', 'http://www.wikidata.org/entity/Q130237354', 'http://www.wikidata.org/entity/Q130237355', 'http://www.wikidata.org/entity/Q130237356', 'http://www.wikidata.org/entity/Q130237357', 'http://www.wikidata.org/entity/Q130237358', 'http://www.wikidata.org/entity/Q130237359', 'http://www.wikidata.org/entity/Q130237360', 'http://www.wikidata.org/entity/Q130237361', 'http://www.wikidata.org/entity/Q130237362', 'http://www.wikidata.org/entity/Q130237363', 'http://www.wikidata.org/entity/Q130237364', 'http://www.wikidata.org/entity/Q130237365', 'http://www.wikidata.org/entity/Q130237366', 'http://www.wikidata.org/entity/Q130237367', 'http://www.wikidata.org/entity/Q130237368', 'http://www.wikidata.org/entity/Q130237369', 'http://www.wikidata.org/entity/Q130237370', 'http://www.wikidata.org/entity/Q130237371', 'http://www.wikidata.org/entity/Q130237372', 'http://www.wikidata.org/entity/Q130237373', 'http://www.wikidata.org/entity/Q130237374', 'http://www.wikidata.org/entity/Q130237375', 'http://www.wikidata.org/entity/Q130237376', 'http://www.wikidata.org/entity/Q130237377', 'http://www.wikidata.org/entity/Q130237378', 'http://www.wikidata.org/entity/Q130237379', 'http://www.wikidata.org/entity/Q130237380', 'http://www.wikidata.org/entity/Q130237381', 'http://www.wikidata.org/entity/Q130237382', 'http://www.wikidata.org/entity/Q130237383', 'http://www.wikidata.org/entity/Q130237384', 'http://www.wikidata.org/entity/Q130237385', 'http://www.wikidata.org/entity/Q130237386', 'http://www.wikidata.org/entity/Q130237387', 'http://www.wikidata.org/entity/Q130237388', 'http://www.wikidata.org/entity/Q130237389', 'http://www.wikidata.org/entity/Q130237390', 'http://www.wikidata.org/entity/Q130237391', 'http://www.wikidata.org/entity/Q130237392', 'http://www.wikidata.org/entity/Q130237393', 'http://www.wikidata.org/entity/Q130237394', 'http://www.wikidata.org/entity/Q130237395', 'http://www.wikidata.org/entity/Q130237396', 'http://www.wikidata.org/entity/Q130237397', 'http://www.wikidata.org/entity/Q130237398', 'http://www.wikidata.org/entity/Q130237399', 'http://www.wikidata.org/entity/Q130237400', 'http://www.wikidata.org/entity/Q130237402', 'http://www.wikidata.org/entity/Q130237403', 'http://www.wikidata.org/entity/Q130237404', 'http://www.wikidata.org/entity/Q130237405', 'http://www.wikidata.org/entity/Q130237406', 'http://www.wikidata.org/entity/Q130237407', 'http://www.wikidata.org/entity/Q130237408', 'http://www.wikidata.org/entity/Q130237409', 'http://www.wikidata.org/entity/Q130237410', 'http://www.wikidata.org/entity/Q130237411', 'http://www.wikidata.org/entity/Q130237412', 'http://www.wikidata.org/entity/Q130237413', 'http://www.wikidata.org/entity/Q130237414', 'http://www.wikidata.org/entity/Q130237415', 'http://www.wikidata.org/entity/Q130237416', 'http://www.wikidata.org/entity/Q130237417', 'http://www.wikidata.org/entity/Q130237419', 'http://www.wikidata.org/entity/Q130237420', 'http://www.wikidata.org/entity/Q130237421', 'http://www.wikidata.org/entity/Q130237422', 'http://www.wikidata.org/entity/Q130237423', 'http://www.wikidata.org/entity/Q130237424', 'http://www.wikidata.org/entity/Q130237425', 'http://www.wikidata.org/entity/Q130237426', 'http://www.wikidata.org/entity/Q130237427', 'http://www.wikidata.org/entity/Q130237428', 'http://www.wikidata.org/entity/Q130237429', 'http://www.wikidata.org/entity/Q130237430', 'http://www.wikidata.org/entity/Q130237431', 'http://www.wikidata.org/entity/Q130237432', 'http://www.wikidata.org/entity/Q130237433', 'http://www.wikidata.org/entity/Q130237434', 'http://www.wikidata.org/entity/Q130237435', 'http://www.wikidata.org/entity/Q130237436', 'http://www.wikidata.org/entity/Q130237437', 'http://www.wikidata.org/entity/Q130237438', 'http://www.wikidata.org/entity/Q130237439', 'http://www.wikidata.org/entity/Q130237440', 'http://www.wikidata.org/entity/Q130237441', 'http://www.wikidata.org/entity/Q130237442', 'http://www.wikidata.org/entity/Q130237443', 'http://www.wikidata.org/entity/Q130237444', 'http://www.wikidata.org/entity/Q130237445', 'http://www.wikidata.org/entity/Q130237446', 'http://www.wikidata.org/entity/Q130237447', 'http://www.wikidata.org/entity/Q130237448', 'http://www.wikidata.org/entity/Q130237449', 'http://www.wikidata.org/entity/Q130237450', 'http://www.wikidata.org/entity/Q130237451', 'http://www.wikidata.org/entity/Q130237452', 'http://www.wikidata.org/entity/Q130237453', 'http://www.wikidata.org/entity/Q130237454', 'http://www.wikidata.org/entity/Q130237455', 'http://www.wikidata.org/entity/Q130237456', 'http://www.wikidata.org/entity/Q130237457', 'http://www.wikidata.org/entity/Q130237458', 'http://www.wikidata.org/entity/Q130237459', 'http://www.wikidata.org/entity/Q130237460', 'http://www.wikidata.org/entity/Q130237461', 'http://www.wikidata.org/entity/Q130237462', 'http://www.wikidata.org/entity/Q130237463', 'http://www.wikidata.org/entity/Q130237464', 'http://www.wikidata.org/entity/Q130237465', 'http://www.wikidata.org/entity/Q130237466', 'http://www.wikidata.org/entity/Q130237467', 'http://www.wikidata.org/entity/Q130237468', 'http://www.wikidata.org/entity/Q130237469', 'http://www.wikidata.org/entity/Q130237471', 'http://www.wikidata.org/entity/Q130237472', 'http://www.wikidata.org/entity/Q130237473', 'http://www.wikidata.org/entity/Q130237474', 'http://www.wikidata.org/entity/Q130237475', 'http://www.wikidata.org/entity/Q130237476', 'http://www.wikidata.org/entity/Q130237477', 'http://www.wikidata.org/entity/Q130237478', 'http://www.wikidata.org/entity/Q130237479', 'http://www.wikidata.org/entity/Q130237480', 'http://www.wikidata.org/entity/Q130237481', 'http://www.wikidata.org/entity/Q130237482', 'http://www.wikidata.org/entity/Q130237484', 'http://www.wikidata.org/entity/Q130237485', 'http://www.wikidata.org/entity/Q130237487', 'http://www.wikidata.org/entity/Q130237488', 'http://www.wikidata.org/entity/Q130237489', 'http://www.wikidata.org/entity/Q130237490', 'http://www.wikidata.org/entity/Q130237491', 'http://www.wikidata.org/entity/Q130237492', 'http://www.wikidata.org/entity/Q130237493', 'http://www.wikidata.org/entity/Q130237494', 'http://www.wikidata.org/entity/Q130237495', 'http://www.wikidata.org/entity/Q130237496', 'http://www.wikidata.org/entity/Q130237497', 'http://www.wikidata.org/entity/Q130237498', 'http://www.wikidata.org/entity/Q130237499', 'http://www.wikidata.org/entity/Q130237500', 'http://www.wikidata.org/entity/Q130237501', 'http://www.wikidata.org/entity/Q130237502', 'http://www.wikidata.org/entity/Q130237503', 'http://www.wikidata.org/entity/Q130237504', 'http://www.wikidata.org/entity/Q130237505', 'http://www.wikidata.org/entity/Q130237506', 'http://www.wikidata.org/entity/Q130237507', 'http://www.wikidata.org/entity/Q130237508', 'http://www.wikidata.org/entity/Q130237509', 'http://www.wikidata.org/entity/Q130237510', 'http://www.wikidata.org/entity/Q130237511', 'http://www.wikidata.org/entity/Q130237513', 'http://www.wikidata.org/entity/Q130237514', 'http://www.wikidata.org/entity/Q130237515', 'http://www.wikidata.org/entity/Q130237516', 'http://www.wikidata.org/entity/Q130237517', 'http://www.wikidata.org/entity/Q130237518', 'http://www.wikidata.org/entity/Q130237520', 'http://www.wikidata.org/entity/Q130237521', 'http://www.wikidata.org/entity/Q130237522', 'http://www.wikidata.org/entity/Q130237524', 'http://www.wikidata.org/entity/Q130237525', 'http://www.wikidata.org/entity/Q130237526', 'http://www.wikidata.org/entity/Q130237527', 'http://www.wikidata.org/entity/Q130237529', 'http://www.wikidata.org/entity/Q130237530', 'http://www.wikidata.org/entity/Q130237531', 'http://www.wikidata.org/entity/Q130237532', 'http://www.wikidata.org/entity/Q130237534', 'http://www.wikidata.org/entity/Q130237535', 'http://www.wikidata.org/entity/Q130237536', 'http://www.wikidata.org/entity/Q130237537', 'http://www.wikidata.org/entity/Q130237538', 'http://www.wikidata.org/entity/Q130237539', 'http://www.wikidata.org/entity/Q130237540', 'http://www.wikidata.org/entity/Q130237541', 'http://www.wikidata.org/entity/Q130237542', 'http://www.wikidata.org/entity/Q130237543', 'http://www.wikidata.org/entity/Q130237544', 'http://www.wikidata.org/entity/Q130237545', 'http://www.wikidata.org/entity/Q130237546', 'http://www.wikidata.org/entity/Q130237547', 'http://www.wikidata.org/entity/Q130237548', 'http://www.wikidata.org/entity/Q130237549', 'http://www.wikidata.org/entity/Q130237550', 'http://www.wikidata.org/entity/Q130237552', 'http://www.wikidata.org/entity/Q130237553', 'http://www.wikidata.org/entity/Q130237554', 'http://www.wikidata.org/entity/Q130237555', 'http://www.wikidata.org/entity/Q130237556', 'http://www.wikidata.org/entity/Q130237557', 'http://www.wikidata.org/entity/Q130237558', 'http://www.wikidata.org/entity/Q130237559', 'http://www.wikidata.org/entity/Q130237560', 'http://www.wikidata.org/entity/Q130237561', 'http://www.wikidata.org/entity/Q130237562', 'http://www.wikidata.org/entity/Q130237563', 'http://www.wikidata.org/entity/Q130237564', 'http://www.wikidata.org/entity/Q130237565', 'http://www.wikidata.org/entity/Q130237566', 'http://www.wikidata.org/entity/Q130237567', 'http://www.wikidata.org/entity/Q130237570', 'http://www.wikidata.org/entity/Q130237571', 'http://www.wikidata.org/entity/Q130237572', 'http://www.wikidata.org/entity/Q130237573', 'http://www.wikidata.org/entity/Q130237574', 'http://www.wikidata.org/entity/Q130237575', 'http://www.wikidata.org/entity/Q130237576', 'http://www.wikidata.org/entity/Q130237577', 'http://www.wikidata.org/entity/Q130237578', 'http://www.wikidata.org/entity/Q130237579', 'http://www.wikidata.org/entity/Q130237581', 'http://www.wikidata.org/entity/Q130237582', 'http://www.wikidata.org/entity/Q130237584', 'http://www.wikidata.org/entity/Q130237585', 'http://www.wikidata.org/entity/Q130237587', 'http://www.wikidata.org/entity/Q130237588', 'http://www.wikidata.org/entity/Q130237589', 'http://www.wikidata.org/entity/Q130237591', 'http://www.wikidata.org/entity/Q130237592', 'http://www.wikidata.org/entity/Q130237593', 'http://www.wikidata.org/entity/Q130237594', 'http://www.wikidata.org/entity/Q130237597', 'http://www.wikidata.org/entity/Q130237598', 'http://www.wikidata.org/entity/Q130237599', 'http://www.wikidata.org/entity/Q130237601', 'http://www.wikidata.org/entity/Q130237602', 'http://www.wikidata.org/entity/Q130237603', 'http://www.wikidata.org/entity/Q130237604', 'http://www.wikidata.org/entity/Q130237605', 'http://www.wikidata.org/entity/Q130237607', 'http://www.wikidata.org/entity/Q130237608', 'http://www.wikidata.org/entity/Q130237609', 'http://www.wikidata.org/entity/Q130237611', 'http://www.wikidata.org/entity/Q130237612', 'http://www.wikidata.org/entity/Q130237613', 'http://www.wikidata.org/entity/Q130237615', 'http://www.wikidata.org/entity/Q130237616', 'http://www.wikidata.org/entity/Q130237617', 'http://www.wikidata.org/entity/Q130237618', 'http://www.wikidata.org/entity/Q130237619', 'http://www.wikidata.org/entity/Q130237620', 'http://www.wikidata.org/entity/Q130237621', 'http://www.wikidata.org/entity/Q130237623', 'http://www.wikidata.org/entity/Q130237624', 'http://www.wikidata.org/entity/Q130237625', 'http://www.wikidata.org/entity/Q130237626', 'http://www.wikidata.org/entity/Q130237627', 'http://www.wikidata.org/entity/Q130237628', 'http://www.wikidata.org/entity/Q130237629', 'http://www.wikidata.org/entity/Q130237630', 'http://www.wikidata.org</t>
+          <t>['http://www.wikidata.org/entity/Q3506451']</t>
         </is>
       </c>
       <c r="D8" t="b">
@@ -598,17 +598,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Give me the birth place of Frank Sinatra.</t>
+          <t>Who was the doctoral supervisor of Albert Einstein?</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q138578']</t>
+          <t>['http://www.wikidata.org/entity/Q116635', 'http://www.wikidata.org/entity/Q4175282', 'http://www.wikidata.org/entity/Q97154']</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q138578']</t>
+          <t>['http://www.wikidata.org/entity/Q116635', 'http://www.wikidata.org/entity/Q4175282', 'http://www.wikidata.org/entity/Q97154']</t>
         </is>
       </c>
       <c r="D9" t="b">
@@ -618,57 +618,57 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>How tall is Michael Jordan?</t>
+          <t>How many people live in Eurasia?</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>['198']</t>
+          <t>['5348554000']</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>['198']</t>
+          <t>['http://www.wikidata.org/entity/statement/Q5401-18d0ead9-483f-7270-c27d-09d51af3c182', 'http://www.wikidata.org/entity/statement/Q5401-b5b3488c-4558-47d1-764a-f68a17726bb5']</t>
         </is>
       </c>
       <c r="D10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Which holidays are celebrated around the world?</t>
+          <t>When was John Adams born?</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q103987830', 'http://www.wikidata.org/entity/Q104013369', 'http://www.wikidata.org/entity/Q116978631', 'http://www.wikidata.org/entity/Q21163268', 'http://www.wikidata.org/entity/Q10283187', 'http://www.wikidata.org/entity/Q111738564', 'http://www.wikidata.org/entity/Q112127159', 'http://www.wikidata.org/entity/Q124422802', 'http://www.wikidata.org/entity/Q18465013', 'http://www.wikidata.org/entity/Q125856465', 'http://www.wikidata.org/entity/Q1361434', 'http://www.wikidata.org/entity/Q1651570', 'http://www.wikidata.org/entity/Q2564633', 'http://www.wikidata.org/entity/Q333016', 'http://www.wikidata.org/entity/Q61359735', 'http://www.wikidata.org/entity/Q72318', 'http://www.wikidata.org/entity/Q744159', 'http://www.wikidata.org/entity/Q751738', 'http://www.wikidata.org/entity/Q110707177', 'http://www.wikidata.org/entity/Q45922130', 'http://www.wikidata.org/entity/Q57350935', 'http://www.wikidata.org/entity/Q57397044', 'http://www.wikidata.org/entity/Q116978568', 'http://www.wikidata.org/entity/Q2859605', 'http://www.wikidata.org/entity/Q113090457', 'http://www.wikidata.org/entity/Q115181793', 'http://www.wikidata.org/entity/Q115369110', 'http://www.wikidata.org/entity/Q115369980', 'http://www.wikidata.org/entity/Q115377287', 'http://www.wikidata.org/entity/Q21697589', 'http://www.wikidata.org/entity/Q122069654', 'http://www.wikidata.org/entity/Q1145566', 'http://www.wikidata.org/entity/Q11406184', 'http://www.wikidata.org/entity/Q11643728', 'http://www.wikidata.org/entity/Q20044441', 'http://www.wikidata.org/entity/Q28685931', 'http://www.wikidata.org/entity/Q11255045', 'http://www.wikidata.org/entity/Q11387821', 'http://www.wikidata.org/entity/Q11436695', 'http://www.wikidata.org/entity/Q11501518', 'http://www.wikidata.org/entity/Q11502138', 'http://www.wikidata.org/entity/Q11512398', 'http://www.wikidata.org/entity/Q11590440', 'http://www.wikidata.org/entity/Q11604982', 'http://www.wikidata.org/entity/Q6455253', 'http://www.wikidata.org/entity/Q111162467', 'http://www.wikidata.org/entity/Q124005660', 'http://www.wikidata.org/entity/Q130611902', 'http://www.wikidata.org/entity/Q13258770', 'http://www.wikidata.org/entity/Q2838743', 'http://www.wikidata.org/entity/Q3092925', 'http://www.wikidata.org/entity/Q123004384', 'http://www.wikidata.org/entity/Q4546230', 'http://www.wikidata.org/entity/Q1009535', 'http://www.wikidata.org/entity/Q1049141', 'http://www.wikidata.org/entity/Q1059995', 'http://www.wikidata.org/entity/Q1137351', 'http://www.wikidata.org/entity/Q1145630', 'http://www.wikidata.org/entity/Q1186410', 'http://www.wikidata.org/entity/Q1355051', 'http://www.wikidata.org/entity/Q1355833', 'http://www.wikidata.org/entity/Q1359602', 'http://www.wikidata.org/entity/Q1361434', 'http://www.wikidata.org/entity/Q1361489', 'http://www.wikidata.org/entity/Q17218111', 'http://www.wikidata.org/entity/Q483226', 'http://www.wikidata.org/entity/Q82405', 'http://www.wikidata.org/entity/Q101706322', 'http://www.wikidata.org/entity/Q10265921', 'http://www.wikidata.org/entity/Q10274', 'http://www.wikidata.org/entity/Q10281751', 'http://www.wikidata.org/entity/Q10313072', 'http://www.wikidata.org/entity/Q1034573', 'http://www.wikidata.org/entity/Q10379695', 'http://www.wikidata.org/entity/Q1038328', 'http://www.wikidata.org/entity/Q104842151', 'http://www.wikidata.org/entity/Q104842171', 'http://www.wikidata.org/entity/Q104844735', 'http://www.wikidata.org/entity/Q104853673', 'http://www.wikidata.org/entity/Q104861126', 'http://www.wikidata.org/entity/Q10488275', 'http://www.wikidata.org/entity/Q105047091', 'http://www.wikidata.org/entity/Q105047582', 'http://www.wikidata.org/entity/Q105047587', 'http://www.wikidata.org/entity/Q105271464', 'http://www.wikidata.org/entity/Q105393636', 'http://www.wikidata.org/entity/Q10560877', 'http://www.wikidata.org/entity/Q105742385', 'http://www.wikidata.org/entity/Q105742388', 'http://www.wikidata.org/entity/Q1058840', 'http://www.wikidata.org/entity/Q106010', 'http://www.wikidata.org/entity/Q106290028', 'http://www.wikidata.org/entity/Q106307776', 'http://www.wikidata.org/entity/Q106806190', 'http://www.wikidata.org/entity/Q106855753', 'http://www.wikidata.org/entity/Q1070437', 'http://www.wikidata.org/entity/Q107139413', 'http://www.wikidata.org/entity/Q10726425', 'http://www.wikidata.org/entity/Q107486932', 'http://www.wikidata.org/entity/Q107643630', 'http://www.wikidata.org/entity/Q108120675', 'http://www.wikidata.org/entity/Q108265918', 'http://www.wikidata.org/entity/Q108305674', 'http://www.wikidata.org/entity/Q108456662', 'http://www.wikidata.org/entity/Q108540687', 'http://www.wikidata.org/entity/Q10862448', 'http://www.wikidata.org/entity/Q108745010', 'http://www.wikidata.org/entity/Q10881633', 'http://www.wikidata.org/entity/Q108936865', 'http://www.wikidata.org/entity/Q10901070', 'http://www.wikidata.org/entity/Q109040869', 'http://www.wikidata.org/entity/Q10921475', 'http://www.wikidata.org/entity/Q109356066', 'http://www.wikidata.org/entity/Q109609391', 'http://www.wikidata.org/entity/Q109796906', 'http://www.wikidata.org/entity/Q110239836', 'http://www.wikidata.org/entity/Q1105149', 'http://www.wikidata.org/entity/Q110712627', 'http://www.wikidata.org/entity/Q110738072', 'http://www.wikidata.org/entity/Q110804043', 'http://www.wikidata.org/entity/Q11095193', 'http://www.wikidata.org/entity/Q11156396', 'http://www.wikidata.org/entity/Q11156590', 'http://www.wikidata.org/entity/Q11156602', 'http://www.wikidata.org/entity/Q111585601', 'http://www.wikidata.org/entity/Q111586257', 'http://www.wikidata.org/entity/Q111588212', 'http://www.wikidata.org/entity/Q111588631', 'http://www.wikidata.org/entity/Q111591927', 'http://www.wikidata.org/entity/Q111592030', 'http://www.wikidata.org/entity/Q111592221', 'http://www.wikidata.org/entity/Q111592231', 'http://www.wikidata.org/entity/Q111592392', 'http://www.wikidata.org/entity/Q111593121', 'http://www.wikidata.org/entity/Q111599061', 'http://www.wikidata.org/entity/Q111605534', 'http://www.wikidata.org/entity/Q111605672', 'http://www.wikidata.org/entity/Q111605780', 'http://www.wikidata.org/entity/Q111619857', 'http://www.wikidata.org/entity/Q111621136', 'http://www.wikidata.org/entity/Q111639188', 'http://www.wikidata.org/entity/Q111639464', 'http://www.wikidata.org/entity/Q111639796', 'http://www.wikidata.org/entity/Q111640394', 'http://www.wikidata.org/entity/Q111644691', 'http://www.wikidata.org/entity/Q111644855', 'http://www.wikidata.org/entity/Q111646483', 'http://www.wikidata.org/entity/Q111646603', 'http://www.wikidata.org/entity/Q111646902', 'http://www.wikidata.org/entity/Q111646942', 'http://www.wikidata.org/entity/Q111647178', 'http://www.wikidata.org/entity/Q111647244', 'http://www.wikidata.org/entity/Q111648147', 'http://www.wikidata.org/entity/Q111648327', 'http://www.wikidata.org/entity/Q111648357', 'http://www.wikidata.org/entity/Q111649590', 'http://www.wikidata.org/entity/Q111649647', 'http://www.wikidata.org/entity/Q111649691', 'http://www.wikidata.org/entity/Q111649919', 'http://www.wikidata.org/entity/Q111653594', 'http://www.wikidata.org/entity/Q111653613', 'http://www.wikidata.org/entity/Q111653631', 'http://www.wikidata.org/entity/Q111653637', 'http://www.wikidata.org/entity/Q111653675', 'http://www.wikidata.org/entity/Q111653779', 'http://www.wikidata.org/entity/Q111653938', 'http://www.wikidata.org/entity/Q111653958', 'http://www.wikidata.org/entity/Q111653969', 'http://www.wikidata.org/entity/Q111654007', 'http://www.wikidata.org/entity/Q111654040', 'http://www.wikidata.org/entity/Q111654093', 'http://www.wikidata.org/entity/Q111654098', 'http://www.wikidata.org/entity/Q111654121', 'http://www.wikidata.org/entity/Q111654136', 'http://www.wikidata.org/entity/Q111654241', 'http://www.wikidata.org/entity/Q111654346', 'http://www.wikidata.org/entity/Q111654469', 'http://www.wikidata.org/entity/Q111654484', 'http://www.wikidata.org/entity/Q111658731', 'http://www.wikidata.org/entity/Q111658801', 'http://www.wikidata.org/entity/Q111658833', 'http://www.wikidata.org/entity/Q111658927', 'http://www.wikidata.org/entity/Q111661297', 'http://www.wikidata.org/entity/Q111661840', 'http://www.wikidata.org/entity/Q111661872', 'http://www.wikidata.org/entity/Q111661886', 'http://www.wikidata.org/entity/Q111662034', 'http://www.wikidata.org/entity/Q111662035', 'http://www.wikidata.org/entity/Q111662040', 'http://www.wikidata.org/entity/Q111662133', 'http://www.wikidata.org/entity/Q111663221', 'http://www.wikidata.org/entity/Q111665328', 'http://www.wikidata.org/entity/Q111665519', 'http://www.wikidata.org/entity/Q111666301', 'http://www.wikidata.org/entity/Q111670117', 'http://www.wikidata.org/entity/Q111670231', 'http://www.wikidata.org/entity/Q111670397', 'http://www.wikidata.org/entity/Q111670481', 'http://www.wikidata.org/entity/Q111670617', 'http://www.wikidata.org/entity/Q111670624', 'http://www.wikidata.org/entity/Q111670628', 'http://www.wikidata.org/entity/Q111671698', 'http://www.wikidata.org/entity/Q111671968', 'http://www.wikidata.org/entity/Q111672442', 'http://www.wikidata.org/entity/Q111675204', 'http://www.wikidata.org/entity/Q111675217', 'http://www.wikidata.org/entity/Q111675293', 'http://www.wikidata.org/entity/Q111675405', 'http://www.wikidata.org/entity/Q111675518', 'http://www.wikidata.org/entity/Q111675816', 'http://www.wikidata.org/entity/Q111676530', 'http://www.wikidata.org/entity/Q111676789', 'http://www.wikidata.org/entity/Q111676828', 'http://www.wikidata.org/entity/Q111676959', 'http://www.wikidata.org/entity/Q111679720', 'http://www.wikidata.org/entity/Q111679753', 'http://www.wikidata.org/entity/Q111679830', 'http://www.wikidata.org/entity/Q111679840', 'http://www.wikidata.org/entity/Q111679871', 'http://www.wikidata.org/entity/Q111679978', 'http://www.wikidata.org/entity/Q111680097', 'http://www.wikidata.org/entity/Q111680142', 'http://www.wikidata.org/entity/Q111680149', 'http://www.wikidata.org/entity/Q111680197', 'http://www.wikidata.org/entity/Q111680221', 'http://www.wikidata.org/entity/Q111680229', 'http://www.wikidata.org/entity/Q111693657', 'http://www.wikidata.org/entity/Q111693675', 'http://www.wikidata.org/entity/Q111693696', 'http://www.wikidata.org/entity/Q111693773', 'http://www.wikidata.org/entity/Q111693781', 'http://www.wikidata.org/entity/Q111693947', 'http://www.wikidata.org/entity/Q111694017', 'http://www.wikidata.org/entity/Q111695525', 'http://www.wikidata.org/entity/Q111702011', 'http://www.wikidata.org/entity/Q111702051', 'http://www.wikidata.org/entity/Q111702063', 'http://www.wikidata.org/entity/Q111705727', 'http://www.wikidata.org/entity/Q111708136', 'http://www.wikidata.org/entity/Q111711151', 'http://www.wikidata.org/entity/Q111711160', 'http://www.wikidata.org/entity/Q111711162', 'http://www.wikidata.org/entity/Q111711184', 'http://www.wikidata.org/entity/Q111711264', 'http://www.wikidata.org/entity/Q111711268', 'http://www.wikidata.org/entity/Q111711270', 'http://www.wikidata.org/entity/Q111711273', 'http://www.wikidata.org/entity/Q111711278', 'http://www.wikidata.org/entity/Q111711311', 'http://www.wikidata.org/entity/Q111711342', 'http://www.wikidata.org/entity/Q111711421', 'http://www.wikidata.org/entity/Q111711540', 'http://www.wikidata.org/entity/Q111711547', 'http://www.wikidata.org/entity/Q111711661', 'http://www.wikidata.org/entity/Q111711757', 'http://www.wikidata.org/entity/Q111711903', 'http://www.wikidata.org/entity/Q111711907', 'http://www.wikidata.org/entity/Q111712005', 'http://www.wikidata.org/entity/Q111712010', 'http://www.wikidata.org/entity/Q111712059', 'http://www.wikidata.org/entity/Q111712123', 'http://www.wikidata.org/entity/Q111716408', 'http://www.wikidata.org/entity/Q111719293', 'http://www.wikidata.org/entity/Q111725575', 'http://www.wikidata.org/entity/Q111725911', 'http://www.wikidata.org/entity/Q111726390', 'http://www.wikidata.org/entity/Q111726615', 'http://www.wikidata.org/entity/Q111726617', 'http://www.wikidata.org/entity/Q111726635', 'http://www.wikidata.org/entity/Q111726669', 'http://www.wikidata.org/entity/Q111726714', 'http://www.wikidata.org/entity/Q111726768', 'http://www.wikidata.org/entity/Q111726774', 'http://www.wikidata.org/entity/Q111726793', 'http://www.wikidata.org/entity/Q111726805', 'http://www.wikidata.org/entity/Q111734330', 'http://www.wikidata.org/entity/Q111734453', 'http://www.wikidata.org/entity/Q111734646', 'http://www.wikidata.org/entity/Q111734661', 'http://www.wikidata.org/entity/Q111734681', 'http://www.wikidata.org/entity/Q111734708', 'http://www.wikidata.org/entity/Q111734879', 'http://www.wikidata.org/entity/Q111734906', 'http://www.wikidata.org/entity/Q111734910', 'http://www.wikidata.org/entity/Q111734978', 'http://www.wikidata.org/entity/Q111735009', 'http://www.wikidata.org/entity/Q111735146', 'http://www.wikidata.org/entity/Q111735183', 'http://www.wikidata.org/entity/Q111735311', 'http://www.wikidata.org/entity/Q111738073', 'http://www.wikidata.org/entity/Q111738552', 'http://www.wikidata.org/entity/Q111738762', 'http://www.wikidata.org/entity/Q111738881', 'http://www.wikidata.org/entity/Q111743473', 'http://www.wikidata.org/entity/Q111743614', 'http://www.wikidata.org/entity/Q111743635', 'http://www.wikidata.org/entity/Q111743658', 'http://www.wikidata.org/entity/Q111743894', 'http://www.wikidata.org/entity/Q111743903', 'http://www.wikidata.org/entity/Q111743905', 'http://www.wikidata.org/entity/Q111743922', 'http://www.wikidata.org/entity/Q111744105', 'http://www.wikidata.org/entity/Q111744185', 'http://www.wikidata.org/entity/Q111744196', 'http://www.wikidata.org/entity/Q111744206', 'http://www.wikidata.org/entity/Q111744231', 'http://www.wikidata.org/entity/Q111744233', 'http://www.wikidata.org/entity/Q111744287', 'http://www.wikidata.org/entity/Q111750057', 'http://www.wikidata.org/entity/Q111750098', 'http://www.wikidata.org/entity/Q111750104', 'http://www.wikidata.org/entity/Q111750108', 'http://www.wikidata.org/entity/Q111750391', 'http://www.wikidata.org/entity/Q111750396', 'http://www.wikidata.org/entity/Q111750414', 'http://www.wikidata.org/entity/Q111750482', 'http://www.wikidata.org/entity/Q111750486', 'http://www.wikidata.org/entity/Q111750538', 'http://www.wikidata.org/entity/Q111750619', 'http://www.wikidata.org/entity/Q111750632', 'http://www.wikidata.org/entity/Q111750636', 'http://www.wikidata.org/entity/Q111750803', 'http://www.wikidata.org/entity/Q111772339', 'http://www.wikidata.org/entity/Q111772429', 'http://www.wikidata.org/entity/Q111772455', 'http://www.wikidata.org/entity/Q111772465', 'http://www.wikidata.org/entity/Q111772467', 'http://www.wikidata.org/entity/Q111772470', 'http://www.wikidata.org/entity/Q111772479', 'http://www.wikidata.org/entity/Q111772481', 'http://www.wikidata.org/entity/Q111772492', 'http://www.wikidata.org/entity/Q111772538', 'http://www.wikidata.org/entity/Q111772542', 'http://www.wikidata.org/entity/Q111772579', 'http://www.wikidata.org/entity/Q111772903', 'http://www.wikidata.org/entity/Q111774488', 'http://www.wikidata.org/entity/Q111774855', 'http://www.wikidata.org/entity/Q111775976', 'http://www.wikidata.org/entity/Q111781307', 'http://www.wikidata.org/entity/Q111781313', 'http://www.wikidata.org/entity/Q111781415', 'http://www.wikidata.org/entity/Q111782305', 'http://www.wikidata.org/entity/Q111782406', 'http://www.wikidata.org/entity/Q111792237', 'http://www.wikidata.org/entity/Q111792287', 'http://www.wikidata.org/entity/Q111792297', 'http://www.wikidata.org/entity/Q111792422', 'http://www.wikidata.org/entity/Q111792427', 'http://www.wikidata.org/entity/Q111792455', 'http://www.wikidata.org/entity/Q111792652', 'http://www.wikidata.org/entity/Q111792657', 'http://www.wikidata.org/entity/Q111792669', 'http://www.wikidata.org/entity/Q111795166', 'http://www.wikidata.org/entity/Q111795170', 'http://www.wikidata.org/entity/Q111795181', 'http://www.wikidata.org/entity/Q111795190', 'http://www.wikidata.org/entity/Q111795208', 'http://www.wikidata.org/entity/Q111795217', 'http://www.wikidata.org/entity/Q111795226', 'http://www.wikidata.org/entity/Q111795230', 'http://www.wikidata.org/entity/Q111795234', 'http://www.wikidata.org/entity/Q111795238', 'http://www.wikidata.org/entity/Q111798789', 'http://www.wikidata.org/entity/Q111799191', 'http://www.wikidata.org/entity/Q111799265', 'http://www.wikidata.org/entity/Q111799326', 'http://www.wikidata.org/entity/Q111799364', 'http://www.wikidata.org/entity/Q111799715', 'http://www.wikidata.org/entity/Q111800151', 'http://www.wikidata.org/entity/Q111800560', 'http://www.wikidata.org/entity/Q111800590', 'http://www.wikidata.org/entity/Q111800661', 'http://www.wikidata.org/entity/Q111800678', 'http://www.wikidata.org/entity/Q111800735', 'http://www.wikidata.org/entity/Q111800758', 'http://www.wikidata.org/entity/Q111801201', 'http://www.wikidata.org/entity/Q111801219', 'http://www.wikidata.org/entity/Q111801257', 'http://www.wikidata.org/entity/Q111801366', 'http://www.wikidata.org/entity/Q111801395', 'http://www.wikidata.org/entity/Q111801411', 'http://www.wikidata.org/entity/Q111801450', 'http://www.wikidata.org/entity/Q111801507', 'http://www.wikidata.org/entity/Q111801550', 'http://www.wikidata.org/entity/Q111810594', 'http://www.wikidata.org/entity/Q111810721', 'http://www.wikidata.org/entity/Q111811564', 'http://www.wikidata.org/entity/Q111811624', 'http://www.wikidata.org/entity/Q111811681', 'http://www.wikidata.org/entity/Q111812563', 'http://www.wikidata.org/entity/Q111812584', 'http://www.wikidata.org/entity/Q111812855', 'http://www.wikidata.org/entity/Q111816790', 'http://www.wikidata.org/entity/Q111817714', 'http://www.wikidata.org/entity/Q111817744', 'http://www.wikidata.org/entity/Q111817829', 'http://www.wikidata.org/entity/Q111817846', 'http://www.wikidata.org/entity/Q111817920', 'http://www.wikidata.org/entity/Q111818123', 'http://www.wikidata.org/entity/Q111824276', 'http://www.wikidata.org/entity/Q111824296', 'http://www.wikidata.org/entity/Q111824414', 'http://www.wikidata.org/entity/Q111824439', 'http://www.wikidata.org/entity/Q111824771', 'http://www.wikidata.org/entity/Q111824800', 'http://www.wikidata.org/entity/Q111824823', 'http://www.wikidata.org/entity/Q111824918', 'http://www.wikidata.org/entity/Q111825400', 'http://www.wikidata.org/entity/Q111825424', 'http://www.wikidata.org/entity/Q111825449', 'http://www.wikidata.org/entity/Q111825554', 'http://www.wikidata.org/entity/Q111825613', 'http://www.wikidata.org/entity/Q111825677', 'http://www.wikidata.org/entity/Q111825713', 'http://www.wikidata.org/entity/Q111825832', 'http://www.wikidata.org/entity/Q111826063', 'http://www.wikidata.org/entity/Q111826089', 'http://www.wikidata.org/entity/Q111830034', 'http://www.wikidata.org/entity/Q111830188', 'http://www.wikidata.org/entity/Q111837290', 'http://www.wikidata.org/entity/Q111837438', 'http://www.wikidata.org/entity/Q111837464', 'http://www.wikidata.org/entity/Q111837474', 'http://www.wikidata.org/entity/Q111837785', 'http://www.wikidata.org/entity/Q111837834', 'http://www.wikidata.org/entity/Q111837845', 'http://www.wikidata.org/entity/Q111837855', 'http://www.wikidata.org/entity/Q111837912', 'http://www.wikidata.org/entity/Q111837991', 'http://www.wikidata.org/entity/Q111848069', 'http://www.wikidata.org/entity/Q111848409', 'http://www.wikidata.org/entity/Q111848456', 'http://www.wikidata.org/entity/Q111848558', 'http://www.wikidata.org/entity/Q111848588', 'http://www.wikidata.org/entity/Q111848721', 'http://www.wikidata.org/entity/Q111848749', 'http://www.wikidata.org/entity/Q111848889', 'http://www.wikidata.org/entity/Q111903596', 'http://www.wikidata.org/entity/Q111903847', 'http://www.wikidata.org/entity/Q111903850', 'http://www.wikidata.org/entity/Q111903876', 'http://www.wikidata.org/entity/Q111903878', 'http://www.wikidata.org/entity/Q111903929', 'http://www.wikidata.org/entity/Q111903935', 'http://www.wikidata.org/entity/Q111903958', 'http://www.wikidata.org/entity/Q111904025', 'http://www.wikidata.org/entity/Q111904053', 'http://www.wikidata.org/entity/Q111904059', 'http://www.wikidata.org/entity/Q111904155', 'http://www.wikidata.org/entity/Q111905212', 'http://www.wikidata.org/entity/Q111905225', 'http://www.wikidata.org/entity/Q111905272', 'http://www.wikidata.org/entity/Q111906585', 'http://www.wikidata.org/entity/Q111906632', 'http://www.wikidata.org/entity/Q111906707', 'http://www.wikidata.org/entity/Q111907290', 'http://www.wikidata.org/entity/Q111907317', 'http://www.wikidata.org/entity/Q111908878', 'http://www.wikidata.org/entity/Q111908880', 'http://www.wikidata.org/entity/Q111908884', 'http://www.wikidata.org/entity/Q111908910', 'http://www.wikidata.org/entity/Q111909231', 'http://www.wikidata.org/entity/Q111909314', 'http://www.wikidata.org/entity/Q111909357', 'http://www.wikidata.org/entity/Q111909361', 'http://www.wikidata.org/entity/Q111909369', 'http://www.wikidata.org/entity/Q111909483', 'http://www.wikidata.org/entity/Q111909520', 'http://www.wikidata.org/entity/Q111909557', 'http://www.wikidata.org/entity/Q111909632', 'http://www.wikidata.org/entity/Q111909656', 'http://www.wikidata.org/entity/Q111909659', 'http://www.wikidata.org/entity/Q111909665', 'http://www.wikidata.org/entity/Q111909679', 'http://www.wikidata.org/entity/Q111909683', 'http://www.wikidata.org/entity/Q111909686', 'http://www.wikidata.org/entity/Q111918622', 'http://www.wikidata.org/entity/Q111972328', 'http://www.wikidata.org/entity/Q111972588', 'http://www.wikidata.org/entity/Q111972596', 'http://www.wikidata.org/entity/Q111972626', 'http://www.wikidata.org/entity/Q111972641', 'http://www.wikidata.org/entity/Q111972655', 'http://www.wikidata.org/entity/Q111972667', 'http://www.wikidata.org/entity/Q111972760', 'http://www.wikidata.org/entity/Q111972775', 'http://www.wikidata.org/entity/Q111981575', 'http://www.wikidata.org/entity/Q111981578', 'http://www.wikidata.org/entity/Q111981586', 'http://www.wikidata.org/entity/Q111981600', 'http://www.wikidata.org/entity/Q111981655', 'http://www.wikidata.org/entity/Q111981806', 'http://www.wikidata.org/entity/Q111984435', 'http://www.wikidata.org/entity/Q111993442', 'http://www.wikidata.org/entity/Q111993561', 'http://www.wikidata.org/entity/Q112028016', 'http://www.wikidata.org/entity/Q112028058', 'http://www.wikidata.org/entity/Q112030707', 'http://www.wikidata.org/entity/Q112037464', 'http://www.wikidata.org/entity/Q112038287', 'http://www.wikidata.org/entity/Q112040430', 'http://www.wikidata.org/entity/Q112053302', 'http://www.wikidata.org/entity/Q112059989', 'http://www.wikidata.org/entity/Q112063713', 'http://www.wikidata.org/entity/Q112087493', 'http://www.wikidata.org/entity/Q112127176', 'http://www.wikidata.org/entity/Q112183753', 'http://www.wikidata.org/entity/Q112190885', 'http://www.wikidata.org/entity/Q112263083', 'http://www.wikidata.org/entity/Q112667083', 'http://www.wikidata.org/entity/Q112667550', 'http://www.wikidata.org/entity/Q112669313', 'http://www.wikidata.org/entity/Q112669383', 'http://www.wikidata.org/entity/Q112681996', 'http://www.wikidata.org/entity/Q112746421', 'http://www.wikidata.org/entity/Q112747808', 'http://www.wikidata.org/entity/Q112894949', 'http://www.wikidata.org/entity/Q112894986', 'http://www.wikidata.org/entity/Q113015050', 'http://www.wikidata.org/entity/Q113072738', 'http://www.wikidata.org/entity/Q1131707', 'http://www.wikidata.org/entity/Q113272299', 'http://www.wikidata.org/entity/Q113272409', 'http://www.wikidata.org/entity/Q113272932', 'http://www.wikidata.org/entity/Q113499373', 'http://www.wikidata.org/entity/Q113499494', 'http://www.wikidata.org/entity/Q113650760', 'http://www.wikidata.org/entity/Q11368765', 'http://www.wikidata.org/entity/Q113811579', 'http://www.wikidata.org/entity/Q113813231', 'http://www.wikidata.org/entity/Q113828978', 'http://www.wikidata.org/entity/Q113830063', 'http://www.wikidata.org/entity/Q113841626', 'http://www.wikidata.org/entity/Q113849016', 'http://www.wikidata.org/entity/Q113860611', 'http://www.wikidata.org/entity/Q113860644', 'http://www.wikidata.org/entity/Q113861194', 'http://www.wikidata.org/entity/Q113882354', 'http://www.wikidata.org/entity/Q113884368', 'http://www.wikidata.org/entity/Q113901976', 'http://www.wikidata.org/entity/Q113904662', 'http://www.wikidata.org/entity/Q1139536', 'http://www.wikidata.org/entity/Q113955599', 'http://www.wikidata.org/entity/Q113955616', 'http://www.wikidata.org/entity/Q113955620', 'http://www.wikidata.org/entity/Q113955692', 'http://www.wikidata.org/entity/Q113961851', 'http://www.wikidata.org/entity/Q113961888', 'http://www.wikidata.org/entity/Q113961932', 'http://www.wikidata.org/entity/Q114028189', 'http://www.wikidata.org/entity/Q114046091', 'http://www.wikidata.org/entity/Q114056617', 'http://www.wikidata.org/entity/Q114057278', 'http://www.wikidata.org/entity/Q114059225', 'http://www.wikidata.org/entity/Q114243677', 'http://www.wikidata.org/entity/Q114454471', 'http://www.wikidata.org/entity/Q1145566', 'http://www.wikidata.org/entity/Q1145630', 'http://www.wikidata.org/entity/Q114582556', 'http://www.wikidata.org/entity/Q114588676', 'http://www.wikidata.org/entity/Q114604', 'http://www.wikidata.org/entity/Q114947458', 'http://www.wikidata.org/entity/Q114948159', 'http://www.wikidata.org/entity/Q114996688', 'http://www.wikidata.org/entity/Q114997174', 'http://www.wikidata.org/entity/Q115341348', 'http://www.wikidata.org/entity/Q115367992', 'http://www.wikidata.org/entity/Q115397386', 'http://www.wikidata.org/entity/Q115517924', 'http://www.wikidata.org/entity/Q115764515', 'http://www.wikidata.org/entity/Q115801523', 'http://www.wikidata.org/entity/Q115912774', 'http://www.wikidata.org/entity/Q115990472', 'http://www.wikidata.org/entity/Q116414186', 'http://www.wikidata.org/entity/Q116690653', 'http://www.wikidata.org/entity/Q117421915', 'http://www.wikidata.org/entity/Q117695225', 'http://www.wikidata.org/entity/Q117751349', 'http://www.wikidata.org/entity/Q117795094', 'http://www.wikidata.org/entity/Q11789705', 'http://www.wikidata.org/entity/Q118128483', 'http://www.wikidata.org/entity/Q11921906', 'http://www.wikidata.org/entity/Q11938851', 'http://www.wikidata.org/entity/Q119496586', 'http://www.wikidata.org/entity/Q11993043', 'http://www.wikidata.org/entity/Q1207931', 'http://www.wikidata.org/entity/Q1207932', 'http://www.wikidata.org/entity/Q120837533', 'http://www.wikidata.org/entity/Q121886956', 'http://www.wikidata.org/entity/Q122068698', 'http://www.wikidata.org/entity/Q122188018', 'http://www.wikidata.org/entity/Q12228863', 'http://www.wikidata.org/entity/Q12228866', 'http://www.wikidata.org/entity/Q12228868', 'http://www.wikidata.org/entity/Q12228876', 'http://www.wikidata.org/entity/Q12228884', 'http://www.wikidata.org/entity/Q12252186', 'http://www.wikidata.org/entity/Q12277858', 'http://www.wikidata.org/entity/Q122832546', 'http://www.wikidata.org/entity/Q12314502', 'http://www.wikidata.org/entity/Q123337193', 'http://www.wikidata.org/entity/Q123592992', 'http://www.wikidata.org/entity/Q12361577', 'http://www.wikidata.org/entity/Q123746478', 'http://www.wikidata.org/entity/Q12376028', 'http://www.wikidata.org/entity/Q12378350', 'http://www.wikidata.org/entity/Q124036138', 'http://www.wikidata.org/entity/Q12407929', 'http://www.wikidata.org/entity/Q12411505', 'http://www.wikidata.org/entity/Q124367042', 'http://www.wikidata.org/entity/Q124504910', 'http://www.wikidata.org/entity/Q124564384', 'http://www.wikidata.org/entity/Q124612831', 'http://www.wikidata.org/entity/Q124615758', 'http://www.wikidata.org/entity/Q124619352', 'http://www.wikidata.org/entity/Q124620804', 'http://www.wikidata.org/entity/Q124620822', 'http://www.wikidata.org/entity/Q124707699', 'http://www.wikidata.org/entity/Q124820083', 'http://www.wikidata.org/entity/Q124830280', 'http://www.wikidata.org/entity/Q124857570', 'http://www.wikidata.org/entity/Q124858688', 'http://www.wikidata.org/entity/Q124858953', 'http://www.wikidata.org/entity/Q125149734', 'http://www.wikidata.org/entity/Q125205121', 'http://www.wikidata.org/entity/Q1254268', 'http://www.wikidata.org/entity/Q125510673', 'http://www.wikidata.org/entity/Q125511630', 'http://www.wikidata.org/entity/Q125521675', 'http://www.wikidata.org/entity/Q125521758', 'http://www.wikidata.org/entity/Q125555445', 'http://www.wikidata.org/entity/Q125566609', 'http://www.wikidata.org/entity/Q125577561', 'http://www.wikidata.org/entity/Q125592462', 'http://www.wikidata.org/entity/Q12560060', 'http://www.wikidata.org/entity/Q125688458', 'http://www.wikidata.org/entity/Q125688603', 'http://www.wikidata.org/entity/Q125700972', 'http://www.wikidata.org/entity/Q125704427', 'http://www.wikidata.org/entity/Q125747483', 'http://www.wikidata.org/entity/Q125749644', 'http://www.wikidata.org/entity/Q125758800', 'http://www.wikidata.org/entity/Q125759229', 'http://www.wikidata.org/entity/Q125845551', 'http://www.wikidata.org/entity/Q12584835', 'http://www.wikidata.org/entity/Q125856465', 'http://www.wikidata.org/entity/Q125867175', 'http://www.wikidata.org/entity/Q125867458', 'http://www.wikidata.org/entity/Q125867756', 'http://www.wikidata.org/entity/Q125867888', 'http://www.wikidata.org/entity/Q125869488', 'http://www.wikidata.org/entity/Q125879646', 'http://www.wikidata.org/entity/Q125879891', 'http://www.wikidata.org/entity/Q125883649', 'http://www.wikidata.org/entity/Q125883847', 'http://www.wikidata.org/entity/Q125890530', 'http://www.wikidata.org/entity/Q125890753', 'http://www.wikidata.org/entity/Q125891443', 'http://www.wikidata.org/entity/Q125891720', 'http://www.wikidata.org/entity/Q125895110', 'http://www.wikidata.org/entity/Q125895155', 'http://www.wikidata.org/entity/Q125899181', 'http://www.wikidata.org/entity/Q125899513', 'http://www.wikidata.org/entity/Q125901134', 'http://www.wikidata.org/entity/Q125903138', 'http://www.wikidata.org/entity/Q125910729', 'http://www.wikidata.org/entity/Q125910806', 'http://www.wikidata.org/entity/Q125911055', 'http://www.wikidata.org/entity/Q125911072', 'http://www.wikidata.org/entity/Q125914666', 'http://www.wikidata.org/entity/Q125914885', 'http://www.wikidata.org/entity/Q125921693', 'http://www.wikidata.org/entity/Q125922831', 'http://www.wikidata.org/entity/Q125922882', 'http://www.wikidata.org/entity/Q125926636', 'http://www.wikidata.org/entity/Q125932740', 'http://www.wikidata.org/entity/Q125936101', 'http://www.wikidata.org/entity/Q125936683', 'http://www.wikidata.org/entity/Q125956876', 'http://www.wikidata.org/entity/Q125959131', 'http://www.wikidata.org/entity/Q125965703', 'http://www.wikidata.org/entity/Q125966437', 'http://www.wikidata.org/entity/Q125966992', 'http://www.wikidata.org/entity/Q125968806', 'http://www.wikidata.org/entity/Q125969610', 'http://www.wikidata.org/entity/Q125970539', 'http://www.wikidata.org/entity/Q125984409', 'http://www.wikidata.org/entity/Q125984492', 'http://www.wikidata.org/entity/Q125994583', 'http://www.wikidata.org/entity/Q125997034', 'http://www.wikidata.org/entity/Q125998688', 'http://www.wikidata.org/entity/Q125998803', 'http://www.wikidata.org/entity/Q125998897', 'http://www.wikidata.org/entity/Q125999072', 'http://www.wikidata.org/entity/Q12599950', 'http://www.wikidata.org/entity/Q126010095', 'http://www.wikidata.org/entity/Q126010128', 'http://www.wikidata.org/entity/Q126028447', 'http://www.wikidata.org/entity/Q126028546', 'http://www.wikidata.org/entity/Q126032653', 'http://www.wikidata.org/entity/Q126126323', 'http://www.wikidata.org/entity/Q126126778', 'http://www.wikidata.org/entity/Q12613371', 'http://www.wikidata.org/entity/Q12629515', 'http://www.wikidata.org/entity/Q126325524', 'http://www.wikidata.org/entity/Q126361854', 'http://www.wikidata.org/entity/Q126362969', 'http://www.wikidata.org/entity/Q126371412', 'http://www.wikidata.org/entity/Q126371457', 'http://www.wikidata.org/entity/Q126371864', 'http://www.wikidata.org/entity/Q126371886', 'http://www.wikidata.org/entity/Q126372368', 'http://www.wikidata.org/entity/Q126372458', 'http://www.wikidata.org/entity/Q126372576', 'http://www.wikidata.org/entity/Q126415038', 'http://www.wikidata.org/entity/Q126456102', 'http://www.wikidata.org/entity/Q126477003', 'http://www.wikidata.org/entity/Q126477086', 'http://www.wikidata.org/entity/Q126477151', 'http://www.wikidata.org/entity/Q126477162', 'http://www.wikidata.org/entity/Q126478091', 'http://www.wikidata.org/entity/Q126478228', 'http://www.wikidata.org/entity/Q126511431', 'http://www.wikidata.org/entity/Q126513767', 'http://www.wikidata.org/entity/Q126593634', 'http://www.wikidata.org/entity/Q12663413', 'http://www.wikidata.org/entity/Q126666887', 'http://www.wikidata.org/entity/Q126709387', 'http://www.wikidata.org/entity/Q126721902', 'http://www.wikidata.org/entity/Q126726117', 'http://www.wikidata.org/entity/Q126811008', 'http://www.wikidata.org/e</t>
+          <t>['1735-10-30T00:00:00Z']</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q100329955', 'http://www.wikidata.org/entity/Q100597341', 'http://www.wikidata.org/entity/Q100860934', 'http://www.wikidata.org/entity/Q101026979', 'http://www.wikidata.org/entity/Q101545880', 'http://www.wikidata.org/entity/Q101627559', 'http://www.wikidata.org/entity/Q1016833', 'http://www.wikidata.org/entity/Q101706322', 'http://www.wikidata.org/entity/Q102276948', 'http://www.wikidata.org/entity/Q102398478', 'http://www.wikidata.org/entity/Q10244', 'http://www.wikidata.org/entity/Q10253', 'http://www.wikidata.org/entity/Q1025481', 'http://www.wikidata.org/entity/Q10259922', 'http://www.wikidata.org/entity/Q10265947', 'http://www.wikidata.org/entity/Q10281787', 'http://www.wikidata.org/entity/Q10329424', 'http://www.wikidata.org/entity/Q103821550', 'http://www.wikidata.org/entity/Q1038328', 'http://www.wikidata.org/entity/Q103956800', 'http://www.wikidata.org/entity/Q10398273', 'http://www.wikidata.org/entity/Q104051143', 'http://www.wikidata.org/entity/Q10412386', 'http://www.wikidata.org/entity/Q10416096', 'http://www.wikidata.org/entity/Q10418897', 'http://www.wikidata.org/entity/Q104224166', 'http://www.wikidata.org/entity/Q1043596', 'http://www.wikidata.org/entity/Q104601590', 'http://www.wikidata.org/entity/Q104625773', 'http://www.wikidata.org/entity/Q104758920', 'http://www.wikidata.org/entity/Q10481350', 'http://www.wikidata.org/entity/Q104920297', 'http://www.wikidata.org/entity/Q10494624', 'http://www.wikidata.org/entity/Q10495964', 'http://www.wikidata.org/entity/Q10496086', 'http://www.wikidata.org/entity/Q10501512', 'http://www.wikidata.org/entity/Q1050292', 'http://www.wikidata.org/entity/Q105043914', 'http://www.wikidata.org/entity/Q105121443', 'http://www.wikidata.org/entity/Q105360445', 'http://www.wikidata.org/entity/Q105393711', 'http://www.wikidata.org/entity/Q105394069', 'http://www.wikidata.org/entity/Q10541207', 'http://www.wikidata.org/entity/Q1054558', 'http://www.wikidata.org/entity/Q105663779', 'http://www.wikidata.org/entity/Q10586365', 'http://www.wikidata.org/entity/Q10601007', 'http://www.wikidata.org/entity/Q10601355', 'http://www.wikidata.org/entity/Q106019359', 'http://www.wikidata.org/entity/Q106043577', 'http://www.wikidata.org/entity/Q106078232', 'http://www.wikidata.org/entity/Q106200291', 'http://www.wikidata.org/entity/Q106240773', 'http://www.wikidata.org/entity/Q106290028', 'http://www.wikidata.org/entity/Q106307776', 'http://www.wikidata.org/entity/Q10631904', 'http://www.wikidata.org/entity/Q106331005', 'http://www.wikidata.org/entity/Q106349026', 'http://www.wikidata.org/entity/Q106369745', 'http://www.wikidata.org/entity/Q106436015', 'http://www.wikidata.org/entity/Q106505905', 'http://www.wikidata.org/entity/Q10666884', 'http://www.wikidata.org/entity/Q106675733', 'http://www.wikidata.org/entity/Q106689897', 'http://www.wikidata.org/entity/Q10669318', 'http://www.wikidata.org/entity/Q10669370', 'http://www.wikidata.org/entity/Q10669371', 'http://www.wikidata.org/entity/Q10685840', 'http://www.wikidata.org/entity/Q10689144', 'http://www.wikidata.org/entity/Q10689145', 'http://www.wikidata.org/entity/Q10689146', 'http://www.wikidata.org/entity/Q106899527', 'http://www.wikidata.org/entity/Q10698576', 'http://www.wikidata.org/entity/Q10698931', 'http://www.wikidata.org/entity/Q10698932', 'http://www.wikidata.org/entity/Q10698935', 'http://www.wikidata.org/entity/Q10698936', 'http://www.wikidata.org/entity/Q10698937', 'http://www.wikidata.org/entity/Q10699347', 'http://www.wikidata.org/entity/Q107015910', 'http://www.wikidata.org/entity/Q10701677', 'http://www.wikidata.org/entity/Q10701968', 'http://www.wikidata.org/entity/Q1070318', 'http://www.wikidata.org/entity/Q10714715', 'http://www.wikidata.org/entity/Q10726998', 'http://www.wikidata.org/entity/Q107309593', 'http://www.wikidata.org/entity/Q107718805', 'http://www.wikidata.org/entity/Q107739995', 'http://www.wikidata.org/entity/Q108010714', 'http://www.wikidata.org/entity/Q108101493', 'http://www.wikidata.org/entity/Q108131371', 'http://www.wikidata.org/entity/Q108219988', 'http://www.wikidata.org/entity/Q108315106', 'http://www.wikidata.org/entity/Q108392466', 'http://www.wikidata.org/entity/Q108424805', 'http://www.wikidata.org/entity/Q10854401', 'http://www.wikidata.org/entity/Q10855559', 'http://www.wikidata.org/entity/Q108660772', 'http://www.wikidata.org/entity/Q10868404', 'http://www.wikidata.org/entity/Q108730127', 'http://www.wikidata.org/entity/Q108749396', 'http://www.wikidata.org/entity/Q108749484', 'http://www.wikidata.org/entity/Q108814176', 'http://www.wikidata.org/entity/Q108936669', 'http://www.wikidata.org/entity/Q10909572', 'http://www.wikidata.org/entity/Q109121006', 'http://www.wikidata.org/entity/Q1091428', 'http://www.wikidata.org/entity/Q10921477', 'http://www.wikidata.org/entity/Q109285268', 'http://www.wikidata.org/entity/Q109329448', 'http://www.wikidata.org/entity/Q109329455', 'http://www.wikidata.org/entity/Q109356066', 'http://www.wikidata.org/entity/Q109381834', 'http://www.wikidata.org/entity/Q109381883', 'http://www.wikidata.org/entity/Q109440429', 'http://www.wikidata.org/entity/Q109455204', 'http://www.wikidata.org/entity/Q10955171', 'http://www.wikidata.org/entity/Q109558468', 'http://www.wikidata.org/entity/Q109609391', 'http://www.wikidata.org/entity/Q10964022', 'http://www.wikidata.org/entity/Q109827527', 'http://www.wikidata.org/entity/Q109838056', 'http://www.wikidata.org/entity/Q109908577', 'http://www.wikidata.org/entity/Q11002663', 'http://www.wikidata.org/entity/Q110091424', 'http://www.wikidata.org/entity/Q110128398', 'http://www.wikidata.org/entity/Q110206440', 'http://www.wikidata.org/entity/Q110239836', 'http://www.wikidata.org/entity/Q110639888', 'http://www.wikidata.org/entity/Q110962934', 'http://www.wikidata.org/entity/Q111149458', 'http://www.wikidata.org/entity/Q111202983', 'http://www.wikidata.org/entity/Q111333928', 'http://www.wikidata.org/entity/Q111574867', 'http://www.wikidata.org/entity/Q111605537', 'http://www.wikidata.org/entity/Q111649462', 'http://www.wikidata.org/entity/Q111649876', 'http://www.wikidata.org/entity/Q111655654', 'http://www.wikidata.org/entity/Q111711222', 'http://www.wikidata.org/entity/Q111732603', 'http://www.wikidata.org/entity/Q111811564', 'http://www.wikidata.org/entity/Q111846538', 'http://www.wikidata.org/entity/Q111914764', 'http://www.wikidata.org/entity/Q112055', 'http://www.wikidata.org/entity/Q112059989', 'http://www.wikidata.org/entity/Q112075710', 'http://www.wikidata.org/entity/Q11219195', 'http://www.wikidata.org/entity/Q112292803', 'http://www.wikidata.org/entity/Q11237670', 'http://www.wikidata.org/entity/Q11244589', 'http://www.wikidata.org/entity/Q112613424', 'http://www.wikidata.org/entity/Q11269', 'http://www.wikidata.org/entity/Q112748137', 'http://www.wikidata.org/entity/Q11277431', 'http://www.wikidata.org/entity/Q112971391', 'http://www.wikidata.org/entity/Q112971396', 'http://www.wikidata.org/entity/Q112971410', 'http://www.wikidata.org/entity/Q112971413', 'http://www.wikidata.org/entity/Q113040064', 'http://www.wikidata.org/entity/Q113114857', 'http://www.wikidata.org/entity/Q113232600', 'http://www.wikidata.org/entity/Q113383597', 'http://www.wikidata.org/entity/Q113470219', 'http://www.wikidata.org/entity/Q113470532', 'http://www.wikidata.org/entity/Q113485231', 'http://www.wikidata.org/entity/Q113499420', 'http://www.wikidata.org/entity/Q113499458', 'http://www.wikidata.org/entity/Q1135034', 'http://www.wikidata.org/entity/Q11354348', 'http://www.wikidata.org/entity/Q113549137', 'http://www.wikidata.org/entity/Q113576165', 'http://www.wikidata.org/entity/Q113581609', 'http://www.wikidata.org/entity/Q113627236', 'http://www.wikidata.org/entity/Q113631347', 'http://www.wikidata.org/entity/Q113631375', 'http://www.wikidata.org/entity/Q113631508', 'http://www.wikidata.org/entity/Q113631563', 'http://www.wikidata.org/entity/Q113631569', 'http://www.wikidata.org/entity/Q113674106', 'http://www.wikidata.org/entity/Q11371391', 'http://www.wikidata.org/entity/Q113714633', 'http://www.wikidata.org/entity/Q11387117', 'http://www.wikidata.org/entity/Q113903854', 'http://www.wikidata.org/entity/Q11391277', 'http://www.wikidata.org/entity/Q1139591', 'http://www.wikidata.org/entity/Q11409712', 'http://www.wikidata.org/entity/Q114315605', 'http://www.wikidata.org/entity/Q114658295', 'http://www.wikidata.org/entity/Q1147008', 'http://www.wikidata.org/entity/Q114779611', 'http://www.wikidata.org/entity/Q114780741', 'http://www.wikidata.org/entity/Q114781351', 'http://www.wikidata.org/entity/Q114840373', 'http://www.wikidata.org/entity/Q114863314', 'http://www.wikidata.org/entity/Q115152362', 'http://www.wikidata.org/entity/Q115209188', 'http://www.wikidata.org/entity/Q115214299', 'http://www.wikidata.org/entity/Q115259173', 'http://www.wikidata.org/entity/Q115294651', 'http://www.wikidata.org/entity/Q115327380', 'http://www.wikidata.org/entity/Q1153848', 'http://www.wikidata.org/entity/Q11545488', 'http://www.wikidata.org/entity/Q115516436', 'http://www.wikidata.org/entity/Q115526578', 'http://www.wikidata.org/entity/Q115624997', 'http://www.wikidata.org/entity/Q115628690', 'http://www.wikidata.org/entity/Q11567159', 'http://www.wikidata.org/entity/Q11590237', 'http://www.wikidata.org/entity/Q115937074', 'http://www.wikidata.org/entity/Q11606287', 'http://www.wikidata.org/entity/Q116113833', 'http://www.wikidata.org/entity/Q116349234', 'http://www.wikidata.org/entity/Q116767714', 'http://www.wikidata.org/entity/Q116790237', 'http://www.wikidata.org/entity/Q116846825', 'http://www.wikidata.org/entity/Q116858640', 'http://www.wikidata.org/entity/Q116938985', 'http://www.wikidata.org/entity/Q11695705', 'http://www.wikidata.org/entity/Q11695707', 'http://www.wikidata.org/entity/Q11695708', 'http://www.wikidata.org/entity/Q11695711', 'http://www.wikidata.org/entity/Q11695713', 'http://www.wikidata.org/entity/Q11695714', 'http://www.wikidata.org/entity/Q11695716', 'http://www.wikidata.org/entity/Q11695717', 'http://www.wikidata.org/entity/Q11695718', 'http://www.wikidata.org/entity/Q11695721', 'http://www.wikidata.org/entity/Q11695722', 'http://www.wikidata.org/entity/Q11695723', 'http://www.wikidata.org/entity/Q116973585', 'http://www.wikidata.org/entity/Q116980492', 'http://www.wikidata.org/entity/Q117035968', 'http://www.wikidata.org/entity/Q11703716', 'http://www.wikidata.org/entity/Q117040282', 'http://www.wikidata.org/entity/Q11706236', 'http://www.wikidata.org/entity/Q1170632', 'http://www.wikidata.org/entity/Q117361394', 'http://www.wikidata.org/entity/Q117421915', 'http://www.wikidata.org/entity/Q117455751', 'http://www.wikidata.org/entity/Q117587270', 'http://www.wikidata.org/entity/Q117711867', 'http://www.wikidata.org/entity/Q11783773', 'http://www.wikidata.org/entity/Q11783808', 'http://www.wikidata.org/entity/Q117844480', 'http://www.wikidata.org/entity/Q11789695', 'http://www.wikidata.org/entity/Q11789705', 'http://www.wikidata.org/entity/Q11789707', 'http://www.wikidata.org/entity/Q11802972', 'http://www.wikidata.org/entity/Q118224784', 'http://www.wikidata.org/entity/Q118288532', 'http://www.wikidata.org/entity/Q118314773', 'http://www.wikidata.org/entity/Q118330188', 'http://www.wikidata.org/entity/Q118369207', 'http://www.wikidata.org/entity/Q118744251', 'http://www.wikidata.org/entity/Q118842681', 'http://www.wikidata.org/entity/Q118849459', 'http://www.wikidata.org/entity/Q118947258', 'http://www.wikidata.org/entity/Q119105010', 'http://www.wikidata.org/entity/Q11919090', 'http://www.wikidata.org/entity/Q119241124', 'http://www.wikidata.org/entity/Q119243817', 'http://www.wikidata.org/entity/Q119285617', 'http://www.wikidata.org/entity/Q119348301', 'http://www.wikidata.org/entity/Q119397277', 'http://www.wikidata.org/entity/Q1194059', 'http://www.wikidata.org/entity/Q11977920', 'http://www.wikidata.org/entity/Q119806244', 'http://www.wikidata.org/entity/Q119853995', 'http://www.wikidata.org/entity/Q120068971', 'http://www.wikidata.org/entity/Q120146391', 'http://www.wikidata.org/entity/Q120403912', 'http://www.wikidata.org/entity/Q120486552', 'http://www.wikidata.org/entity/Q12060958', 'http://www.wikidata.org/entity/Q120823815', 'http://www.wikidata.org/entity/Q120837533', 'http://www.wikidata.org/entity/Q12090941', 'http://www.wikidata.org/entity/Q1209940', 'http://www.wikidata.org/entity/Q12100125', 'http://www.wikidata.org/entity/Q12100126', 'http://www.wikidata.org/entity/Q12100128', 'http://www.wikidata.org/entity/Q12100132', 'http://www.wikidata.org/entity/Q12100138', 'http://www.wikidata.org/entity/Q12100141', 'http://www.wikidata.org/entity/Q12100152', 'http://www.wikidata.org/entity/Q12100160', 'http://www.wikidata.org/entity/Q12131090', 'http://www.wikidata.org/entity/Q121322780', 'http://www.wikidata.org/entity/Q121393', 'http://www.wikidata.org/entity/Q12149731', 'http://www.wikidata.org/entity/Q12174361', 'http://www.wikidata.org/entity/Q121759535', 'http://www.wikidata.org/entity/Q121852183', 'http://www.wikidata.org/entity/Q121864546', 'http://www.wikidata.org/entity/Q121991381', 'http://www.wikidata.org/entity/Q122057715', 'http://www.wikidata.org/entity/Q122058042', 'http://www.wikidata.org/entity/Q122144115', 'http://www.wikidata.org/entity/Q122199376', 'http://www.wikidata.org/entity/Q122341064', 'http://www.wikidata.org/entity/Q122460010', 'http://www.wikidata.org/entity/Q122495885', 'http://www.wikidata.org/entity/Q1226845', 'http://www.wikidata.org/entity/Q122767100', 'http://www.wikidata.org/entity/Q12284238', 'http://www.wikidata.org/entity/Q12286265', 'http://www.wikidata.org/entity/Q12286390', 'http://www.wikidata.org/entity/Q12289674', 'http://www.wikidata.org/entity/Q12292151', 'http://www.wikidata.org/entity/Q12293119', 'http://www.wikidata.org/entity/Q12293243', 'http://www.wikidata.org/entity/Q12299913', 'http://www.wikidata.org/entity/Q123111964', 'http://www.wikidata.org/entity/Q1231872', 'http://www.wikidata.org/entity/Q123253535', 'http://www.wikidata.org/entity/Q123265528', 'http://www.wikidata.org/entity/Q123450314', 'http://www.wikidata.org/entity/Q123515600', 'http://www.wikidata.org/entity/Q12353618', 'http://www.wikidata.org/entity/Q123746478', 'http://www.wikidata.org/entity/Q123757853', 'http://www.wikidata.org/entity/Q1239437', 'http://www.wikidata.org/entity/Q12407917', 'http://www.wikidata.org/entity/Q12407923', 'http://www.wikidata.org/entity/Q1241858', 'http://www.wikidata.org/entity/Q12422844', 'http://www.wikidata.org/entity/Q124250314', 'http://www.wikidata.org/entity/Q124250951', 'http://www.wikidata.org/entity/Q124255532', 'http://www.wikidata.org/entity/Q124318023', 'http://www.wikidata.org/entity/Q124352953', 'http://www.wikidata.org/entity/Q124367000', 'http://www.wikidata.org/entity/Q12438967', 'http://www.wikidata.org/entity/Q124408550', 'http://www.wikidata.org/entity/Q12441237', 'http://www.wikidata.org/entity/Q124498473', 'http://www.wikidata.org/entity/Q124498859', 'http://www.wikidata.org/entity/Q124568688', 'http://www.wikidata.org/entity/Q124747000', 'http://www.wikidata.org/entity/Q124799998', 'http://www.wikidata.org/entity/Q124830290', 'http://www.wikidata.org/entity/Q124854084', 'http://www.wikidata.org/entity/Q12513670', 'http://www.wikidata.org/entity/Q12525597', 'http://www.wikidata.org/entity/Q1252585', 'http://www.wikidata.org/entity/Q1252596', 'http://www.wikidata.org/entity/Q125505711', 'http://www.wikidata.org/entity/Q1255099', 'http://www.wikidata.org/entity/Q125524227', 'http://www.wikidata.org/entity/Q125613295', 'http://www.wikidata.org/entity/Q125912847', 'http://www.wikidata.org/entity/Q125928736', 'http://www.wikidata.org/entity/Q12601109', 'http://www.wikidata.org/entity/Q12602481', 'http://www.wikidata.org/entity/Q126083299', 'http://www.wikidata.org/entity/Q126083373', 'http://www.wikidata.org/entity/Q126113071', 'http://www.wikidata.org/entity/Q12614307', 'http://www.wikidata.org/entity/Q12614875', 'http://www.wikidata.org/entity/Q126192995', 'http://www.wikidata.org/entity/Q126260200', 'http://www.wikidata.org/entity/Q12650252', 'http://www.wikidata.org/entity/Q12663498', 'http://www.wikidata.org/entity/Q126708915', 'http://www.wikidata.org/entity/Q126902823', 'http://www.wikidata.org/entity/Q126903060', 'http://www.wikidata.org/entity/Q126910647', 'http://www.wikidata.org/entity/Q126948133', 'http://www.wikidata.org/entity/Q126949840', 'http://www.wikidata.org/entity/Q1270782', 'http://www.wikidata.org/entity/Q12713841', 'http://www.wikidata.org/entity/Q12716026', 'http://www.wikidata.org/entity/Q12719109', 'http://www.wikidata.org/entity/Q127393146', 'http://www.wikidata.org/entity/Q127502506', 'http://www.wikidata.org/entity/Q12750635', 'http://www.wikidata.org/entity/Q127597840', 'http://www.wikidata.org/entity/Q127798249', 'http://www.wikidata.org/entity/Q12787253', 'http://www.wikidata.org/entity/Q12787255', 'http://www.wikidata.org/entity/Q127922454', 'http://www.wikidata.org/entity/Q12803843', 'http://www.wikidata.org/entity/Q12836659', 'http://www.wikidata.org/entity/Q12859165', 'http://www.wikidata.org/entity/Q12864158', 'http://www.wikidata.org/entity/Q1290276', 'http://www.wikidata.org/entity/Q12927731', 'http://www.wikidata.org/entity/Q129726', 'http://www.wikidata.org/entity/Q12986877', 'http://www.wikidata.org/entity/Q129876847', 'http://www.wikidata.org/entity/Q129876849', 'http://www.wikidata.org/entity/Q129876851', 'http://www.wikidata.org/entity/Q129876853', 'http://www.wikidata.org/entity/Q129876855', 'http://www.wikidata.org/entity/Q129876857', 'http://www.wikidata.org/entity/Q12989464', 'http://www.wikidata.org/entity/Q13020973', 'http://www.wikidata.org/entity/Q130215597', 'http://www.wikidata.org/entity/Q130237269', 'http://www.wikidata.org/entity/Q130237270', 'http://www.wikidata.org/entity/Q130237271', 'http://www.wikidata.org/entity/Q130237272', 'http://www.wikidata.org/entity/Q130237273', 'http://www.wikidata.org/entity/Q130237274', 'http://www.wikidata.org/entity/Q130237276', 'http://www.wikidata.org/entity/Q130237277', 'http://www.wikidata.org/entity/Q130237278', 'http://www.wikidata.org/entity/Q130237279', 'http://www.wikidata.org/entity/Q130237280', 'http://www.wikidata.org/entity/Q130237281', 'http://www.wikidata.org/entity/Q130237282', 'http://www.wikidata.org/entity/Q130237283', 'http://www.wikidata.org/entity/Q130237284', 'http://www.wikidata.org/entity/Q130237285', 'http://www.wikidata.org/entity/Q130237286', 'http://www.wikidata.org/entity/Q130237287', 'http://www.wikidata.org/entity/Q130237288', 'http://www.wikidata.org/entity/Q130237289', 'http://www.wikidata.org/entity/Q130237290', 'http://www.wikidata.org/entity/Q130237291', 'http://www.wikidata.org/entity/Q130237292', 'http://www.wikidata.org/entity/Q130237293', 'http://www.wikidata.org/entity/Q130237294', 'http://www.wikidata.org/entity/Q130237295', 'http://www.wikidata.org/entity/Q130237296', 'http://www.wikidata.org/entity/Q130237297', 'http://www.wikidata.org/entity/Q130237298', 'http://www.wikidata.org/entity/Q130237299', 'http://www.wikidata.org/entity/Q130237300', 'http://www.wikidata.org/entity/Q130237301', 'http://www.wikidata.org/entity/Q130237302', 'http://www.wikidata.org/entity/Q130237303', 'http://www.wikidata.org/entity/Q130237304', 'http://www.wikidata.org/entity/Q130237305', 'http://www.wikidata.org/entity/Q130237306', 'http://www.wikidata.org/entity/Q130237307', 'http://www.wikidata.org/entity/Q130237308', 'http://www.wikidata.org/entity/Q130237309', 'http://www.wikidata.org/entity/Q130237310', 'http://www.wikidata.org/entity/Q130237311', 'http://www.wikidata.org/entity/Q130237312', 'http://www.wikidata.org/entity/Q130237314', 'http://www.wikidata.org/entity/Q130237315', 'http://www.wikidata.org/entity/Q130237316', 'http://www.wikidata.org/entity/Q130237317', 'http://www.wikidata.org/entity/Q130237318', 'http://www.wikidata.org/entity/Q130237319', 'http://www.wikidata.org/entity/Q130237320', 'http://www.wikidata.org/entity/Q130237321', 'http://www.wikidata.org/entity/Q130237322', 'http://www.wikidata.org/entity/Q130237323', 'http://www.wikidata.org/entity/Q130237324', 'http://www.wikidata.org/entity/Q130237325', 'http://www.wikidata.org/entity/Q130237326', 'http://www.wikidata.org/entity/Q130237327', 'http://www.wikidata.org/entity/Q130237328', 'http://www.wikidata.org/entity/Q130237329', 'http://www.wikidata.org/entity/Q130237330', 'http://www.wikidata.org/entity/Q130237331', 'http://www.wikidata.org/entity/Q130237332', 'http://www.wikidata.org/entity/Q130237333', 'http://www.wikidata.org/entity/Q130237334', 'http://www.wikidata.org/entity/Q130237335', 'http://www.wikidata.org/entity/Q130237336', 'http://www.wikidata.org/entity/Q130237337', 'http://www.wikidata.org/entity/Q130237338', 'http://www.wikidata.org/entity/Q130237339', 'http://www.wikidata.org/entity/Q130237340', 'http://www.wikidata.org/entity/Q130237341', 'http://www.wikidata.org/entity/Q130237342', 'http://www.wikidata.org/entity/Q130237343', 'http://www.wikidata.org/entity/Q130237344', 'http://www.wikidata.org/entity/Q130237345', 'http://www.wikidata.org/entity/Q130237346', 'http://www.wikidata.org/entity/Q130237347', 'http://www.wikidata.org/entity/Q130237348', 'http://www.wikidata.org/entity/Q130237349', 'http://www.wikidata.org/entity/Q130237350', 'http://www.wikidata.org/entity/Q130237351', 'http://www.wikidata.org/entity/Q130237353', 'http://www.wikidata.org/entity/Q130237354', 'http://www.wikidata.org/entity/Q130237355', 'http://www.wikidata.org/entity/Q130237356', 'http://www.wikidata.org/entity/Q130237357', 'http://www.wikidata.org/entity/Q130237358', 'http://www.wikidata.org/entity/Q130237359', 'http://www.wikidata.org/entity/Q130237360', 'http://www.wikidata.org/entity/Q130237361', 'http://www.wikidata.org/entity/Q130237362', 'http://www.wikidata.org/entity/Q130237363', 'http://www.wikidata.org/entity/Q130237364', 'http://www.wikidata.org/entity/Q130237365', 'http://www.wikidata.org/entity/Q130237366', 'http://www.wikidata.org/entity/Q130237367', 'http://www.wikidata.org/entity/Q130237368', 'http://www.wikidata.org/entity/Q130237369', 'http://www.wikidata.org/entity/Q130237370', 'http://www.wikidata.org/entity/Q130237371', 'http://www.wikidata.org/entity/Q130237372', 'http://www.wikidata.org/entity/Q130237373', 'http://www.wikidata.org/entity/Q130237374', 'http://www.wikidata.org/entity/Q130237375', 'http://www.wikidata.org/entity/Q130237376', 'http://www.wikidata.org/entity/Q130237377', 'http://www.wikidata.org/entity/Q130237378', 'http://www.wikidata.org/entity/Q130237379', 'http://www.wikidata.org/entity/Q130237380', 'http://www.wikidata.org/entity/Q130237381', 'http://www.wikidata.org/entity/Q130237382', 'http://www.wikidata.org/entity/Q130237383', 'http://www.wikidata.org/entity/Q130237384', 'http://www.wikidata.org/entity/Q130237385', 'http://www.wikidata.org/entity/Q130237386', 'http://www.wikidata.org/entity/Q130237387', 'http://www.wikidata.org/entity/Q130237388', 'http://www.wikidata.org/entity/Q130237389', 'http://www.wikidata.org/entity/Q130237390', 'http://www.wikidata.org/entity/Q130237391', 'http://www.wikidata.org/entity/Q130237392', 'http://www.wikidata.org/entity/Q130237393', 'http://www.wikidata.org/entity/Q130237394', 'http://www.wikidata.org/entity/Q130237395', 'http://www.wikidata.org/entity/Q130237396', 'http://www.wikidata.org/entity/Q130237397', 'http://www.wikidata.org/entity/Q130237398', 'http://www.wikidata.org/entity/Q130237399', 'http://www.wikidata.org/entity/Q130237400', 'http://www.wikidata.org/entity/Q130237402', 'http://www.wikidata.org/entity/Q130237403', 'http://www.wikidata.org/entity/Q130237404', 'http://www.wikidata.org/entity/Q130237405', 'http://www.wikidata.org/entity/Q130237406', 'http://www.wikidata.org/entity/Q130237407', 'http://www.wikidata.org/entity/Q130237408', 'http://www.wikidata.org/entity/Q130237409', 'http://www.wikidata.org/entity/Q130237410', 'http://www.wikidata.org/entity/Q130237411', 'http://www.wikidata.org/entity/Q130237412', 'http://www.wikidata.org/entity/Q130237413', 'http://www.wikidata.org/entity/Q130237414', 'http://www.wikidata.org/entity/Q130237415', 'http://www.wikidata.org/entity/Q130237416', 'http://www.wikidata.org/entity/Q130237417', 'http://www.wikidata.org/entity/Q130237419', 'http://www.wikidata.org/entity/Q130237420', 'http://www.wikidata.org/entity/Q130237421', 'http://www.wikidata.org/entity/Q130237422', 'http://www.wikidata.org/entity/Q130237423', 'http://www.wikidata.org/entity/Q130237424', 'http://www.wikidata.org/entity/Q130237425', 'http://www.wikidata.org/entity/Q130237426', 'http://www.wikidata.org/entity/Q130237427', 'http://www.wikidata.org/entity/Q130237428', 'http://www.wikidata.org/entity/Q130237429', 'http://www.wikidata.org/entity/Q130237430', 'http://www.wikidata.org/entity/Q130237431', 'http://www.wikidata.org/entity/Q130237432', 'http://www.wikidata.org/entity/Q130237433', 'http://www.wikidata.org/entity/Q130237434', 'http://www.wikidata.org/entity/Q130237435', 'http://www.wikidata.org/entity/Q130237436', 'http://www.wikidata.org/entity/Q130237437', 'http://www.wikidata.org/entity/Q130237438', 'http://www.wikidata.org/entity/Q130237439', 'http://www.wikidata.org/entity/Q130237440', 'http://www.wikidata.org/entity/Q130237441', 'http://www.wikidata.org/entity/Q130237442', 'http://www.wikidata.org/entity/Q130237443', 'http://www.wikidata.org/entity/Q130237444', 'http://www.wikidata.org/entity/Q130237445', 'http://www.wikidata.org/entity/Q130237446', 'http://www.wikidata.org/entity/Q130237447', 'http://www.wikidata.org/entity/Q130237448', 'http://www.wikidata.org/entity/Q130237449', 'http://www.wikidata.org/entity/Q130237450', 'http://www.wikidata.org/entity/Q130237451', 'http://www.wikidata.org/entity/Q130237452', 'http://www.wikidata.org/entity/Q130237453', 'http://www.wikidata.org/entity/Q130237454', 'http://www.wikidata.org/entity/Q130237455', 'http://www.wikidata.org/entity/Q130237456', 'http://www.wikidata.org/entity/Q130237457', 'http://www.wikidata.org/entity/Q130237458', 'http://www.wikidata.org/entity/Q130237459', 'http://www.wikidata.org/entity/Q130237460', 'http://www.wikidata.org/entity/Q130237461', 'http://www.wikidata.org/entity/Q130237462', 'http://www.wikidata.org/entity/Q130237463', 'http://www.wikidata.org/entity/Q130237464', 'http://www.wikidata.org/entity/Q130237465', 'http://www.wikidata.org/entity/Q130237466', 'http://www.wikidata.org/entity/Q130237467', 'http://www.wikidata.org/entity/Q130237468', 'http://www.wikidata.org/entity/Q130237469', 'http://www.wikidata.org/entity/Q130237471', 'http://www.wikidata.org/entity/Q130237472', 'http://www.wikidata.org/entity/Q130237473', 'http://www.wikidata.org/entity/Q130237474', 'http://www.wikidata.org/entity/Q130237475', 'http://www.wikidata.org/entity/Q130237476', 'http://www.wikidata.org/entity/Q130237477', 'http://www.wikidata.org/entity/Q130237478', 'http://www.wikidata.org/entity/Q130237479', 'http://www.wikidata.org/entity/Q130237480', 'http://www.wikidata.org/entity/Q130237481', 'http://www.wikidata.org/entity/Q130237482', 'http://www.wikidata.org/entity/Q130237484', 'http://www.wikidata.org/entity/Q130237485', 'http://www.wikidata.org/entity/Q130237487', 'http://www.wikidata.org/entity/Q130237488', 'http://www.wikidata.org/entity/Q130237489', 'http://www.wikidata.org/entity/Q130237490', 'http://www.wikidata.org/entity/Q130237491', 'http://www.wikidata.org/entity/Q130237492', 'http://www.wikidata.org/entity/Q130237493', 'http://www.wikidata.org/entity/Q130237494', 'http://www.wikidata.org/entity/Q130237495', 'http://www.wikidata.org/entity/Q130237496', 'http://www.wikidata.org/entity/Q130237497', 'http://www.wikidata.org/entity/Q130237498', 'http://www.wikidata.org/entity/Q130237499', 'http://www.wikidata.org/entity/Q130237500', 'http://www.wikidata.org/entity/Q130237501', 'http://www.wikidata.org/entity/Q130237502', 'http://www.wikidata.org/entity/Q130237503', 'http://www.wikidata.org/entity/Q130237504', 'http://www.wikidata.org/entity/Q130237505', 'http://www.wikidata.org/entity/Q130237506', 'http://www.wikidata.org/entity/Q130237507', 'http://www.wikidata.org/entity/Q130237508', 'http://www.wikidata.org/entity/Q130237509', 'http://www.wikidata.org/entity/Q130237510', 'http://www.wikidata.org/entity/Q130237511', 'http://www.wikidata.org/entity/Q130237513', 'http://www.wikidata.org/entity/Q130237514', 'http://www.wikidata.org/entity/Q130237515', 'http://www.wikidata.org/entity/Q130237516', 'http://www.wikidata.org/entity/Q130237517', 'http://www.wikidata.org/entity/Q130237518', 'http://www.wikidata.org/entity/Q130237520', 'http://www.wikidata.org/entity/Q130237521', 'http://www.wikidata.org/entity/Q130237522', 'http://www.wikidata.org/entity/Q130237524', 'http://www.wikidata.org/entity/Q130237525', 'http://www.wikidata.org/entity/Q130237526', 'http://www.wikidata.org/entity/Q130237527', 'http://www.wikidata.org/entity/Q130237529', 'http://www.wikidata.org/entity/Q130237530', 'http://www.wikidata.org/entity/Q130237531', 'http://www.wikidata.org/entity/Q130237532', 'http://www.wikidata.org/entity/Q130237534', 'http://www.wikidata.org/entity/Q130237535', 'http://www.wikidata.org/entity/Q130237536', 'http://www.wikidata.org/entity/Q130237537', 'http://www.wikidata.org/entity/Q130237538', 'http://www.wikidata.org/entity/Q130237539', 'http://www.wikidata.org/entity/Q130237540', 'http://www.wikidata.org/entity/Q130237541', 'http://www.wikidata.org/entity/Q130237542', 'http://www.wikidata.org/entity/Q130237543', 'http://www.wikidata.org/entity/Q130237544', 'http://www.wikidata.org/entity/Q130237545', 'http://www.wikidata.org/entity/Q130237546', 'http://www.wikidata.org/entity/Q130237547', 'http://www.wikidata.org/entity/Q130237548', 'http://www.wikidata.org/entity/Q130237549', 'http://www.wikidata.org/entity/Q130237550', 'http://www.wikidata.org/entity/Q130237552', 'http://www.wikidata.org/entity/Q130237553', 'http://www.wikidata.org/entity/Q130237554', 'http://www.wikidata.org/entity/Q130237555', 'http://www.wikidata.org/entity/Q130237556', 'http://www.wikidata.org/entity/Q130237557', 'http://www.wikidata.org/entity/Q130237558', 'http://www.wikidata.org/entity/Q130237559', 'http://www.wikidata.org/entity/Q130237560', 'http://www.wikidata.org/entity/Q130237561', 'http://www.wikidata.org/entity/Q130237562', 'http://www.wikidata.org/entity/Q130237563', 'http://www.wikidata.org/entity/Q130237564', 'http://www.wikidata.org/entity/Q130237565', 'http://www.wikidata.org/entity/Q130237566', 'http://www.wikidata.org/entity/Q130237567', 'http://www.wikidata.org/entity/Q130237570', 'http://www.wikidata.org/entity/Q130237571', 'http://www.wikidata.org/entity/Q130237572', 'http://www.wikidata.org/entity/Q130237573', 'http://www.wikidata.org/entity/Q130237574', 'http://www.wikidata.org/entity/Q130237575', 'http://www.wikidata.org/entity/Q130237576', 'http://www.wikidata.org/entity/Q130237577', 'http://www.wikidata.org/entity/Q130237578', 'http://www.wikidata.org/entity/Q130237579', 'http://www.wikidata.org/entity/Q130237581', 'http://www.wikidata.org/entity/Q130237582', 'http://www.wikidata.org/entity/Q130237584', 'http://www.wikidata.org/entity/Q130237585', 'http://www.wikidata.org/entity/Q130237587', 'http://www.wikidata.org/entity/Q130237588', 'http://www.wikidata.org/entity/Q130237589', 'http://www.wikidata.org/entity/Q130237591', 'http://www.wikidata.org/entity/Q130237592', 'http://www.wikidata.org/entity/Q130237593', 'http://www.wikidata.org/entity/Q130237594', 'http://www.wikidata.org/entity/Q130237597', 'http://www.wikidata.org/entity/Q130237598', 'http://www.wikidata.org/entity/Q130237599', 'http://www.wikidata.org/entity/Q130237601', 'http://www.wikidata.org/entity/Q130237602', 'http://www.wikidata.org/entity/Q130237603', 'http://www.wikidata.org/entity/Q130237604', 'http://www.wikidata.org/entity/Q130237605', 'http://www.wikidata.org/entity/Q130237607', 'http://www.wikidata.org/entity/Q130237608', 'http://www.wikidata.org/entity/Q130237609', 'http://www.wikidata.org/entity/Q130237611', 'http://www.wikidata.org/entity/Q130237612', 'http://www.wikidata.org/entity/Q130237613', 'http://www.wikidata.org/entity/Q130237615', 'http://www.wikidata.org/entity/Q130237616', 'http://www.wikidata.org/entity/Q130237617', 'http://www.wikidata.org/entity/Q130237618', 'http://www.wikidata.org/entity/Q130237619', 'http://www.wikidata.org/entity/Q130237620', 'http://www.wikidata.org/entity/Q130237621', 'http://www.wikidata.org/entity/Q130237623', 'http://www.wikidata.org/entity/Q130237624', 'http://www.wikidata.org/entity/Q130237625', 'http://www.wikidata.org/entity/Q130237626', 'http://www.wikidata.org/entity/Q130237627', 'http://www.wikidata.org/entity/Q130237628', 'http://www.wikidata.org/entity/Q130237629', 'http://www.wikidata.org/entity/Q130237630', 'http://www.wikidata.org</t>
+          <t>['1735-10-30T00:00:00Z']</t>
         </is>
       </c>
       <c r="D11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Give me the birthdays of all actors of the television show Charmed.</t>
+          <t>how much is the total population of european union?</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>['1971-04-12T00:00:00Z', '1972-12-19T00:00:00Z', '1973-09-05T00:00:00Z', '1973-12-03T00:00:00Z']</t>
+          <t>['447706209']</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>['1971-04-12T00:00:00Z', '1972-12-19T00:00:00Z', '1973-09-05T00:00:00Z', '1973-12-03T00:00:00Z']</t>
+          <t>['447706209']</t>
         </is>
       </c>
       <c r="D12" t="b">
@@ -678,17 +678,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Who designed the Brooklyn Bridge?</t>
+          <t>Give me the currency of China.</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q77237']</t>
+          <t>['http://www.wikidata.org/entity/Q39099']</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q77237']</t>
+          <t>['http://www.wikidata.org/entity/Q39099']</t>
         </is>
       </c>
       <c r="D13" t="b">
@@ -698,37 +698,37 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Who wrote the Game of Thrones theme?</t>
+          <t>When was the death of Shakespeare?</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q57577']</t>
+          <t>['1616-05-03T00:00:00Z']</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q57577']</t>
+          <t>['http://www.wikidata.org/entity/statement/Q692-d9ff2687-4821-c33f-3134-1ea816d00b24']</t>
         </is>
       </c>
       <c r="D14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>What is the birth name of Adele?</t>
+          <t>Give me all islands that belong to Japan.</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>['Adele Laurie Blue Adkins']</t>
+          <t xml:space="preserve">['http://www.wikidata.org/entity/Q100695440', 'http://www.wikidata.org/entity/Q1019313', 'http://www.wikidata.org/entity/Q102245375', 'http://www.wikidata.org/entity/Q1039445', 'http://www.wikidata.org/entity/Q104186080', 'http://www.wikidata.org/entity/Q10449219', 'http://www.wikidata.org/entity/Q1047492', 'http://www.wikidata.org/entity/Q1061394', 'http://www.wikidata.org/entity/Q106150403', 'http://www.wikidata.org/entity/Q106363078', 'http://www.wikidata.org/entity/Q1072125', 'http://www.wikidata.org/entity/Q1083890', 'http://www.wikidata.org/entity/Q10855760', 'http://www.wikidata.org/entity/Q10855761', 'http://www.wikidata.org/entity/Q10856210', 'http://www.wikidata.org/entity/Q10859834', 'http://www.wikidata.org/entity/Q10860535', 'http://www.wikidata.org/entity/Q10889854', 'http://www.wikidata.org/entity/Q109368351', 'http://www.wikidata.org/entity/Q10938711', 'http://www.wikidata.org/entity/Q109405713', 'http://www.wikidata.org/entity/Q10943140', 'http://www.wikidata.org/entity/Q109673419', 'http://www.wikidata.org/entity/Q1111504', 'http://www.wikidata.org/entity/Q112224546', 'http://www.wikidata.org/entity/Q11234719', 'http://www.wikidata.org/entity/Q11241368', 'http://www.wikidata.org/entity/Q11261668', 'http://www.wikidata.org/entity/Q112673064', 'http://www.wikidata.org/entity/Q11276631', 'http://www.wikidata.org/entity/Q11285385', 'http://www.wikidata.org/entity/Q11286923', 'http://www.wikidata.org/entity/Q11353972', 'http://www.wikidata.org/entity/Q11354008', 'http://www.wikidata.org/entity/Q11356195', 'http://www.wikidata.org/entity/Q11357220', 'http://www.wikidata.org/entity/Q11358913', 'http://www.wikidata.org/entity/Q11360086', 'http://www.wikidata.org/entity/Q11360847', 'http://www.wikidata.org/entity/Q11361905', 'http://www.wikidata.org/entity/Q11362796', 'http://www.wikidata.org/entity/Q11362797', 'http://www.wikidata.org/entity/Q11362799', 'http://www.wikidata.org/entity/Q11369263', 'http://www.wikidata.org/entity/Q11369927', 'http://www.wikidata.org/entity/Q11370029', 'http://www.wikidata.org/entity/Q11370104', 'http://www.wikidata.org/entity/Q11371742', 'http://www.wikidata.org/entity/Q11373491', 'http://www.wikidata.org/entity/Q11376329', 'http://www.wikidata.org/entity/Q11377524', 'http://www.wikidata.org/entity/Q11378204', 'http://www.wikidata.org/entity/Q11379228', 'http://www.wikidata.org/entity/Q11379335', 'http://www.wikidata.org/entity/Q11382608', 'http://www.wikidata.org/entity/Q11383201', 'http://www.wikidata.org/entity/Q11383217', 'http://www.wikidata.org/entity/Q11385812', 'http://www.wikidata.org/entity/Q11386818', 'http://www.wikidata.org/entity/Q11390867', 'http://www.wikidata.org/entity/Q11390868', 'http://www.wikidata.org/entity/Q11392330', 'http://www.wikidata.org/entity/Q11394726', 'http://www.wikidata.org/entity/Q11395612', 'http://www.wikidata.org/entity/Q11395786', 'http://www.wikidata.org/entity/Q11397118', 'http://www.wikidata.org/entity/Q11398556', 'http://www.wikidata.org/entity/Q11399769', 'http://www.wikidata.org/entity/Q11401908', 'http://www.wikidata.org/entity/Q11402215', 'http://www.wikidata.org/entity/Q11402223', 'http://www.wikidata.org/entity/Q11407776', 'http://www.wikidata.org/entity/Q11409587', 'http://www.wikidata.org/entity/Q11410659', 'http://www.wikidata.org/entity/Q11415949', 'http://www.wikidata.org/entity/Q11415951', 'http://www.wikidata.org/entity/Q11415952', 'http://www.wikidata.org/entity/Q11415953', 'http://www.wikidata.org/entity/Q11416626', 'http://www.wikidata.org/entity/Q11418533', 'http://www.wikidata.org/entity/Q11419386', 'http://www.wikidata.org/entity/Q11419637', 'http://www.wikidata.org/entity/Q11420237', 'http://www.wikidata.org/entity/Q11424450', 'http://www.wikidata.org/entity/Q11424752', 'http://www.wikidata.org/entity/Q11425641', 'http://www.wikidata.org/entity/Q11430798', 'http://www.wikidata.org/entity/Q11431830', 'http://www.wikidata.org/entity/Q11432478', 'http://www.wikidata.org/entity/Q11434172', 'http://www.wikidata.org/entity/Q11434804', 'http://www.wikidata.org/entity/Q11434805', 'http://www.wikidata.org/entity/Q11434806', 'http://www.wikidata.org/entity/Q11434807', 'http://www.wikidata.org/entity/Q11434809', 'http://www.wikidata.org/entity/Q11434813', 'http://www.wikidata.org/entity/Q11434815', 'http://www.wikidata.org/entity/Q11434816', 'http://www.wikidata.org/entity/Q11434819', 'http://www.wikidata.org/entity/Q11435005', 'http://www.wikidata.org/entity/Q11435006', 'http://www.wikidata.org/entity/Q11436454', 'http://www.wikidata.org/entity/Q11436765', 'http://www.wikidata.org/entity/Q11437275', 'http://www.wikidata.org/entity/Q11438136', 'http://www.wikidata.org/entity/Q11438379', 'http://www.wikidata.org/entity/Q11439590', 'http://www.wikidata.org/entity/Q11442082', 'http://www.wikidata.org/entity/Q11443237', 'http://www.wikidata.org/entity/Q11445536', 'http://www.wikidata.org/entity/Q11446412', 'http://www.wikidata.org/entity/Q11447403', 'http://www.wikidata.org/entity/Q11447404', 'http://www.wikidata.org/entity/Q11449014', 'http://www.wikidata.org/entity/Q11449464', 'http://www.wikidata.org/entity/Q11450585', 'http://www.wikidata.org/entity/Q11454772', 'http://www.wikidata.org/entity/Q11458850', 'http://www.wikidata.org/entity/Q11459344', 'http://www.wikidata.org/entity/Q11459579', 'http://www.wikidata.org/entity/Q11460065', 'http://www.wikidata.org/entity/Q11460438', 'http://www.wikidata.org/entity/Q11464517', 'http://www.wikidata.org/entity/Q11465691', 'http://www.wikidata.org/entity/Q11474307', 'http://www.wikidata.org/entity/Q11474346', 'http://www.wikidata.org/entity/Q11475712', 'http://www.wikidata.org/entity/Q11476827', 'http://www.wikidata.org/entity/Q11476897', 'http://www.wikidata.org/entity/Q11477129', 'http://www.wikidata.org/entity/Q11477305', 'http://www.wikidata.org/entity/Q11477410', 'http://www.wikidata.org/entity/Q11481155', 'http://www.wikidata.org/entity/Q11482668', 'http://www.wikidata.org/entity/Q11482669', 'http://www.wikidata.org/entity/Q11483492', 'http://www.wikidata.org/entity/Q11483589', 'http://www.wikidata.org/entity/Q11483827', 'http://www.wikidata.org/entity/Q11484404', 'http://www.wikidata.org/entity/Q11486132', 'http://www.wikidata.org/entity/Q11486908', 'http://www.wikidata.org/entity/Q11486909', 'http://www.wikidata.org/entity/Q11486910', 'http://www.wikidata.org/entity/Q11486911', 'http://www.wikidata.org/entity/Q11487067', 'http://www.wikidata.org/entity/Q11487395', 'http://www.wikidata.org/entity/Q11488768', 'http://www.wikidata.org/entity/Q11489067', 'http://www.wikidata.org/entity/Q11489240', 'http://www.wikidata.org/entity/Q11489251', 'http://www.wikidata.org/entity/Q11490807', 'http://www.wikidata.org/entity/Q11491460', 'http://www.wikidata.org/entity/Q11491674', 'http://www.wikidata.org/entity/Q11492404', 'http://www.wikidata.org/entity/Q11492410', 'http://www.wikidata.org/entity/Q11492883', 'http://www.wikidata.org/entity/Q11492884', 'http://www.wikidata.org/entity/Q11496323', 'http://www.wikidata.org/entity/Q11496324', 'http://www.wikidata.org/entity/Q11496670', 'http://www.wikidata.org/entity/Q11497087', 'http://www.wikidata.org/entity/Q11497519', 'http://www.wikidata.org/entity/Q11500406', 'http://www.wikidata.org/entity/Q11501924', 'http://www.wikidata.org/entity/Q11502024', 'http://www.wikidata.org/entity/Q11502876', 'http://www.wikidata.org/entity/Q11504920', 'http://www.wikidata.org/entity/Q11505281', 'http://www.wikidata.org/entity/Q11505343', 'http://www.wikidata.org/entity/Q11511249', 'http://www.wikidata.org/entity/Q11516644', 'http://www.wikidata.org/entity/Q11520216', 'http://www.wikidata.org/entity/Q11530091', 'http://www.wikidata.org/entity/Q11530093', 'http://www.wikidata.org/entity/Q11532746', 'http://www.wikidata.org/entity/Q11533729', 'http://www.wikidata.org/entity/Q11542683', 'http://www.wikidata.org/entity/Q11542685', 'http://www.wikidata.org/entity/Q11543672', 'http://www.wikidata.org/entity/Q11544654', 'http://www.wikidata.org/entity/Q11544655', 'http://www.wikidata.org/entity/Q11545996', 'http://www.wikidata.org/entity/Q11547731', 'http://www.wikidata.org/entity/Q11548193', 'http://www.wikidata.org/entity/Q11548462', 'http://www.wikidata.org/entity/Q11550173', 'http://www.wikidata.org/entity/Q11550842', 'http://www.wikidata.org/entity/Q11550845', 'http://www.wikidata.org/entity/Q11551591', 'http://www.wikidata.org/entity/Q11552439', 'http://www.wikidata.org/entity/Q11552466', 'http://www.wikidata.org/entity/Q11552477', 'http://www.wikidata.org/entity/Q11552498', 'http://www.wikidata.org/entity/Q11552502', 'http://www.wikidata.org/entity/Q11552549', 'http://www.wikidata.org/entity/Q11553027', 'http://www.wikidata.org/entity/Q11555929', 'http://www.wikidata.org/entity/Q11555966', 'http://www.wikidata.org/entity/Q11556058', 'http://www.wikidata.org/entity/Q11556221', 'http://www.wikidata.org/entity/Q11558501', 'http://www.wikidata.org/entity/Q11558503', 'http://www.wikidata.org/entity/Q11558824', 'http://www.wikidata.org/entity/Q11559068', 'http://www.wikidata.org/entity/Q11559418', 'http://www.wikidata.org/entity/Q11559763', 'http://www.wikidata.org/entity/Q11559986', 'http://www.wikidata.org/entity/Q11562837', 'http://www.wikidata.org/entity/Q11563518', 'http://www.wikidata.org/entity/Q11567224', 'http://www.wikidata.org/entity/Q11567245', 'http://www.wikidata.org/entity/Q11567267', 'http://www.wikidata.org/entity/Q11572200', 'http://www.wikidata.org/entity/Q11572311', 'http://www.wikidata.org/entity/Q11573306', 'http://www.wikidata.org/entity/Q11573823', 'http://www.wikidata.org/entity/Q11574179', 'http://www.wikidata.org/entity/Q11574434', 'http://www.wikidata.org/entity/Q11574442', 'http://www.wikidata.org/entity/Q11574503', 'http://www.wikidata.org/entity/Q11574566', 'http://www.wikidata.org/entity/Q11574873', 'http://www.wikidata.org/entity/Q11576597', 'http://www.wikidata.org/entity/Q11577548', 'http://www.wikidata.org/entity/Q11577742', 'http://www.wikidata.org/entity/Q11578144', 'http://www.wikidata.org/entity/Q11578192', 'http://www.wikidata.org/entity/Q11578542', 'http://www.wikidata.org/entity/Q11579570', 'http://www.wikidata.org/entity/Q11580729', 'http://www.wikidata.org/entity/Q11580862', 'http://www.wikidata.org/entity/Q11580911', 'http://www.wikidata.org/entity/Q11581974', 'http://www.wikidata.org/entity/Q11581975', 'http://www.wikidata.org/entity/Q11583780', 'http://www.wikidata.org/entity/Q11583965', 'http://www.wikidata.org/entity/Q11588028', 'http://www.wikidata.org/entity/Q11588453', 'http://www.wikidata.org/entity/Q11589438', 'http://www.wikidata.org/entity/Q11589594', 'http://www.wikidata.org/entity/Q11591024', 'http://www.wikidata.org/entity/Q11592984', 'http://www.wikidata.org/entity/Q11596394', 'http://www.wikidata.org/entity/Q11598512', 'http://www.wikidata.org/entity/Q11598646', 'http://www.wikidata.org/entity/Q11598647', 'http://www.wikidata.org/entity/Q11599897', 'http://www.wikidata.org/entity/Q11602695', 'http://www.wikidata.org/entity/Q11603507', 'http://www.wikidata.org/entity/Q11603714', 'http://www.wikidata.org/entity/Q11604580', 'http://www.wikidata.org/entity/Q11604657', 'http://www.wikidata.org/entity/Q11605347', 'http://www.wikidata.org/entity/Q11607173', 'http://www.wikidata.org/entity/Q11610036', 'http://www.wikidata.org/entity/Q11612025', 'http://www.wikidata.org/entity/Q11613384', 'http://www.wikidata.org/entity/Q11614676', 'http://www.wikidata.org/entity/Q11616271', 'http://www.wikidata.org/entity/Q11622569', 'http://www.wikidata.org/entity/Q11625567', 'http://www.wikidata.org/entity/Q11626891', 'http://www.wikidata.org/entity/Q11630243', 'http://www.wikidata.org/entity/Q11631382', 'http://www.wikidata.org/entity/Q11633491', 'http://www.wikidata.org/entity/Q11633492', 'http://www.wikidata.org/entity/Q11634353', 'http://www.wikidata.org/entity/Q11635889', 'http://www.wikidata.org/entity/Q11636071', 'http://www.wikidata.org/entity/Q11636883', 'http://www.wikidata.org/entity/Q116373818', 'http://www.wikidata.org/entity/Q11645346', 'http://www.wikidata.org/entity/Q11645453', 'http://www.wikidata.org/entity/Q11647939', 'http://www.wikidata.org/entity/Q11648162', 'http://www.wikidata.org/entity/Q11648224', 'http://www.wikidata.org/entity/Q11650283', 'http://www.wikidata.org/entity/Q11650626', 'http://www.wikidata.org/entity/Q11652193', 'http://www.wikidata.org/entity/Q11652198', 'http://www.wikidata.org/entity/Q11652204', 'http://www.wikidata.org/entity/Q11652207', 'http://www.wikidata.org/entity/Q11655424', 'http://www.wikidata.org/entity/Q11657147', 'http://www.wikidata.org/entity/Q11657359', 'http://www.wikidata.org/entity/Q11659209', 'http://www.wikidata.org/entity/Q11661369', 'http://www.wikidata.org/entity/Q11661370', 'http://www.wikidata.org/entity/Q11661371', 'http://www.wikidata.org/entity/Q11661373', 'http://www.wikidata.org/entity/Q11662600', 'http://www.wikidata.org/entity/Q11664922', 'http://www.wikidata.org/entity/Q11664932', 'http://www.wikidata.org/entity/Q11665527', 'http://www.wikidata.org/entity/Q11665758', 'http://www.wikidata.org/entity/Q11665759', 'http://www.wikidata.org/entity/Q11667955', 'http://www.wikidata.org/entity/Q11667995', 'http://www.wikidata.org/entity/Q11668024', 'http://www.wikidata.org/entity/Q11668037', 'http://www.wikidata.org/entity/Q11668718', 'http://www.wikidata.org/entity/Q11669590', 'http://www.wikidata.org/entity/Q11669595', 'http://www.wikidata.org/entity/Q11669597', 'http://www.wikidata.org/entity/Q11669598', 'http://www.wikidata.org/entity/Q11669599', 'http://www.wikidata.org/entity/Q11669603', 'http://www.wikidata.org/entity/Q11669605', 'http://www.wikidata.org/entity/Q11670635', 'http://www.wikidata.org/entity/Q11673959', 'http://www.wikidata.org/entity/Q11674270', 'http://www.wikidata.org/entity/Q11675635', 'http://www.wikidata.org/entity/Q11675694', 'http://www.wikidata.org/entity/Q11675705', 'http://www.wikidata.org/entity/Q11675721', 'http://www.wikidata.org/entity/Q11675825', 'http://www.wikidata.org/entity/Q11676467', 'http://www.wikidata.org/entity/Q11677072', 'http://www.wikidata.org/entity/Q116774724', 'http://www.wikidata.org/entity/Q11678083', 'http://www.wikidata.org/entity/Q11678144', 'http://www.wikidata.org/entity/Q11678145', 'http://www.wikidata.org/entity/Q11678146', 'http://www.wikidata.org/entity/Q11678147', 'http://www.wikidata.org/entity/Q11678919', 'http://www.wikidata.org/entity/Q1204188', 'http://www.wikidata.org/entity/Q12122598', 'http://www.wikidata.org/entity/Q12168088', 'http://www.wikidata.org/entity/Q122792969', 'http://www.wikidata.org/entity/Q123092880', 'http://www.wikidata.org/entity/Q123554758', 'http://www.wikidata.org/entity/Q123554899', 'http://www.wikidata.org/entity/Q123563180', 'http://www.wikidata.org/entity/Q123568579', 'http://www.wikidata.org/entity/Q123592347', 'http://www.wikidata.org/entity/Q123592528', 'http://www.wikidata.org/entity/Q123630881', 'http://www.wikidata.org/entity/Q123631133', 'http://www.wikidata.org/entity/Q123848497', 'http://www.wikidata.org/entity/Q126617200', 'http://www.wikidata.org/entity/Q130120', 'http://www.wikidata.org/entity/Q130535', 'http://www.wikidata.org/entity/Q1344326', 'http://www.wikidata.org/entity/Q137962', 'http://www.wikidata.org/entity/Q13987', 'http://www.wikidata.org/entity/Q13991', 'http://www.wikidata.org/entity/Q1414691', 'http://www.wikidata.org/entity/Q145371', 'http://www.wikidata.org/entity/Q1475428', 'http://www.wikidata.org/entity/Q14948405', 'http://www.wikidata.org/entity/Q14948406', 'http://www.wikidata.org/entity/Q15231937', 'http://www.wikidata.org/entity/Q15233224', 'http://www.wikidata.org/entity/Q1532472', 'http://www.wikidata.org/entity/Q15914611', 'http://www.wikidata.org/entity/Q15914636', 'http://www.wikidata.org/entity/Q15914793', 'http://www.wikidata.org/entity/Q15914839', 'http://www.wikidata.org/entity/Q15914850', 'http://www.wikidata.org/entity/Q15914965', 'http://www.wikidata.org/entity/Q15915038', 'http://www.wikidata.org/entity/Q15915094', 'http://www.wikidata.org/entity/Q15915371', 'http://www.wikidata.org/entity/Q15915516', 'http://www.wikidata.org/entity/Q15915542', 'http://www.wikidata.org/entity/Q15915739', 'http://www.wikidata.org/entity/Q15915768', 'http://www.wikidata.org/entity/Q15915877', 'http://www.wikidata.org/entity/Q15915985', 'http://www.wikidata.org/entity/Q15916001', 'http://www.wikidata.org/entity/Q15916180', 'http://www.wikidata.org/entity/Q15916186', 'http://www.wikidata.org/entity/Q15916187', 'http://www.wikidata.org/entity/Q15916216', 'http://www.wikidata.org/entity/Q15916253', 'http://www.wikidata.org/entity/Q15916254', 'http://www.wikidata.org/entity/Q15916285', 'http://www.wikidata.org/entity/Q15916297', 'http://www.wikidata.org/entity/Q15916298', 'http://www.wikidata.org/entity/Q15916369', 'http://www.wikidata.org/entity/Q15916370', 'http://www.wikidata.org/entity/Q15916387', 'http://www.wikidata.org/entity/Q15916410', 'http://www.wikidata.org/entity/Q15916434', 'http://www.wikidata.org/entity/Q15916435', 'http://www.wikidata.org/entity/Q15916437', 'http://www.wikidata.org/entity/Q15916438', 'http://www.wikidata.org/entity/Q15916508', 'http://www.wikidata.org/entity/Q15923957', 'http://www.wikidata.org/entity/Q15924538', 'http://www.wikidata.org/entity/Q15925138', 'http://www.wikidata.org/entity/Q15925270', 'http://www.wikidata.org/entity/Q1676132', 'http://www.wikidata.org/entity/Q169589', 'http://www.wikidata.org/entity/Q17021654', 'http://www.wikidata.org/entity/Q17023687', 'http://www.wikidata.org/entity/Q17031459', 'http://www.wikidata.org/entity/Q17039990', 'http://www.wikidata.org/entity/Q17191315', 'http://www.wikidata.org/entity/Q17191378', 'http://www.wikidata.org/entity/Q17192049', 'http://www.wikidata.org/entity/Q17192826', 'http://www.wikidata.org/entity/Q17193690', 'http://www.wikidata.org/entity/Q17210135', 'http://www.wikidata.org/entity/Q17210185', 'http://www.wikidata.org/entity/Q17211889', 'http://www.wikidata.org/entity/Q17214084', 'http://www.wikidata.org/entity/Q17215469', 'http://www.wikidata.org/entity/Q17216064', 'http://www.wikidata.org/entity/Q17216375', 'http://www.wikidata.org/entity/Q17217423', 'http://www.wikidata.org/entity/Q17219919', 'http://www.wikidata.org/entity/Q17221048', 'http://www.wikidata.org/entity/Q17222656', 'http://www.wikidata.org/entity/Q17223389', 'http://www.wikidata.org/entity/Q17225029', 'http://www.wikidata.org/entity/Q17989148', 'http://www.wikidata.org/entity/Q17989626', 'http://www.wikidata.org/entity/Q17992764', 'http://www.wikidata.org/entity/Q17993734', 'http://www.wikidata.org/entity/Q17995776', 'http://www.wikidata.org/entity/Q18003098', 'http://www.wikidata.org/entity/Q18009413', 'http://www.wikidata.org/entity/Q18010599', 'http://www.wikidata.org/entity/Q1803811', 'http://www.wikidata.org/entity/Q18335728', 'http://www.wikidata.org/entity/Q18336591', 'http://www.wikidata.org/entity/Q18336657', 'http://www.wikidata.org/entity/Q18338827', 'http://www.wikidata.org/entity/Q18338974', 'http://www.wikidata.org/entity/Q18339013', 'http://www.wikidata.org/entity/Q18339157', 'http://www.wikidata.org/entity/Q18339362', 'http://www.wikidata.org/entity/Q18339537', 'http://www.wikidata.org/entity/Q18339548', 'http://www.wikidata.org/entity/Q18700735', 'http://www.wikidata.org/entity/Q187366', 'http://www.wikidata.org/entity/Q196701', 'http://www.wikidata.org/entity/Q19926707', 'http://www.wikidata.org/entity/Q19927579', 'http://www.wikidata.org/entity/Q19927913', 'http://www.wikidata.org/entity/Q19928028', 'http://www.wikidata.org/entity/Q1995509', 'http://www.wikidata.org/entity/Q19969455', 'http://www.wikidata.org/entity/Q19969456', 'http://www.wikidata.org/entity/Q19969457', 'http://www.wikidata.org/entity/Q19969459', 'http://www.wikidata.org/entity/Q19969461', 'http://www.wikidata.org/entity/Q19969462', 'http://www.wikidata.org/entity/Q19969463', 'http://www.wikidata.org/entity/Q20043639', 'http://www.wikidata.org/entity/Q20160219', 'http://www.wikidata.org/entity/Q2018422', 'http://www.wikidata.org/entity/Q20207875', 'http://www.wikidata.org/entity/Q20208336', 'http://www.wikidata.org/entity/Q20208605', 'http://www.wikidata.org/entity/Q20220282', 'http://www.wikidata.org/entity/Q20220291', 'http://www.wikidata.org/entity/Q20249559', 'http://www.wikidata.org/entity/Q20251315', 'http://www.wikidata.org/entity/Q20267482', 'http://www.wikidata.org/entity/Q20441459', 'http://www.wikidata.org/entity/Q20441495', 'http://www.wikidata.org/entity/Q20441538', 'http://www.wikidata.org/entity/Q20441672', 'http://www.wikidata.org/entity/Q20441835', 'http://www.wikidata.org/entity/Q20442833', 'http://www.wikidata.org/entity/Q20442886', 'http://www.wikidata.org/entity/Q20454159', 'http://www.wikidata.org/entity/Q20652984', 'http://www.wikidata.org/entity/Q20653009', 'http://www.wikidata.org/entity/Q20653020', 'http://www.wikidata.org/entity/Q20653048', 'http://www.wikidata.org/entity/Q20653083', 'http://www.wikidata.org/entity/Q20653128', 'http://www.wikidata.org/entity/Q20655767', 'http://www.wikidata.org/entity/Q20655779', 'http://www.wikidata.org/entity/Q20655824', 'http://www.wikidata.org/entity/Q20655829', 'http://www.wikidata.org/entity/Q20655854', 'http://www.wikidata.org/entity/Q20655861', 'http://www.wikidata.org/entity/Q20656218', 'http://www.wikidata.org/entity/Q20662194', 'http://www.wikidata.org/entity/Q20662421', 'http://www.wikidata.org/entity/Q20665543', 'http://www.wikidata.org/entity/Q20669152', 'http://www.wikidata.org/entity/Q20669173', 'http://www.wikidata.org/entity/Q20669188', 'http://www.wikidata.org/entity/Q20669201', 'http://www.wikidata.org/entity/Q20669474', 'http://www.wikidata.org/entity/Q20670485', 'http://www.wikidata.org/entity/Q20670486', 'http://www.wikidata.org/entity/Q20670489', 'http://www.wikidata.org/entity/Q20670490', 'http://www.wikidata.org/entity/Q20670802', 'http://www.wikidata.org/entity/Q20670818', 'http://www.wikidata.org/entity/Q20670842', 'http://www.wikidata.org/entity/Q20680346', 'http://www.wikidata.org/entity/Q20681784', 'http://www.wikidata.org/entity/Q20681836', 'http://www.wikidata.org/entity/Q20687296', 'http://www.wikidata.org/entity/Q20706572', 'http://www.wikidata.org/entity/Q20706579', 'http://www.wikidata.org/entity/Q20706699', 'http://www.wikidata.org/entity/Q20709285', 'http://www.wikidata.org/entity/Q2118388', 'http://www.wikidata.org/entity/Q21652956', 'http://www.wikidata.org/entity/Q21652975', 'http://www.wikidata.org/entity/Q21653337', 'http://www.wikidata.org/entity/Q21653909', 'http://www.wikidata.org/entity/Q21654565', 'http://www.wikidata.org/entity/Q2166413', 'http://www.wikidata.org/entity/Q220701', 'http://www.wikidata.org/entity/Q23069893', 'http://www.wikidata.org/entity/Q2407298', 'http://www.wikidata.org/entity/Q242176', 'http://www.wikidata.org/entity/Q24488445', 'http://www.wikidata.org/entity/Q247515', 'http://www.wikidata.org/entity/Q24871573', 'http://www.wikidata.org/entity/Q24872138', 'http://www.wikidata.org/entity/Q24875184', 'http://www.wikidata.org/entity/Q24898648', 'http://www.wikidata.org/entity/Q24902485', 'http://www.wikidata.org/entity/Q27560716', 'http://www.wikidata.org/entity/Q277035', 'http://www.wikidata.org/entity/Q28155659', 'http://www.wikidata.org/entity/Q285468', 'http://www.wikidata.org/entity/Q28682242', 'http://www.wikidata.org/entity/Q28682892', 'http://www.wikidata.org/entity/Q28682901', 'http://www.wikidata.org/entity/Q28683300', 'http://www.wikidata.org/entity/Q28684991', 'http://www.wikidata.org/entity/Q28684995', 'http://www.wikidata.org/entity/Q28687509', 'http://www.wikidata.org/entity/Q28687512', 'http://www.wikidata.org/entity/Q28687517', 'http://www.wikidata.org/entity/Q28687518', 'http://www.wikidata.org/entity/Q28687526', 'http://www.wikidata.org/entity/Q28687528', 'http://www.wikidata.org/entity/Q28687549', 'http://www.wikidata.org/entity/Q28687551', 'http://www.wikidata.org/entity/Q28687556', 'http://www.wikidata.org/entity/Q28687561', 'http://www.wikidata.org/entity/Q28687591', 'http://www.wikidata.org/entity/Q28693411', 'http://www.wikidata.org/entity/Q29980548', 'http://www.wikidata.org/entity/Q30925772', 'http://www.wikidata.org/entity/Q30925773', 'http://www.wikidata.org/entity/Q30931692', 'http://www.wikidata.org/entity/Q30931979', 'http://www.wikidata.org/entity/Q3108859', 'http://www.wikidata.org/entity/Q3199146', 'http://www.wikidata.org/entity/Q3285144', 'http://www.wikidata.org/entity/Q328533', 'http://www.wikidata.org/entity/Q3349795', 'http://www.wikidata.org/entity/Q339004', 'http://www.wikidata.org/entity/Q34783955', 'http://www.wikidata.org/entity/Q34783964', 'http://www.wikidata.org/entity/Q34783974', 'http://www.wikidata.org/entity/Q34784035', 'http://www.wikidata.org/entity/Q34784045', 'http://www.wikidata.org/entity/Q34784074', 'http://www.wikidata.org/entity/Q34784082', 'http://www.wikidata.org/entity/Q34784090', 'http://www.wikidata.org/entity/Q34784099', 'http://www.wikidata.org/entity/Q34784108', 'http://www.wikidata.org/entity/Q34784117', 'http://www.wikidata.org/entity/Q34784145', 'http://www.wikidata.org/entity/Q34784154', 'http://www.wikidata.org/entity/Q34784163', 'http://www.wikidata.org/entity/Q34784172', 'http://www.wikidata.org/entity/Q34784180', 'http://www.wikidata.org/entity/Q34784236', 'http://www.wikidata.org/entity/Q34784245', 'http://www.wikidata.org/entity/Q34784264', 'http://www.wikidata.org/entity/Q34784309', 'http://www.wikidata.org/entity/Q34784328', 'http://www.wikidata.org/entity/Q34784514', 'http://www.wikidata.org/entity/Q34785535', 'http://www.wikidata.org/entity/Q34785547', 'http://www.wikidata.org/entity/Q34787923', 'http://www.wikidata.org/entity/Q34787927', 'http://www.wikidata.org/entity/Q34787936', 'http://www.wikidata.org/entity/Q34787940', 'http://www.wikidata.org/entity/Q34787945', 'http://www.wikidata.org/entity/Q34787948', 'http://www.wikidata.org/entity/Q34787955', 'http://www.wikidata.org/entity/Q34787960', 'http://www.wikidata.org/entity/Q34787964', 'http://www.wikidata.org/entity/Q34787968', 'http://www.wikidata.org/entity/Q34787980', 'http://www.wikidata.org/entity/Q34787985', 'http://www.wikidata.org/entity/Q34788048', 'http://www.wikidata.org/entity/Q34788086', 'http://www.wikidata.org/entity/Q34788091', 'http://www.wikidata.org/entity/Q34788095', 'http://www.wikidata.org/entity/Q34788578', 'http://www.wikidata.org/entity/Q34788581', 'http://www.wikidata.org/entity/Q34788617', 'http://www.wikidata.org/entity/Q34788621', 'http://www.wikidata.org/entity/Q34788699', 'http://www.wikidata.org/entity/Q34795633', 'http://www.wikidata.org/entity/Q34795652', 'http://www.wikidata.org/entity/Q34795659', 'http://www.wikidata.org/entity/Q34795671', 'http://www.wikidata.org/entity/Q34795678', 'http://www.wikidata.org/entity/Q34795686', 'http://www.wikidata.org/entity/Q34795693', 'http://www.wikidata.org/entity/Q34795722', 'http://www.wikidata.org/entity/Q34795734', 'http://www.wikidata.org/entity/Q34795744', 'http://www.wikidata.org/entity/Q34795753', 'http://www.wikidata.org/entity/Q34795770', 'http://www.wikidata.org/entity/Q34795778', 'http://www.wikidata.org/entity/Q34795788', 'http://www.wikidata.org/entity/Q34795804', 'http://www.wikidata.org/entity/Q34795808', 'http://www.wikidata.org/entity/Q34795832', 'http://www.wikidata.org/entity/Q34795844', 'http://www.wikidata.org/entity/Q34795856', 'http://www.wikidata.org/entity/Q34795867', 'http://www.wikidata.org/entity/Q34795874', 'http://www.wikidata.org/entity/Q34795887', 'http://www.wikidata.org/entity/Q34795901', 'http://www.wikidata.org/entity/Q34795907', 'http://www.wikidata.org/entity/Q34795913', 'http://www.wikidata.org/entity/Q34795937', 'http://www.wikidata.org/entity/Q34795942', 'http://www.wikidata.org/entity/Q34795954', 'http://www.wikidata.org/entity/Q34795961', 'http://www.wikidata.org/entity/Q34795967', 'http://www.wikidata.org/entity/Q34795972', 'http://www.wikidata.org/entity/Q34795984', 'http://www.wikidata.org/entity/Q34795990', 'http://www.wikidata.org/entity/Q34795996', 'http://www.wikidata.org/entity/Q34796002', 'http://www.wikidata.org/entity/Q34796008', 'http://www.wikidata.org/entity/Q34796015', 'http://www.wikidata.org/entity/Q34796021', 'http://www.wikidata.org/entity/Q34796028', 'http://www.wikidata.org/entity/Q34796033', 'http://www.wikidata.org/entity/Q34796043', 'http://www.wikidata.org/entity/Q34796055', 'http://www.wikidata.org/entity/Q34796071', 'http://www.wikidata.org/entity/Q34796095', 'http://www.wikidata.org/entity/Q34796102', 'http://www.wikidata.org/entity/Q34796119', 'http://www.wikidata.org/entity/Q34796134', 'http://www.wikidata.org/entity/Q34796146', 'http://www.wikidata.org/entity/Q34796151', 'http://www.wikidata.org/entity/Q34796158', 'http://www.wikidata.org/entity/Q34796163', 'http://www.wikidata.org/entity/Q34796170', 'http://www.wikidata.org/entity/Q34796175', 'http://www.wikidata.org/entity/Q34796180', 'http://www.wikidata.org/entity/Q34861379', 'http://www.wikidata.org/entity/Q34861390', 'http://www.wikidata.org/entity/Q34861523', 'http://www.wikidata.org/entity/Q34861562', 'http://www.wikidata.org/entity/Q34861821', 'http://www.wikidata.org/entity/Q34862653', 'http://www.wikidata.org/entity/Q3579074', 'http://www.wikidata.org/entity/Q3594049', 'http://www.wikidata.org/entity/Q3623017', 'http://www.wikidata.org/entity/Q3785700', 'http://www.wikidata.org/entity/Q382082', 'http://www.wikidata.org/entity/Q38266996', 'http://www.wikidata.org/entity/Q385313', 'http://www.wikidata.org/entity/Q385710', 'http://www.wikidata.org/entity/Q393031', 'http://www.wikidata.org/entity/Q398636', 'http://www.wikidata.org/entity/Q432124', 'http://www.wikidata.org/entity/Q4419675', 'http://www.wikidata.org/entity/Q4419682', 'http://www.wikidata.org/entity/Q4478859', 'http://www.wikidata.org/entity/Q4497854', 'http://www.wikidata.org/entity/Q4518163', 'http://www.wikidata.org/entity/Q4518364', 'http://www.wikidata.org/entity/Q4518483', 'http://www.wikidata.org/entity/Q4518560', 'http://www.wikidata.org/entity/Q4518632', 'http://www.wikidata.org/entity/Q4518662', 'http://www.wikidata.org/entity/Q4518698', 'http://www.wikidata.org/entity/Q4518728', 'http://www.wikidata.org/entity/Q4518764', 'http://www.wikidata.org/entity/Q4518813', 'http://www.wikidata.org/entity/Q4518835', 'http://www.wikidata.org/entity/Q4518882', 'http://www.wikidata.org/entity/Q4518914', 'http://www.wikidata.org/entity/Q4518946', 'http://www.wikidata.org/entity/Q4519060', 'http://www.wikidata.org/entity/Q4519100', 'http://www.wikidata.org/entity/Q4519127', 'http://www.wikidata.org/entity/Q4519202', 'http://www.wikidata.org/entity/Q4519334', 'http://www.wikidata.org/entity/Q4519416', 'http://www.wikidata.org/entity/Q4519472', 'http://www.wikidata.org/entity/Q4520401', 'http://www.wikidata.org/entity/Q4520501', 'http://www.wikidata.org/entity/Q4520623', 'http://www.wikidata.org/entity/Q4520676', 'http://www.wikidata.org/entity/Q4520740', 'http://www.wikidata.org/entity/Q473472', 'http://www.wikidata.org/entity/Q474560', 'http://www.wikidata.org/entity/Q48752569', 'http://www.wikidata.org/entity/Q48752621', 'http://www.wikidata.org/entity/Q490610', 'http://www.wikidata.org/entity/Q49333374', 'http://www.wikidata.org/entity/Q494914', 'http://www.wikidata.org/entity/Q49493', 'http://www.wikidata.org/entity/Q49500', 'http://www.wikidata.org/entity/Q49507', 'http://www.wikidata.org/entity/Q49511', 'http://www.wikidata.org/entity/Q49513', 'http://www.wikidata.org/entity/Q49631357', 'http://www.wikidata.org/entity/Q49631388', 'http://www.wikidata.org/entity/Q49631402', 'http://www.wikidata.org/entity/Q49631408', 'http://www.wikidata.org/entity/Q49631415', 'http://www.wikidata.org/entity/Q49631418', 'http://www.wikidata.org/entity/Q49631448', 'http://www.wikidata.org/entity/Q49631449', 'http://www.wikidata.org/entity/Q49631468', 'http://www.wikidata.org/entity/Q49631471', 'http://www.wikidata.org/entity/Q49631484', 'http://www.wikidata.org/entity/Q49631487', 'http://www.wikidata.org/entity/Q49631489', 'http://www.wikidata.org/entity/Q49631490', 'http://www.wikidata.org/entity/Q49631492', 'http://www.wikidata.org/entity/Q49631493', 'http://www.wikidata.org/entity/Q49631495', 'http://www.wikidata.org/entity/Q49631497', 'http://www.wikidata.org/entity/Q49631501', 'http://www.wikidata.org/entity/Q49631532', 'http://www.wikidata.org/entity/Q49631657', 'http://www.wikidata.org/entity/Q49631707', 'http://www.wikidata.org/entity/Q49631712', 'http://www.wikidata.org/entity/Q49631766', 'http://www.wikidata.org/entity/Q49631801', 'http://www.wikidata.org/entity/Q49631841', 'http://www.wikidata.org/entity/Q49631849', 'http://www.wikidata.org/entity/Q49631851', 'http://www.wikidata.org/entity/Q49631852', 'http://www.wikidata.org/entity/Q49631855', 'http://www.wikidata.org/entity/Q49631874', 'http://www.wikidata.org/entity/Q49631881', 'http://www.wikidata.org/entity/Q49631883', </t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>['Adele Laurie Blue Adkins']</t>
+          <t xml:space="preserve">['http://www.wikidata.org/entity/Q100695440', 'http://www.wikidata.org/entity/Q1019313', 'http://www.wikidata.org/entity/Q102245375', 'http://www.wikidata.org/entity/Q1039445', 'http://www.wikidata.org/entity/Q104186080', 'http://www.wikidata.org/entity/Q10449219', 'http://www.wikidata.org/entity/Q1047492', 'http://www.wikidata.org/entity/Q1061394', 'http://www.wikidata.org/entity/Q106150403', 'http://www.wikidata.org/entity/Q106363078', 'http://www.wikidata.org/entity/Q1072125', 'http://www.wikidata.org/entity/Q1083890', 'http://www.wikidata.org/entity/Q10855760', 'http://www.wikidata.org/entity/Q10855761', 'http://www.wikidata.org/entity/Q10856210', 'http://www.wikidata.org/entity/Q10859834', 'http://www.wikidata.org/entity/Q10860535', 'http://www.wikidata.org/entity/Q10889854', 'http://www.wikidata.org/entity/Q109368351', 'http://www.wikidata.org/entity/Q10938711', 'http://www.wikidata.org/entity/Q109405713', 'http://www.wikidata.org/entity/Q10943140', 'http://www.wikidata.org/entity/Q109673419', 'http://www.wikidata.org/entity/Q1111504', 'http://www.wikidata.org/entity/Q112224546', 'http://www.wikidata.org/entity/Q11234719', 'http://www.wikidata.org/entity/Q11241368', 'http://www.wikidata.org/entity/Q11261668', 'http://www.wikidata.org/entity/Q112673064', 'http://www.wikidata.org/entity/Q11276631', 'http://www.wikidata.org/entity/Q11285385', 'http://www.wikidata.org/entity/Q11286923', 'http://www.wikidata.org/entity/Q11353972', 'http://www.wikidata.org/entity/Q11354008', 'http://www.wikidata.org/entity/Q11356195', 'http://www.wikidata.org/entity/Q11357220', 'http://www.wikidata.org/entity/Q11358913', 'http://www.wikidata.org/entity/Q11360086', 'http://www.wikidata.org/entity/Q11360847', 'http://www.wikidata.org/entity/Q11361905', 'http://www.wikidata.org/entity/Q11362796', 'http://www.wikidata.org/entity/Q11362797', 'http://www.wikidata.org/entity/Q11362799', 'http://www.wikidata.org/entity/Q11369263', 'http://www.wikidata.org/entity/Q11369927', 'http://www.wikidata.org/entity/Q11370029', 'http://www.wikidata.org/entity/Q11370104', 'http://www.wikidata.org/entity/Q11371742', 'http://www.wikidata.org/entity/Q11373491', 'http://www.wikidata.org/entity/Q11376329', 'http://www.wikidata.org/entity/Q11377524', 'http://www.wikidata.org/entity/Q11378204', 'http://www.wikidata.org/entity/Q11379228', 'http://www.wikidata.org/entity/Q11379335', 'http://www.wikidata.org/entity/Q11382608', 'http://www.wikidata.org/entity/Q11383201', 'http://www.wikidata.org/entity/Q11383217', 'http://www.wikidata.org/entity/Q11385812', 'http://www.wikidata.org/entity/Q11386818', 'http://www.wikidata.org/entity/Q11390867', 'http://www.wikidata.org/entity/Q11390868', 'http://www.wikidata.org/entity/Q11392330', 'http://www.wikidata.org/entity/Q11394726', 'http://www.wikidata.org/entity/Q11395612', 'http://www.wikidata.org/entity/Q11395786', 'http://www.wikidata.org/entity/Q11397118', 'http://www.wikidata.org/entity/Q11398556', 'http://www.wikidata.org/entity/Q11399769', 'http://www.wikidata.org/entity/Q11401908', 'http://www.wikidata.org/entity/Q11402215', 'http://www.wikidata.org/entity/Q11402223', 'http://www.wikidata.org/entity/Q11407776', 'http://www.wikidata.org/entity/Q11409587', 'http://www.wikidata.org/entity/Q11410659', 'http://www.wikidata.org/entity/Q11415949', 'http://www.wikidata.org/entity/Q11415951', 'http://www.wikidata.org/entity/Q11415952', 'http://www.wikidata.org/entity/Q11415953', 'http://www.wikidata.org/entity/Q11416626', 'http://www.wikidata.org/entity/Q11418533', 'http://www.wikidata.org/entity/Q11419386', 'http://www.wikidata.org/entity/Q11419637', 'http://www.wikidata.org/entity/Q11420237', 'http://www.wikidata.org/entity/Q11424450', 'http://www.wikidata.org/entity/Q11424752', 'http://www.wikidata.org/entity/Q11425641', 'http://www.wikidata.org/entity/Q11430798', 'http://www.wikidata.org/entity/Q11431830', 'http://www.wikidata.org/entity/Q11432478', 'http://www.wikidata.org/entity/Q11434172', 'http://www.wikidata.org/entity/Q11434804', 'http://www.wikidata.org/entity/Q11434805', 'http://www.wikidata.org/entity/Q11434806', 'http://www.wikidata.org/entity/Q11434807', 'http://www.wikidata.org/entity/Q11434809', 'http://www.wikidata.org/entity/Q11434813', 'http://www.wikidata.org/entity/Q11434815', 'http://www.wikidata.org/entity/Q11434816', 'http://www.wikidata.org/entity/Q11434819', 'http://www.wikidata.org/entity/Q11435005', 'http://www.wikidata.org/entity/Q11435006', 'http://www.wikidata.org/entity/Q11436454', 'http://www.wikidata.org/entity/Q11436765', 'http://www.wikidata.org/entity/Q11437275', 'http://www.wikidata.org/entity/Q11438136', 'http://www.wikidata.org/entity/Q11438379', 'http://www.wikidata.org/entity/Q11439590', 'http://www.wikidata.org/entity/Q11442082', 'http://www.wikidata.org/entity/Q11443237', 'http://www.wikidata.org/entity/Q11445536', 'http://www.wikidata.org/entity/Q11446412', 'http://www.wikidata.org/entity/Q11447403', 'http://www.wikidata.org/entity/Q11447404', 'http://www.wikidata.org/entity/Q11449014', 'http://www.wikidata.org/entity/Q11449464', 'http://www.wikidata.org/entity/Q11450585', 'http://www.wikidata.org/entity/Q11454772', 'http://www.wikidata.org/entity/Q11458850', 'http://www.wikidata.org/entity/Q11459344', 'http://www.wikidata.org/entity/Q11459579', 'http://www.wikidata.org/entity/Q11460065', 'http://www.wikidata.org/entity/Q11460438', 'http://www.wikidata.org/entity/Q11464517', 'http://www.wikidata.org/entity/Q11465691', 'http://www.wikidata.org/entity/Q11474307', 'http://www.wikidata.org/entity/Q11474346', 'http://www.wikidata.org/entity/Q11475712', 'http://www.wikidata.org/entity/Q11476827', 'http://www.wikidata.org/entity/Q11476897', 'http://www.wikidata.org/entity/Q11477129', 'http://www.wikidata.org/entity/Q11477305', 'http://www.wikidata.org/entity/Q11477410', 'http://www.wikidata.org/entity/Q11481155', 'http://www.wikidata.org/entity/Q11482668', 'http://www.wikidata.org/entity/Q11482669', 'http://www.wikidata.org/entity/Q11483492', 'http://www.wikidata.org/entity/Q11483589', 'http://www.wikidata.org/entity/Q11483827', 'http://www.wikidata.org/entity/Q11484404', 'http://www.wikidata.org/entity/Q11486132', 'http://www.wikidata.org/entity/Q11486908', 'http://www.wikidata.org/entity/Q11486909', 'http://www.wikidata.org/entity/Q11486910', 'http://www.wikidata.org/entity/Q11486911', 'http://www.wikidata.org/entity/Q11487067', 'http://www.wikidata.org/entity/Q11487395', 'http://www.wikidata.org/entity/Q11488768', 'http://www.wikidata.org/entity/Q11489067', 'http://www.wikidata.org/entity/Q11489240', 'http://www.wikidata.org/entity/Q11489251', 'http://www.wikidata.org/entity/Q11490807', 'http://www.wikidata.org/entity/Q11491460', 'http://www.wikidata.org/entity/Q11491674', 'http://www.wikidata.org/entity/Q11492404', 'http://www.wikidata.org/entity/Q11492410', 'http://www.wikidata.org/entity/Q11492883', 'http://www.wikidata.org/entity/Q11492884', 'http://www.wikidata.org/entity/Q11496323', 'http://www.wikidata.org/entity/Q11496324', 'http://www.wikidata.org/entity/Q11496670', 'http://www.wikidata.org/entity/Q11497087', 'http://www.wikidata.org/entity/Q11497519', 'http://www.wikidata.org/entity/Q11500406', 'http://www.wikidata.org/entity/Q11501924', 'http://www.wikidata.org/entity/Q11502024', 'http://www.wikidata.org/entity/Q11502876', 'http://www.wikidata.org/entity/Q11504920', 'http://www.wikidata.org/entity/Q11505281', 'http://www.wikidata.org/entity/Q11505343', 'http://www.wikidata.org/entity/Q11511249', 'http://www.wikidata.org/entity/Q11516644', 'http://www.wikidata.org/entity/Q11520216', 'http://www.wikidata.org/entity/Q11530091', 'http://www.wikidata.org/entity/Q11530093', 'http://www.wikidata.org/entity/Q11532746', 'http://www.wikidata.org/entity/Q11533729', 'http://www.wikidata.org/entity/Q11542683', 'http://www.wikidata.org/entity/Q11542685', 'http://www.wikidata.org/entity/Q11543672', 'http://www.wikidata.org/entity/Q11544654', 'http://www.wikidata.org/entity/Q11544655', 'http://www.wikidata.org/entity/Q11545996', 'http://www.wikidata.org/entity/Q11547731', 'http://www.wikidata.org/entity/Q11548193', 'http://www.wikidata.org/entity/Q11548462', 'http://www.wikidata.org/entity/Q11550173', 'http://www.wikidata.org/entity/Q11550842', 'http://www.wikidata.org/entity/Q11550845', 'http://www.wikidata.org/entity/Q11551591', 'http://www.wikidata.org/entity/Q11552439', 'http://www.wikidata.org/entity/Q11552466', 'http://www.wikidata.org/entity/Q11552477', 'http://www.wikidata.org/entity/Q11552498', 'http://www.wikidata.org/entity/Q11552502', 'http://www.wikidata.org/entity/Q11552549', 'http://www.wikidata.org/entity/Q11553027', 'http://www.wikidata.org/entity/Q11555929', 'http://www.wikidata.org/entity/Q11555966', 'http://www.wikidata.org/entity/Q11556058', 'http://www.wikidata.org/entity/Q11556221', 'http://www.wikidata.org/entity/Q11558501', 'http://www.wikidata.org/entity/Q11558503', 'http://www.wikidata.org/entity/Q11558824', 'http://www.wikidata.org/entity/Q11559068', 'http://www.wikidata.org/entity/Q11559418', 'http://www.wikidata.org/entity/Q11559763', 'http://www.wikidata.org/entity/Q11559986', 'http://www.wikidata.org/entity/Q11562837', 'http://www.wikidata.org/entity/Q11563518', 'http://www.wikidata.org/entity/Q11567224', 'http://www.wikidata.org/entity/Q11567245', 'http://www.wikidata.org/entity/Q11567267', 'http://www.wikidata.org/entity/Q11572200', 'http://www.wikidata.org/entity/Q11572311', 'http://www.wikidata.org/entity/Q11573306', 'http://www.wikidata.org/entity/Q11573823', 'http://www.wikidata.org/entity/Q11574179', 'http://www.wikidata.org/entity/Q11574434', 'http://www.wikidata.org/entity/Q11574442', 'http://www.wikidata.org/entity/Q11574503', 'http://www.wikidata.org/entity/Q11574566', 'http://www.wikidata.org/entity/Q11574873', 'http://www.wikidata.org/entity/Q11576597', 'http://www.wikidata.org/entity/Q11577548', 'http://www.wikidata.org/entity/Q11577742', 'http://www.wikidata.org/entity/Q11578144', 'http://www.wikidata.org/entity/Q11578192', 'http://www.wikidata.org/entity/Q11578542', 'http://www.wikidata.org/entity/Q11579570', 'http://www.wikidata.org/entity/Q11580729', 'http://www.wikidata.org/entity/Q11580862', 'http://www.wikidata.org/entity/Q11580911', 'http://www.wikidata.org/entity/Q11581974', 'http://www.wikidata.org/entity/Q11581975', 'http://www.wikidata.org/entity/Q11583780', 'http://www.wikidata.org/entity/Q11583965', 'http://www.wikidata.org/entity/Q11588028', 'http://www.wikidata.org/entity/Q11588453', 'http://www.wikidata.org/entity/Q11589438', 'http://www.wikidata.org/entity/Q11589594', 'http://www.wikidata.org/entity/Q11591024', 'http://www.wikidata.org/entity/Q11592984', 'http://www.wikidata.org/entity/Q11596394', 'http://www.wikidata.org/entity/Q11598512', 'http://www.wikidata.org/entity/Q11598646', 'http://www.wikidata.org/entity/Q11598647', 'http://www.wikidata.org/entity/Q11599897', 'http://www.wikidata.org/entity/Q11602695', 'http://www.wikidata.org/entity/Q11603507', 'http://www.wikidata.org/entity/Q11603714', 'http://www.wikidata.org/entity/Q11604580', 'http://www.wikidata.org/entity/Q11604657', 'http://www.wikidata.org/entity/Q11605347', 'http://www.wikidata.org/entity/Q11607173', 'http://www.wikidata.org/entity/Q11610036', 'http://www.wikidata.org/entity/Q11612025', 'http://www.wikidata.org/entity/Q11613384', 'http://www.wikidata.org/entity/Q11614676', 'http://www.wikidata.org/entity/Q11616271', 'http://www.wikidata.org/entity/Q11622569', 'http://www.wikidata.org/entity/Q11625567', 'http://www.wikidata.org/entity/Q11626891', 'http://www.wikidata.org/entity/Q11630243', 'http://www.wikidata.org/entity/Q11631382', 'http://www.wikidata.org/entity/Q11633491', 'http://www.wikidata.org/entity/Q11633492', 'http://www.wikidata.org/entity/Q11634353', 'http://www.wikidata.org/entity/Q11635889', 'http://www.wikidata.org/entity/Q11636071', 'http://www.wikidata.org/entity/Q11636883', 'http://www.wikidata.org/entity/Q116373818', 'http://www.wikidata.org/entity/Q11645346', 'http://www.wikidata.org/entity/Q11645453', 'http://www.wikidata.org/entity/Q11647939', 'http://www.wikidata.org/entity/Q11648162', 'http://www.wikidata.org/entity/Q11648224', 'http://www.wikidata.org/entity/Q11650283', 'http://www.wikidata.org/entity/Q11650626', 'http://www.wikidata.org/entity/Q11652193', 'http://www.wikidata.org/entity/Q11652198', 'http://www.wikidata.org/entity/Q11652204', 'http://www.wikidata.org/entity/Q11652207', 'http://www.wikidata.org/entity/Q11655424', 'http://www.wikidata.org/entity/Q11657147', 'http://www.wikidata.org/entity/Q11657359', 'http://www.wikidata.org/entity/Q11659209', 'http://www.wikidata.org/entity/Q11661369', 'http://www.wikidata.org/entity/Q11661370', 'http://www.wikidata.org/entity/Q11661371', 'http://www.wikidata.org/entity/Q11661373', 'http://www.wikidata.org/entity/Q11662600', 'http://www.wikidata.org/entity/Q11664922', 'http://www.wikidata.org/entity/Q11664932', 'http://www.wikidata.org/entity/Q11665527', 'http://www.wikidata.org/entity/Q11665758', 'http://www.wikidata.org/entity/Q11665759', 'http://www.wikidata.org/entity/Q11667955', 'http://www.wikidata.org/entity/Q11667995', 'http://www.wikidata.org/entity/Q11668024', 'http://www.wikidata.org/entity/Q11668037', 'http://www.wikidata.org/entity/Q11668718', 'http://www.wikidata.org/entity/Q11669590', 'http://www.wikidata.org/entity/Q11669595', 'http://www.wikidata.org/entity/Q11669597', 'http://www.wikidata.org/entity/Q11669598', 'http://www.wikidata.org/entity/Q11669599', 'http://www.wikidata.org/entity/Q11669603', 'http://www.wikidata.org/entity/Q11669605', 'http://www.wikidata.org/entity/Q11670635', 'http://www.wikidata.org/entity/Q11673959', 'http://www.wikidata.org/entity/Q11674270', 'http://www.wikidata.org/entity/Q11675635', 'http://www.wikidata.org/entity/Q11675694', 'http://www.wikidata.org/entity/Q11675705', 'http://www.wikidata.org/entity/Q11675721', 'http://www.wikidata.org/entity/Q11675825', 'http://www.wikidata.org/entity/Q11676467', 'http://www.wikidata.org/entity/Q11677072', 'http://www.wikidata.org/entity/Q116774724', 'http://www.wikidata.org/entity/Q11678083', 'http://www.wikidata.org/entity/Q11678144', 'http://www.wikidata.org/entity/Q11678145', 'http://www.wikidata.org/entity/Q11678146', 'http://www.wikidata.org/entity/Q11678147', 'http://www.wikidata.org/entity/Q11678919', 'http://www.wikidata.org/entity/Q1204188', 'http://www.wikidata.org/entity/Q12122598', 'http://www.wikidata.org/entity/Q12168088', 'http://www.wikidata.org/entity/Q122792969', 'http://www.wikidata.org/entity/Q123092880', 'http://www.wikidata.org/entity/Q123554758', 'http://www.wikidata.org/entity/Q123554899', 'http://www.wikidata.org/entity/Q123563180', 'http://www.wikidata.org/entity/Q123568579', 'http://www.wikidata.org/entity/Q123592347', 'http://www.wikidata.org/entity/Q123592528', 'http://www.wikidata.org/entity/Q123630881', 'http://www.wikidata.org/entity/Q123631133', 'http://www.wikidata.org/entity/Q123848497', 'http://www.wikidata.org/entity/Q126617200', 'http://www.wikidata.org/entity/Q130120', 'http://www.wikidata.org/entity/Q130535', 'http://www.wikidata.org/entity/Q1344326', 'http://www.wikidata.org/entity/Q137962', 'http://www.wikidata.org/entity/Q13987', 'http://www.wikidata.org/entity/Q13991', 'http://www.wikidata.org/entity/Q1414691', 'http://www.wikidata.org/entity/Q145371', 'http://www.wikidata.org/entity/Q1475428', 'http://www.wikidata.org/entity/Q14948405', 'http://www.wikidata.org/entity/Q14948406', 'http://www.wikidata.org/entity/Q15231937', 'http://www.wikidata.org/entity/Q15233224', 'http://www.wikidata.org/entity/Q1532472', 'http://www.wikidata.org/entity/Q15914611', 'http://www.wikidata.org/entity/Q15914636', 'http://www.wikidata.org/entity/Q15914793', 'http://www.wikidata.org/entity/Q15914839', 'http://www.wikidata.org/entity/Q15914850', 'http://www.wikidata.org/entity/Q15914965', 'http://www.wikidata.org/entity/Q15915038', 'http://www.wikidata.org/entity/Q15915094', 'http://www.wikidata.org/entity/Q15915371', 'http://www.wikidata.org/entity/Q15915516', 'http://www.wikidata.org/entity/Q15915542', 'http://www.wikidata.org/entity/Q15915739', 'http://www.wikidata.org/entity/Q15915768', 'http://www.wikidata.org/entity/Q15915877', 'http://www.wikidata.org/entity/Q15915985', 'http://www.wikidata.org/entity/Q15916001', 'http://www.wikidata.org/entity/Q15916180', 'http://www.wikidata.org/entity/Q15916186', 'http://www.wikidata.org/entity/Q15916187', 'http://www.wikidata.org/entity/Q15916216', 'http://www.wikidata.org/entity/Q15916253', 'http://www.wikidata.org/entity/Q15916254', 'http://www.wikidata.org/entity/Q15916285', 'http://www.wikidata.org/entity/Q15916297', 'http://www.wikidata.org/entity/Q15916298', 'http://www.wikidata.org/entity/Q15916369', 'http://www.wikidata.org/entity/Q15916370', 'http://www.wikidata.org/entity/Q15916387', 'http://www.wikidata.org/entity/Q15916410', 'http://www.wikidata.org/entity/Q15916434', 'http://www.wikidata.org/entity/Q15916435', 'http://www.wikidata.org/entity/Q15916437', 'http://www.wikidata.org/entity/Q15916438', 'http://www.wikidata.org/entity/Q15916508', 'http://www.wikidata.org/entity/Q15923957', 'http://www.wikidata.org/entity/Q15924538', 'http://www.wikidata.org/entity/Q15925138', 'http://www.wikidata.org/entity/Q15925270', 'http://www.wikidata.org/entity/Q1676132', 'http://www.wikidata.org/entity/Q169589', 'http://www.wikidata.org/entity/Q17021654', 'http://www.wikidata.org/entity/Q17023687', 'http://www.wikidata.org/entity/Q17031459', 'http://www.wikidata.org/entity/Q17039990', 'http://www.wikidata.org/entity/Q17191315', 'http://www.wikidata.org/entity/Q17191378', 'http://www.wikidata.org/entity/Q17192049', 'http://www.wikidata.org/entity/Q17192826', 'http://www.wikidata.org/entity/Q17193690', 'http://www.wikidata.org/entity/Q17210135', 'http://www.wikidata.org/entity/Q17210185', 'http://www.wikidata.org/entity/Q17211889', 'http://www.wikidata.org/entity/Q17214084', 'http://www.wikidata.org/entity/Q17215469', 'http://www.wikidata.org/entity/Q17216064', 'http://www.wikidata.org/entity/Q17216375', 'http://www.wikidata.org/entity/Q17217423', 'http://www.wikidata.org/entity/Q17219919', 'http://www.wikidata.org/entity/Q17221048', 'http://www.wikidata.org/entity/Q17222656', 'http://www.wikidata.org/entity/Q17223389', 'http://www.wikidata.org/entity/Q17225029', 'http://www.wikidata.org/entity/Q17989148', 'http://www.wikidata.org/entity/Q17989626', 'http://www.wikidata.org/entity/Q17992764', 'http://www.wikidata.org/entity/Q17993734', 'http://www.wikidata.org/entity/Q17995776', 'http://www.wikidata.org/entity/Q18003098', 'http://www.wikidata.org/entity/Q18009413', 'http://www.wikidata.org/entity/Q18010599', 'http://www.wikidata.org/entity/Q1803811', 'http://www.wikidata.org/entity/Q18335728', 'http://www.wikidata.org/entity/Q18336591', 'http://www.wikidata.org/entity/Q18336657', 'http://www.wikidata.org/entity/Q18338827', 'http://www.wikidata.org/entity/Q18338974', 'http://www.wikidata.org/entity/Q18339013', 'http://www.wikidata.org/entity/Q18339157', 'http://www.wikidata.org/entity/Q18339362', 'http://www.wikidata.org/entity/Q18339537', 'http://www.wikidata.org/entity/Q18339548', 'http://www.wikidata.org/entity/Q18700735', 'http://www.wikidata.org/entity/Q187366', 'http://www.wikidata.org/entity/Q196701', 'http://www.wikidata.org/entity/Q19926707', 'http://www.wikidata.org/entity/Q19927579', 'http://www.wikidata.org/entity/Q19927913', 'http://www.wikidata.org/entity/Q19928028', 'http://www.wikidata.org/entity/Q1995509', 'http://www.wikidata.org/entity/Q19969455', 'http://www.wikidata.org/entity/Q19969456', 'http://www.wikidata.org/entity/Q19969457', 'http://www.wikidata.org/entity/Q19969459', 'http://www.wikidata.org/entity/Q19969461', 'http://www.wikidata.org/entity/Q19969462', 'http://www.wikidata.org/entity/Q19969463', 'http://www.wikidata.org/entity/Q20043639', 'http://www.wikidata.org/entity/Q20160219', 'http://www.wikidata.org/entity/Q2018422', 'http://www.wikidata.org/entity/Q20207875', 'http://www.wikidata.org/entity/Q20208336', 'http://www.wikidata.org/entity/Q20208605', 'http://www.wikidata.org/entity/Q20220282', 'http://www.wikidata.org/entity/Q20220291', 'http://www.wikidata.org/entity/Q20249559', 'http://www.wikidata.org/entity/Q20251315', 'http://www.wikidata.org/entity/Q20267482', 'http://www.wikidata.org/entity/Q20441459', 'http://www.wikidata.org/entity/Q20441495', 'http://www.wikidata.org/entity/Q20441538', 'http://www.wikidata.org/entity/Q20441672', 'http://www.wikidata.org/entity/Q20441835', 'http://www.wikidata.org/entity/Q20442833', 'http://www.wikidata.org/entity/Q20442886', 'http://www.wikidata.org/entity/Q20454159', 'http://www.wikidata.org/entity/Q20652984', 'http://www.wikidata.org/entity/Q20653009', 'http://www.wikidata.org/entity/Q20653020', 'http://www.wikidata.org/entity/Q20653048', 'http://www.wikidata.org/entity/Q20653083', 'http://www.wikidata.org/entity/Q20653128', 'http://www.wikidata.org/entity/Q20655767', 'http://www.wikidata.org/entity/Q20655779', 'http://www.wikidata.org/entity/Q20655824', 'http://www.wikidata.org/entity/Q20655829', 'http://www.wikidata.org/entity/Q20655854', 'http://www.wikidata.org/entity/Q20655861', 'http://www.wikidata.org/entity/Q20656218', 'http://www.wikidata.org/entity/Q20662194', 'http://www.wikidata.org/entity/Q20662421', 'http://www.wikidata.org/entity/Q20665543', 'http://www.wikidata.org/entity/Q20669152', 'http://www.wikidata.org/entity/Q20669173', 'http://www.wikidata.org/entity/Q20669188', 'http://www.wikidata.org/entity/Q20669201', 'http://www.wikidata.org/entity/Q20669474', 'http://www.wikidata.org/entity/Q20670485', 'http://www.wikidata.org/entity/Q20670486', 'http://www.wikidata.org/entity/Q20670489', 'http://www.wikidata.org/entity/Q20670490', 'http://www.wikidata.org/entity/Q20670802', 'http://www.wikidata.org/entity/Q20670818', 'http://www.wikidata.org/entity/Q20670842', 'http://www.wikidata.org/entity/Q20680346', 'http://www.wikidata.org/entity/Q20681784', 'http://www.wikidata.org/entity/Q20681836', 'http://www.wikidata.org/entity/Q20687296', 'http://www.wikidata.org/entity/Q20706572', 'http://www.wikidata.org/entity/Q20706579', 'http://www.wikidata.org/entity/Q20706699', 'http://www.wikidata.org/entity/Q20709285', 'http://www.wikidata.org/entity/Q2118388', 'http://www.wikidata.org/entity/Q21652956', 'http://www.wikidata.org/entity/Q21652975', 'http://www.wikidata.org/entity/Q21653337', 'http://www.wikidata.org/entity/Q21653909', 'http://www.wikidata.org/entity/Q21654565', 'http://www.wikidata.org/entity/Q2166413', 'http://www.wikidata.org/entity/Q220701', 'http://www.wikidata.org/entity/Q23069893', 'http://www.wikidata.org/entity/Q2407298', 'http://www.wikidata.org/entity/Q242176', 'http://www.wikidata.org/entity/Q24488445', 'http://www.wikidata.org/entity/Q247515', 'http://www.wikidata.org/entity/Q24871573', 'http://www.wikidata.org/entity/Q24872138', 'http://www.wikidata.org/entity/Q24875184', 'http://www.wikidata.org/entity/Q24898648', 'http://www.wikidata.org/entity/Q24902485', 'http://www.wikidata.org/entity/Q27560716', 'http://www.wikidata.org/entity/Q277035', 'http://www.wikidata.org/entity/Q28155659', 'http://www.wikidata.org/entity/Q285468', 'http://www.wikidata.org/entity/Q28682242', 'http://www.wikidata.org/entity/Q28682892', 'http://www.wikidata.org/entity/Q28682901', 'http://www.wikidata.org/entity/Q28683300', 'http://www.wikidata.org/entity/Q28684991', 'http://www.wikidata.org/entity/Q28684995', 'http://www.wikidata.org/entity/Q28687509', 'http://www.wikidata.org/entity/Q28687512', 'http://www.wikidata.org/entity/Q28687517', 'http://www.wikidata.org/entity/Q28687518', 'http://www.wikidata.org/entity/Q28687526', 'http://www.wikidata.org/entity/Q28687528', 'http://www.wikidata.org/entity/Q28687549', 'http://www.wikidata.org/entity/Q28687551', 'http://www.wikidata.org/entity/Q28687556', 'http://www.wikidata.org/entity/Q28687561', 'http://www.wikidata.org/entity/Q28687591', 'http://www.wikidata.org/entity/Q28693411', 'http://www.wikidata.org/entity/Q29980548', 'http://www.wikidata.org/entity/Q30925772', 'http://www.wikidata.org/entity/Q30925773', 'http://www.wikidata.org/entity/Q30931692', 'http://www.wikidata.org/entity/Q30931979', 'http://www.wikidata.org/entity/Q3108859', 'http://www.wikidata.org/entity/Q3199146', 'http://www.wikidata.org/entity/Q3285144', 'http://www.wikidata.org/entity/Q328533', 'http://www.wikidata.org/entity/Q3349795', 'http://www.wikidata.org/entity/Q339004', 'http://www.wikidata.org/entity/Q34783955', 'http://www.wikidata.org/entity/Q34783964', 'http://www.wikidata.org/entity/Q34783974', 'http://www.wikidata.org/entity/Q34784035', 'http://www.wikidata.org/entity/Q34784045', 'http://www.wikidata.org/entity/Q34784074', 'http://www.wikidata.org/entity/Q34784082', 'http://www.wikidata.org/entity/Q34784090', 'http://www.wikidata.org/entity/Q34784099', 'http://www.wikidata.org/entity/Q34784108', 'http://www.wikidata.org/entity/Q34784117', 'http://www.wikidata.org/entity/Q34784145', 'http://www.wikidata.org/entity/Q34784154', 'http://www.wikidata.org/entity/Q34784163', 'http://www.wikidata.org/entity/Q34784172', 'http://www.wikidata.org/entity/Q34784180', 'http://www.wikidata.org/entity/Q34784236', 'http://www.wikidata.org/entity/Q34784245', 'http://www.wikidata.org/entity/Q34784264', 'http://www.wikidata.org/entity/Q34784309', 'http://www.wikidata.org/entity/Q34784328', 'http://www.wikidata.org/entity/Q34784514', 'http://www.wikidata.org/entity/Q34785535', 'http://www.wikidata.org/entity/Q34785547', 'http://www.wikidata.org/entity/Q34787923', 'http://www.wikidata.org/entity/Q34787927', 'http://www.wikidata.org/entity/Q34787936', 'http://www.wikidata.org/entity/Q34787940', 'http://www.wikidata.org/entity/Q34787945', 'http://www.wikidata.org/entity/Q34787948', 'http://www.wikidata.org/entity/Q34787955', 'http://www.wikidata.org/entity/Q34787960', 'http://www.wikidata.org/entity/Q34787964', 'http://www.wikidata.org/entity/Q34787968', 'http://www.wikidata.org/entity/Q34787980', 'http://www.wikidata.org/entity/Q34787985', 'http://www.wikidata.org/entity/Q34788048', 'http://www.wikidata.org/entity/Q34788086', 'http://www.wikidata.org/entity/Q34788091', 'http://www.wikidata.org/entity/Q34788095', 'http://www.wikidata.org/entity/Q34788578', 'http://www.wikidata.org/entity/Q34788581', 'http://www.wikidata.org/entity/Q34788617', 'http://www.wikidata.org/entity/Q34788621', 'http://www.wikidata.org/entity/Q34788699', 'http://www.wikidata.org/entity/Q34795633', 'http://www.wikidata.org/entity/Q34795652', 'http://www.wikidata.org/entity/Q34795659', 'http://www.wikidata.org/entity/Q34795671', 'http://www.wikidata.org/entity/Q34795678', 'http://www.wikidata.org/entity/Q34795686', 'http://www.wikidata.org/entity/Q34795693', 'http://www.wikidata.org/entity/Q34795722', 'http://www.wikidata.org/entity/Q34795734', 'http://www.wikidata.org/entity/Q34795744', 'http://www.wikidata.org/entity/Q34795753', 'http://www.wikidata.org/entity/Q34795770', 'http://www.wikidata.org/entity/Q34795778', 'http://www.wikidata.org/entity/Q34795788', 'http://www.wikidata.org/entity/Q34795804', 'http://www.wikidata.org/entity/Q34795808', 'http://www.wikidata.org/entity/Q34795832', 'http://www.wikidata.org/entity/Q34795844', 'http://www.wikidata.org/entity/Q34795856', 'http://www.wikidata.org/entity/Q34795867', 'http://www.wikidata.org/entity/Q34795874', 'http://www.wikidata.org/entity/Q34795887', 'http://www.wikidata.org/entity/Q34795901', 'http://www.wikidata.org/entity/Q34795907', 'http://www.wikidata.org/entity/Q34795913', 'http://www.wikidata.org/entity/Q34795937', 'http://www.wikidata.org/entity/Q34795942', 'http://www.wikidata.org/entity/Q34795954', 'http://www.wikidata.org/entity/Q34795961', 'http://www.wikidata.org/entity/Q34795967', 'http://www.wikidata.org/entity/Q34795972', 'http://www.wikidata.org/entity/Q34795984', 'http://www.wikidata.org/entity/Q34795990', 'http://www.wikidata.org/entity/Q34795996', 'http://www.wikidata.org/entity/Q34796002', 'http://www.wikidata.org/entity/Q34796008', 'http://www.wikidata.org/entity/Q34796015', 'http://www.wikidata.org/entity/Q34796021', 'http://www.wikidata.org/entity/Q34796028', 'http://www.wikidata.org/entity/Q34796033', 'http://www.wikidata.org/entity/Q34796043', 'http://www.wikidata.org/entity/Q34796055', 'http://www.wikidata.org/entity/Q34796071', 'http://www.wikidata.org/entity/Q34796095', 'http://www.wikidata.org/entity/Q34796102', 'http://www.wikidata.org/entity/Q34796119', 'http://www.wikidata.org/entity/Q34796134', 'http://www.wikidata.org/entity/Q34796146', 'http://www.wikidata.org/entity/Q34796151', 'http://www.wikidata.org/entity/Q34796158', 'http://www.wikidata.org/entity/Q34796163', 'http://www.wikidata.org/entity/Q34796170', 'http://www.wikidata.org/entity/Q34796175', 'http://www.wikidata.org/entity/Q34796180', 'http://www.wikidata.org/entity/Q34861379', 'http://www.wikidata.org/entity/Q34861390', 'http://www.wikidata.org/entity/Q34861523', 'http://www.wikidata.org/entity/Q34861562', 'http://www.wikidata.org/entity/Q34861821', 'http://www.wikidata.org/entity/Q34862653', 'http://www.wikidata.org/entity/Q3579074', 'http://www.wikidata.org/entity/Q3594049', 'http://www.wikidata.org/entity/Q3623017', 'http://www.wikidata.org/entity/Q3785700', 'http://www.wikidata.org/entity/Q382082', 'http://www.wikidata.org/entity/Q38266996', 'http://www.wikidata.org/entity/Q385313', 'http://www.wikidata.org/entity/Q385710', 'http://www.wikidata.org/entity/Q393031', 'http://www.wikidata.org/entity/Q398636', 'http://www.wikidata.org/entity/Q432124', 'http://www.wikidata.org/entity/Q4419675', 'http://www.wikidata.org/entity/Q4419682', 'http://www.wikidata.org/entity/Q4478859', 'http://www.wikidata.org/entity/Q4497854', 'http://www.wikidata.org/entity/Q4518163', 'http://www.wikidata.org/entity/Q4518364', 'http://www.wikidata.org/entity/Q4518483', 'http://www.wikidata.org/entity/Q4518560', 'http://www.wikidata.org/entity/Q4518632', 'http://www.wikidata.org/entity/Q4518662', 'http://www.wikidata.org/entity/Q4518698', 'http://www.wikidata.org/entity/Q4518728', 'http://www.wikidata.org/entity/Q4518764', 'http://www.wikidata.org/entity/Q4518813', 'http://www.wikidata.org/entity/Q4518835', 'http://www.wikidata.org/entity/Q4518882', 'http://www.wikidata.org/entity/Q4518914', 'http://www.wikidata.org/entity/Q4518946', 'http://www.wikidata.org/entity/Q4519060', 'http://www.wikidata.org/entity/Q4519100', 'http://www.wikidata.org/entity/Q4519127', 'http://www.wikidata.org/entity/Q4519202', 'http://www.wikidata.org/entity/Q4519334', 'http://www.wikidata.org/entity/Q4519416', 'http://www.wikidata.org/entity/Q4519472', 'http://www.wikidata.org/entity/Q4520401', 'http://www.wikidata.org/entity/Q4520501', 'http://www.wikidata.org/entity/Q4520623', 'http://www.wikidata.org/entity/Q4520676', 'http://www.wikidata.org/entity/Q4520740', 'http://www.wikidata.org/entity/Q473472', 'http://www.wikidata.org/entity/Q474560', 'http://www.wikidata.org/entity/Q48752569', 'http://www.wikidata.org/entity/Q48752621', 'http://www.wikidata.org/entity/Q490610', 'http://www.wikidata.org/entity/Q49333374', 'http://www.wikidata.org/entity/Q494914', 'http://www.wikidata.org/entity/Q49493', 'http://www.wikidata.org/entity/Q49500', 'http://www.wikidata.org/entity/Q49507', 'http://www.wikidata.org/entity/Q49511', 'http://www.wikidata.org/entity/Q49513', 'http://www.wikidata.org/entity/Q49631357', 'http://www.wikidata.org/entity/Q49631388', 'http://www.wikidata.org/entity/Q49631402', 'http://www.wikidata.org/entity/Q49631408', 'http://www.wikidata.org/entity/Q49631415', 'http://www.wikidata.org/entity/Q49631418', 'http://www.wikidata.org/entity/Q49631448', 'http://www.wikidata.org/entity/Q49631449', 'http://www.wikidata.org/entity/Q49631468', 'http://www.wikidata.org/entity/Q49631471', 'http://www.wikidata.org/entity/Q49631484', 'http://www.wikidata.org/entity/Q49631487', 'http://www.wikidata.org/entity/Q49631489', 'http://www.wikidata.org/entity/Q49631490', 'http://www.wikidata.org/entity/Q49631492', 'http://www.wikidata.org/entity/Q49631493', 'http://www.wikidata.org/entity/Q49631495', 'http://www.wikidata.org/entity/Q49631497', 'http://www.wikidata.org/entity/Q49631501', 'http://www.wikidata.org/entity/Q49631532', 'http://www.wikidata.org/entity/Q49631657', 'http://www.wikidata.org/entity/Q49631707', 'http://www.wikidata.org/entity/Q49631712', 'http://www.wikidata.org/entity/Q49631766', 'http://www.wikidata.org/entity/Q49631801', 'http://www.wikidata.org/entity/Q49631841', 'http://www.wikidata.org/entity/Q49631849', 'http://www.wikidata.org/entity/Q49631851', 'http://www.wikidata.org/entity/Q49631852', 'http://www.wikidata.org/entity/Q49631855', 'http://www.wikidata.org/entity/Q49631874', 'http://www.wikidata.org/entity/Q49631881', 'http://www.wikidata.org/entity/Q49631883', </t>
         </is>
       </c>
       <c r="D15" t="b">
@@ -738,17 +738,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>What was the first Queen album?</t>
+          <t>Who developed the video game World of Warcraft?</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q193490']</t>
+          <t>['http://www.wikidata.org/entity/Q178824']</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q193490']</t>
+          <t>['http://www.wikidata.org/entity/Q178824']</t>
         </is>
       </c>
       <c r="D16" t="b">
@@ -758,17 +758,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>What is the currency of the Czech Republic?</t>
+          <t>Where was JFK assassinated?</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q131016']</t>
+          <t>['http://www.wikidata.org/entity/Q3896131']</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q131016']</t>
+          <t>['http://www.wikidata.org/entity/Q3896131']</t>
         </is>
       </c>
       <c r="D17" t="b">
@@ -778,17 +778,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>In which films did Julia Roberts as well as Richard Gere play?</t>
+          <t>Which river does the Brooklyn Bridge cross?</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q1160813', 'http://www.wikidata.org/entity/Q207954']</t>
+          <t>['http://www.wikidata.org/entity/Q212862']</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q1160813', 'http://www.wikidata.org/entity/Q207954']</t>
+          <t>['http://www.wikidata.org/entity/Q212862']</t>
         </is>
       </c>
       <c r="D18" t="b">
@@ -798,57 +798,57 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>What is the capital of Canada?</t>
+          <t>How many children did Benjamin Franklin have?</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q1930']</t>
+          <t>['3']</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q3876']</t>
+          <t>['3']</t>
         </is>
       </c>
       <c r="D19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Who created Family Guy?</t>
+          <t>how much is the elevation of Düsseldorf Airport ?</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q188492']</t>
+          <t>['147']</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/statement/q5930-1f0cd544-41d4-4bc1-1b53-8c9766759dc6']</t>
+          <t>['147']</t>
         </is>
       </c>
       <c r="D20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>How much is the population of mexico city ?</t>
+          <t>In which country is Mecca located?</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>['9209944']</t>
+          <t>['http://www.wikidata.org/entity/Q851']</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>['9209944']</t>
+          <t>['http://www.wikidata.org/entity/Q851']</t>
         </is>
       </c>
       <c r="D21" t="b">
@@ -858,17 +858,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Who created Batman?</t>
+          <t>How tall is Claudia Schiffer?</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q313048', 'http://www.wikidata.org/entity/Q464282']</t>
+          <t>['180']</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q313048', 'http://www.wikidata.org/entity/Q464282']</t>
+          <t>['180']</t>
         </is>
       </c>
       <c r="D22" t="b">
@@ -878,41 +878,401 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>To which countries does the Himalayan mountain system extend?</t>
+          <t>What kind of music did Lou Reed play?</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q148', 'http://www.wikidata.org/entity/Q668', 'http://www.wikidata.org/entity/Q836', 'http://www.wikidata.org/entity/Q837', 'http://www.wikidata.org/entity/Q843', 'http://www.wikidata.org/entity/Q889', 'http://www.wikidata.org/entity/Q917']</t>
+          <t>['http://www.wikidata.org/entity/Q11366', 'http://www.wikidata.org/entity/Q11399', 'http://www.wikidata.org/entity/Q1428637', 'http://www.wikidata.org/entity/Q1641839', 'http://www.wikidata.org/entity/Q181861', 'http://www.wikidata.org/entity/Q186472', 'http://www.wikidata.org/entity/Q206159', 'http://www.wikidata.org/entity/Q217467', 'http://www.wikidata.org/entity/Q27190', 'http://www.wikidata.org/entity/Q650316', 'http://www.wikidata.org/entity/Q76092', 'http://www.wikidata.org/entity/Q885561']</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q148', 'http://www.wikidata.org/entity/Q252', 'http://www.wikidata.org/entity/Q668', 'http://www.wikidata.org/entity/Q836', 'http://www.wikidata.org/entity/Q837', 'http://www.wikidata.org/entity/Q843', 'http://www.wikidata.org/entity/Q889', 'http://www.wikidata.org/entity/Q917']</t>
+          <t>['http://www.wikidata.org/entity/Q11366', 'http://www.wikidata.org/entity/Q11399', 'http://www.wikidata.org/entity/Q1428637', 'http://www.wikidata.org/entity/Q1641839', 'http://www.wikidata.org/entity/Q181861', 'http://www.wikidata.org/entity/Q186472', 'http://www.wikidata.org/entity/Q206159', 'http://www.wikidata.org/entity/Q217467', 'http://www.wikidata.org/entity/Q27190', 'http://www.wikidata.org/entity/Q650316', 'http://www.wikidata.org/entity/Q76092', 'http://www.wikidata.org/entity/Q885561']</t>
         </is>
       </c>
       <c r="D23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Who created Goofy?</t>
+          <t>Give me the birth place of Frank Sinatra.</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q2420722']</t>
+          <t>['http://www.wikidata.org/entity/Q138578']</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>['http://www.wikidata.org/entity/Q2420722']</t>
+          <t>['http://www.wikidata.org/entity/Q138578']</t>
         </is>
       </c>
       <c r="D24" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Give me all Swedish holidays.</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q1348730', 'http://www.wikidata.org/entity/Q39864', 'http://www.wikidata.org/entity/Q40317']</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q10541207', 'http://www.wikidata.org/entity/Q10685840', 'http://www.wikidata.org/entity/Q10689144', 'http://www.wikidata.org/entity/Q124498859', 'http://www.wikidata.org/entity/Q1661478', 'http://www.wikidata.org/entity/Q19978123', 'http://www.wikidata.org/entity/Q200982', 'http://www.wikidata.org/entity/Q3013206', 'http://www.wikidata.org/entity/Q883628']</t>
+        </is>
+      </c>
+      <c r="D25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Where did Abraham Lincoln die?</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q4799733']</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/statement/Q91-40962CC7-37A3-43CC-A010-B910CF7B73AB', 'http://www.wikidata.org/entity/statement/q91-F8A39865-BC06-4C48-A8BB-996B8E786EA0']</t>
+        </is>
+      </c>
+      <c r="D26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Give me the capitals of all countries that the Himalayas run through.</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q1362', 'http://www.wikidata.org/entity/Q3037', 'http://www.wikidata.org/entity/Q37400', 'http://www.wikidata.org/entity/Q5838', 'http://www.wikidata.org/entity/Q9270', 'http://www.wikidata.org/entity/Q956', 'http://www.wikidata.org/entity/Q987']</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q1362', 'http://www.wikidata.org/entity/Q3037', 'http://www.wikidata.org/entity/Q37400', 'http://www.wikidata.org/entity/Q5838', 'http://www.wikidata.org/entity/Q9270', 'http://www.wikidata.org/entity/Q956', 'http://www.wikidata.org/entity/Q987']</t>
+        </is>
+      </c>
+      <c r="D27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>In which country is the Limerick Lake?</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q16']</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q16']</t>
+        </is>
+      </c>
+      <c r="D28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>In which countries can you pay using the West African CFA franc?</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q1007', 'http://www.wikidata.org/entity/Q1008', 'http://www.wikidata.org/entity/Q1032', 'http://www.wikidata.org/entity/Q1041', 'http://www.wikidata.org/entity/Q18408563', 'http://www.wikidata.org/entity/Q1929699', 'http://www.wikidata.org/entity/Q2386787', 'http://www.wikidata.org/entity/Q5148343', 'http://www.wikidata.org/entity/Q5148520', 'http://www.wikidata.org/entity/Q620942', 'http://www.wikidata.org/entity/Q862701', 'http://www.wikidata.org/entity/Q912', 'http://www.wikidata.org/entity/Q945', 'http://www.wikidata.org/entity/Q962', 'http://www.wikidata.org/entity/Q965']</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q1007', 'http://www.wikidata.org/entity/Q1008', 'http://www.wikidata.org/entity/Q1032', 'http://www.wikidata.org/entity/Q1041', 'http://www.wikidata.org/entity/Q18408563', 'http://www.wikidata.org/entity/Q1929699', 'http://www.wikidata.org/entity/Q2386787', 'http://www.wikidata.org/entity/Q5148343', 'http://www.wikidata.org/entity/Q5148520', 'http://www.wikidata.org/entity/Q620942', 'http://www.wikidata.org/entity/Q862701', 'http://www.wikidata.org/entity/Q912', 'http://www.wikidata.org/entity/Q945', 'http://www.wikidata.org/entity/Q962', 'http://www.wikidata.org/entity/Q965']</t>
+        </is>
+      </c>
+      <c r="D29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Which holidays are celebrated around the world?</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q103987830', 'http://www.wikidata.org/entity/Q104013369', 'http://www.wikidata.org/entity/Q116978631', 'http://www.wikidata.org/entity/Q21163268', 'http://www.wikidata.org/entity/Q10283187', 'http://www.wikidata.org/entity/Q111738564', 'http://www.wikidata.org/entity/Q112127159', 'http://www.wikidata.org/entity/Q124422802', 'http://www.wikidata.org/entity/Q18465013', 'http://www.wikidata.org/entity/Q125856465', 'http://www.wikidata.org/entity/Q1361434', 'http://www.wikidata.org/entity/Q1651570', 'http://www.wikidata.org/entity/Q2564633', 'http://www.wikidata.org/entity/Q333016', 'http://www.wikidata.org/entity/Q61359735', 'http://www.wikidata.org/entity/Q72318', 'http://www.wikidata.org/entity/Q744159', 'http://www.wikidata.org/entity/Q751738', 'http://www.wikidata.org/entity/Q110707177', 'http://www.wikidata.org/entity/Q45922130', 'http://www.wikidata.org/entity/Q57350935', 'http://www.wikidata.org/entity/Q57397044', 'http://www.wikidata.org/entity/Q116978568', 'http://www.wikidata.org/entity/Q2859605', 'http://www.wikidata.org/entity/Q113090457', 'http://www.wikidata.org/entity/Q115181793', 'http://www.wikidata.org/entity/Q115369110', 'http://www.wikidata.org/entity/Q115369980', 'http://www.wikidata.org/entity/Q115377287', 'http://www.wikidata.org/entity/Q21697589', 'http://www.wikidata.org/entity/Q122069654', 'http://www.wikidata.org/entity/Q1145566', 'http://www.wikidata.org/entity/Q11406184', 'http://www.wikidata.org/entity/Q11643728', 'http://www.wikidata.org/entity/Q20044441', 'http://www.wikidata.org/entity/Q28685931', 'http://www.wikidata.org/entity/Q11255045', 'http://www.wikidata.org/entity/Q11387821', 'http://www.wikidata.org/entity/Q11436695', 'http://www.wikidata.org/entity/Q11501518', 'http://www.wikidata.org/entity/Q11502138', 'http://www.wikidata.org/entity/Q11512398', 'http://www.wikidata.org/entity/Q11590440', 'http://www.wikidata.org/entity/Q11604982', 'http://www.wikidata.org/entity/Q6455253', 'http://www.wikidata.org/entity/Q111162467', 'http://www.wikidata.org/entity/Q124005660', 'http://www.wikidata.org/entity/Q130611902', 'http://www.wikidata.org/entity/Q13258770', 'http://www.wikidata.org/entity/Q2838743', 'http://www.wikidata.org/entity/Q3092925', 'http://www.wikidata.org/entity/Q123004384', 'http://www.wikidata.org/entity/Q4546230', 'http://www.wikidata.org/entity/Q1009535', 'http://www.wikidata.org/entity/Q1049141', 'http://www.wikidata.org/entity/Q1059995', 'http://www.wikidata.org/entity/Q1137351', 'http://www.wikidata.org/entity/Q1145630', 'http://www.wikidata.org/entity/Q1186410', 'http://www.wikidata.org/entity/Q1355051', 'http://www.wikidata.org/entity/Q1355833', 'http://www.wikidata.org/entity/Q1359602', 'http://www.wikidata.org/entity/Q1361434', 'http://www.wikidata.org/entity/Q1361489', 'http://www.wikidata.org/entity/Q17218111', 'http://www.wikidata.org/entity/Q483226', 'http://www.wikidata.org/entity/Q82405', 'http://www.wikidata.org/entity/Q101706322', 'http://www.wikidata.org/entity/Q10265921', 'http://www.wikidata.org/entity/Q10274', 'http://www.wikidata.org/entity/Q10281751', 'http://www.wikidata.org/entity/Q10313072', 'http://www.wikidata.org/entity/Q1034573', 'http://www.wikidata.org/entity/Q10379695', 'http://www.wikidata.org/entity/Q1038328', 'http://www.wikidata.org/entity/Q104842151', 'http://www.wikidata.org/entity/Q104842171', 'http://www.wikidata.org/entity/Q104844735', 'http://www.wikidata.org/entity/Q104853673', 'http://www.wikidata.org/entity/Q104861126', 'http://www.wikidata.org/entity/Q10488275', 'http://www.wikidata.org/entity/Q105047091', 'http://www.wikidata.org/entity/Q105047582', 'http://www.wikidata.org/entity/Q105047587', 'http://www.wikidata.org/entity/Q105271464', 'http://www.wikidata.org/entity/Q105393636', 'http://www.wikidata.org/entity/Q10560877', 'http://www.wikidata.org/entity/Q105742385', 'http://www.wikidata.org/entity/Q105742388', 'http://www.wikidata.org/entity/Q1058840', 'http://www.wikidata.org/entity/Q106010', 'http://www.wikidata.org/entity/Q106290028', 'http://www.wikidata.org/entity/Q106307776', 'http://www.wikidata.org/entity/Q106806190', 'http://www.wikidata.org/entity/Q106855753', 'http://www.wikidata.org/entity/Q1070437', 'http://www.wikidata.org/entity/Q107139413', 'http://www.wikidata.org/entity/Q10726425', 'http://www.wikidata.org/entity/Q107486932', 'http://www.wikidata.org/entity/Q107643630', 'http://www.wikidata.org/entity/Q108120675', 'http://www.wikidata.org/entity/Q108265918', 'http://www.wikidata.org/entity/Q108305674', 'http://www.wikidata.org/entity/Q108456662', 'http://www.wikidata.org/entity/Q108540687', 'http://www.wikidata.org/entity/Q10862448', 'http://www.wikidata.org/entity/Q108745010', 'http://www.wikidata.org/entity/Q10881633', 'http://www.wikidata.org/entity/Q108936865', 'http://www.wikidata.org/entity/Q10901070', 'http://www.wikidata.org/entity/Q109040869', 'http://www.wikidata.org/entity/Q10921475', 'http://www.wikidata.org/entity/Q109356066', 'http://www.wikidata.org/entity/Q109609391', 'http://www.wikidata.org/entity/Q109796906', 'http://www.wikidata.org/entity/Q110239836', 'http://www.wikidata.org/entity/Q1105149', 'http://www.wikidata.org/entity/Q110712627', 'http://www.wikidata.org/entity/Q110738072', 'http://www.wikidata.org/entity/Q110804043', 'http://www.wikidata.org/entity/Q11095193', 'http://www.wikidata.org/entity/Q11156396', 'http://www.wikidata.org/entity/Q11156590', 'http://www.wikidata.org/entity/Q11156602', 'http://www.wikidata.org/entity/Q111585601', 'http://www.wikidata.org/entity/Q111586257', 'http://www.wikidata.org/entity/Q111588212', 'http://www.wikidata.org/entity/Q111588631', 'http://www.wikidata.org/entity/Q111591927', 'http://www.wikidata.org/entity/Q111592030', 'http://www.wikidata.org/entity/Q111592221', 'http://www.wikidata.org/entity/Q111592231', 'http://www.wikidata.org/entity/Q111592392', 'http://www.wikidata.org/entity/Q111593121', 'http://www.wikidata.org/entity/Q111599061', 'http://www.wikidata.org/entity/Q111605534', 'http://www.wikidata.org/entity/Q111605672', 'http://www.wikidata.org/entity/Q111605780', 'http://www.wikidata.org/entity/Q111619857', 'http://www.wikidata.org/entity/Q111621136', 'http://www.wikidata.org/entity/Q111639188', 'http://www.wikidata.org/entity/Q111639464', 'http://www.wikidata.org/entity/Q111639796', 'http://www.wikidata.org/entity/Q111640394', 'http://www.wikidata.org/entity/Q111644691', 'http://www.wikidata.org/entity/Q111644855', 'http://www.wikidata.org/entity/Q111646483', 'http://www.wikidata.org/entity/Q111646603', 'http://www.wikidata.org/entity/Q111646902', 'http://www.wikidata.org/entity/Q111646942', 'http://www.wikidata.org/entity/Q111647178', 'http://www.wikidata.org/entity/Q111647244', 'http://www.wikidata.org/entity/Q111648147', 'http://www.wikidata.org/entity/Q111648327', 'http://www.wikidata.org/entity/Q111648357', 'http://www.wikidata.org/entity/Q111649590', 'http://www.wikidata.org/entity/Q111649647', 'http://www.wikidata.org/entity/Q111649691', 'http://www.wikidata.org/entity/Q111649919', 'http://www.wikidata.org/entity/Q111653594', 'http://www.wikidata.org/entity/Q111653613', 'http://www.wikidata.org/entity/Q111653631', 'http://www.wikidata.org/entity/Q111653637', 'http://www.wikidata.org/entity/Q111653675', 'http://www.wikidata.org/entity/Q111653779', 'http://www.wikidata.org/entity/Q111653938', 'http://www.wikidata.org/entity/Q111653958', 'http://www.wikidata.org/entity/Q111653969', 'http://www.wikidata.org/entity/Q111654007', 'http://www.wikidata.org/entity/Q111654040', 'http://www.wikidata.org/entity/Q111654093', 'http://www.wikidata.org/entity/Q111654098', 'http://www.wikidata.org/entity/Q111654121', 'http://www.wikidata.org/entity/Q111654136', 'http://www.wikidata.org/entity/Q111654241', 'http://www.wikidata.org/entity/Q111654346', 'http://www.wikidata.org/entity/Q111654469', 'http://www.wikidata.org/entity/Q111654484', 'http://www.wikidata.org/entity/Q111658731', 'http://www.wikidata.org/entity/Q111658801', 'http://www.wikidata.org/entity/Q111658833', 'http://www.wikidata.org/entity/Q111658927', 'http://www.wikidata.org/entity/Q111661297', 'http://www.wikidata.org/entity/Q111661840', 'http://www.wikidata.org/entity/Q111661872', 'http://www.wikidata.org/entity/Q111661886', 'http://www.wikidata.org/entity/Q111662034', 'http://www.wikidata.org/entity/Q111662035', 'http://www.wikidata.org/entity/Q111662040', 'http://www.wikidata.org/entity/Q111662133', 'http://www.wikidata.org/entity/Q111663221', 'http://www.wikidata.org/entity/Q111665328', 'http://www.wikidata.org/entity/Q111665519', 'http://www.wikidata.org/entity/Q111666301', 'http://www.wikidata.org/entity/Q111670117', 'http://www.wikidata.org/entity/Q111670231', 'http://www.wikidata.org/entity/Q111670397', 'http://www.wikidata.org/entity/Q111670481', 'http://www.wikidata.org/entity/Q111670617', 'http://www.wikidata.org/entity/Q111670624', 'http://www.wikidata.org/entity/Q111670628', 'http://www.wikidata.org/entity/Q111671698', 'http://www.wikidata.org/entity/Q111671968', 'http://www.wikidata.org/entity/Q111672442', 'http://www.wikidata.org/entity/Q111675204', 'http://www.wikidata.org/entity/Q111675217', 'http://www.wikidata.org/entity/Q111675293', 'http://www.wikidata.org/entity/Q111675405', 'http://www.wikidata.org/entity/Q111675518', 'http://www.wikidata.org/entity/Q111675816', 'http://www.wikidata.org/entity/Q111676530', 'http://www.wikidata.org/entity/Q111676789', 'http://www.wikidata.org/entity/Q111676828', 'http://www.wikidata.org/entity/Q111676959', 'http://www.wikidata.org/entity/Q111679720', 'http://www.wikidata.org/entity/Q111679753', 'http://www.wikidata.org/entity/Q111679830', 'http://www.wikidata.org/entity/Q111679840', 'http://www.wikidata.org/entity/Q111679871', 'http://www.wikidata.org/entity/Q111679978', 'http://www.wikidata.org/entity/Q111680097', 'http://www.wikidata.org/entity/Q111680142', 'http://www.wikidata.org/entity/Q111680149', 'http://www.wikidata.org/entity/Q111680197', 'http://www.wikidata.org/entity/Q111680221', 'http://www.wikidata.org/entity/Q111680229', 'http://www.wikidata.org/entity/Q111693657', 'http://www.wikidata.org/entity/Q111693675', 'http://www.wikidata.org/entity/Q111693696', 'http://www.wikidata.org/entity/Q111693773', 'http://www.wikidata.org/entity/Q111693781', 'http://www.wikidata.org/entity/Q111693947', 'http://www.wikidata.org/entity/Q111694017', 'http://www.wikidata.org/entity/Q111695525', 'http://www.wikidata.org/entity/Q111702011', 'http://www.wikidata.org/entity/Q111702051', 'http://www.wikidata.org/entity/Q111702063', 'http://www.wikidata.org/entity/Q111705727', 'http://www.wikidata.org/entity/Q111708136', 'http://www.wikidata.org/entity/Q111711151', 'http://www.wikidata.org/entity/Q111711160', 'http://www.wikidata.org/entity/Q111711162', 'http://www.wikidata.org/entity/Q111711184', 'http://www.wikidata.org/entity/Q111711264', 'http://www.wikidata.org/entity/Q111711268', 'http://www.wikidata.org/entity/Q111711270', 'http://www.wikidata.org/entity/Q111711273', 'http://www.wikidata.org/entity/Q111711278', 'http://www.wikidata.org/entity/Q111711311', 'http://www.wikidata.org/entity/Q111711342', 'http://www.wikidata.org/entity/Q111711421', 'http://www.wikidata.org/entity/Q111711540', 'http://www.wikidata.org/entity/Q111711547', 'http://www.wikidata.org/entity/Q111711661', 'http://www.wikidata.org/entity/Q111711757', 'http://www.wikidata.org/entity/Q111711903', 'http://www.wikidata.org/entity/Q111711907', 'http://www.wikidata.org/entity/Q111712005', 'http://www.wikidata.org/entity/Q111712010', 'http://www.wikidata.org/entity/Q111712059', 'http://www.wikidata.org/entity/Q111712123', 'http://www.wikidata.org/entity/Q111716408', 'http://www.wikidata.org/entity/Q111719293', 'http://www.wikidata.org/entity/Q111725575', 'http://www.wikidata.org/entity/Q111725911', 'http://www.wikidata.org/entity/Q111726390', 'http://www.wikidata.org/entity/Q111726615', 'http://www.wikidata.org/entity/Q111726617', 'http://www.wikidata.org/entity/Q111726635', 'http://www.wikidata.org/entity/Q111726669', 'http://www.wikidata.org/entity/Q111726714', 'http://www.wikidata.org/entity/Q111726768', 'http://www.wikidata.org/entity/Q111726774', 'http://www.wikidata.org/entity/Q111726793', 'http://www.wikidata.org/entity/Q111726805', 'http://www.wikidata.org/entity/Q111734330', 'http://www.wikidata.org/entity/Q111734453', 'http://www.wikidata.org/entity/Q111734646', 'http://www.wikidata.org/entity/Q111734661', 'http://www.wikidata.org/entity/Q111734681', 'http://www.wikidata.org/entity/Q111734708', 'http://www.wikidata.org/entity/Q111734879', 'http://www.wikidata.org/entity/Q111734906', 'http://www.wikidata.org/entity/Q111734910', 'http://www.wikidata.org/entity/Q111734978', 'http://www.wikidata.org/entity/Q111735009', 'http://www.wikidata.org/entity/Q111735146', 'http://www.wikidata.org/entity/Q111735183', 'http://www.wikidata.org/entity/Q111735311', 'http://www.wikidata.org/entity/Q111738073', 'http://www.wikidata.org/entity/Q111738552', 'http://www.wikidata.org/entity/Q111738762', 'http://www.wikidata.org/entity/Q111738881', 'http://www.wikidata.org/entity/Q111743473', 'http://www.wikidata.org/entity/Q111743614', 'http://www.wikidata.org/entity/Q111743635', 'http://www.wikidata.org/entity/Q111743658', 'http://www.wikidata.org/entity/Q111743894', 'http://www.wikidata.org/entity/Q111743903', 'http://www.wikidata.org/entity/Q111743905', 'http://www.wikidata.org/entity/Q111743922', 'http://www.wikidata.org/entity/Q111744105', 'http://www.wikidata.org/entity/Q111744185', 'http://www.wikidata.org/entity/Q111744196', 'http://www.wikidata.org/entity/Q111744206', 'http://www.wikidata.org/entity/Q111744231', 'http://www.wikidata.org/entity/Q111744233', 'http://www.wikidata.org/entity/Q111744287', 'http://www.wikidata.org/entity/Q111750057', 'http://www.wikidata.org/entity/Q111750098', 'http://www.wikidata.org/entity/Q111750104', 'http://www.wikidata.org/entity/Q111750108', 'http://www.wikidata.org/entity/Q111750391', 'http://www.wikidata.org/entity/Q111750396', 'http://www.wikidata.org/entity/Q111750414', 'http://www.wikidata.org/entity/Q111750482', 'http://www.wikidata.org/entity/Q111750486', 'http://www.wikidata.org/entity/Q111750538', 'http://www.wikidata.org/entity/Q111750619', 'http://www.wikidata.org/entity/Q111750632', 'http://www.wikidata.org/entity/Q111750636', 'http://www.wikidata.org/entity/Q111750803', 'http://www.wikidata.org/entity/Q111772339', 'http://www.wikidata.org/entity/Q111772429', 'http://www.wikidata.org/entity/Q111772455', 'http://www.wikidata.org/entity/Q111772465', 'http://www.wikidata.org/entity/Q111772467', 'http://www.wikidata.org/entity/Q111772470', 'http://www.wikidata.org/entity/Q111772479', 'http://www.wikidata.org/entity/Q111772481', 'http://www.wikidata.org/entity/Q111772492', 'http://www.wikidata.org/entity/Q111772538', 'http://www.wikidata.org/entity/Q111772542', 'http://www.wikidata.org/entity/Q111772579', 'http://www.wikidata.org/entity/Q111772903', 'http://www.wikidata.org/entity/Q111774488', 'http://www.wikidata.org/entity/Q111774855', 'http://www.wikidata.org/entity/Q111775976', 'http://www.wikidata.org/entity/Q111781307', 'http://www.wikidata.org/entity/Q111781313', 'http://www.wikidata.org/entity/Q111781415', 'http://www.wikidata.org/entity/Q111782305', 'http://www.wikidata.org/entity/Q111782406', 'http://www.wikidata.org/entity/Q111792237', 'http://www.wikidata.org/entity/Q111792287', 'http://www.wikidata.org/entity/Q111792297', 'http://www.wikidata.org/entity/Q111792422', 'http://www.wikidata.org/entity/Q111792427', 'http://www.wikidata.org/entity/Q111792455', 'http://www.wikidata.org/entity/Q111792652', 'http://www.wikidata.org/entity/Q111792657', 'http://www.wikidata.org/entity/Q111792669', 'http://www.wikidata.org/entity/Q111795166', 'http://www.wikidata.org/entity/Q111795170', 'http://www.wikidata.org/entity/Q111795181', 'http://www.wikidata.org/entity/Q111795190', 'http://www.wikidata.org/entity/Q111795208', 'http://www.wikidata.org/entity/Q111795217', 'http://www.wikidata.org/entity/Q111795226', 'http://www.wikidata.org/entity/Q111795230', 'http://www.wikidata.org/entity/Q111795234', 'http://www.wikidata.org/entity/Q111795238', 'http://www.wikidata.org/entity/Q111798789', 'http://www.wikidata.org/entity/Q111799191', 'http://www.wikidata.org/entity/Q111799265', 'http://www.wikidata.org/entity/Q111799326', 'http://www.wikidata.org/entity/Q111799364', 'http://www.wikidata.org/entity/Q111799715', 'http://www.wikidata.org/entity/Q111800151', 'http://www.wikidata.org/entity/Q111800560', 'http://www.wikidata.org/entity/Q111800590', 'http://www.wikidata.org/entity/Q111800661', 'http://www.wikidata.org/entity/Q111800678', 'http://www.wikidata.org/entity/Q111800735', 'http://www.wikidata.org/entity/Q111800758', 'http://www.wikidata.org/entity/Q111801201', 'http://www.wikidata.org/entity/Q111801219', 'http://www.wikidata.org/entity/Q111801257', 'http://www.wikidata.org/entity/Q111801366', 'http://www.wikidata.org/entity/Q111801395', 'http://www.wikidata.org/entity/Q111801411', 'http://www.wikidata.org/entity/Q111801450', 'http://www.wikidata.org/entity/Q111801507', 'http://www.wikidata.org/entity/Q111801550', 'http://www.wikidata.org/entity/Q111810594', 'http://www.wikidata.org/entity/Q111810721', 'http://www.wikidata.org/entity/Q111811564', 'http://www.wikidata.org/entity/Q111811624', 'http://www.wikidata.org/entity/Q111811681', 'http://www.wikidata.org/entity/Q111812563', 'http://www.wikidata.org/entity/Q111812584', 'http://www.wikidata.org/entity/Q111812855', 'http://www.wikidata.org/entity/Q111816790', 'http://www.wikidata.org/entity/Q111817714', 'http://www.wikidata.org/entity/Q111817744', 'http://www.wikidata.org/entity/Q111817829', 'http://www.wikidata.org/entity/Q111817846', 'http://www.wikidata.org/entity/Q111817920', 'http://www.wikidata.org/entity/Q111818123', 'http://www.wikidata.org/entity/Q111824276', 'http://www.wikidata.org/entity/Q111824296', 'http://www.wikidata.org/entity/Q111824414', 'http://www.wikidata.org/entity/Q111824439', 'http://www.wikidata.org/entity/Q111824771', 'http://www.wikidata.org/entity/Q111824800', 'http://www.wikidata.org/entity/Q111824823', 'http://www.wikidata.org/entity/Q111824918', 'http://www.wikidata.org/entity/Q111825400', 'http://www.wikidata.org/entity/Q111825424', 'http://www.wikidata.org/entity/Q111825449', 'http://www.wikidata.org/entity/Q111825554', 'http://www.wikidata.org/entity/Q111825613', 'http://www.wikidata.org/entity/Q111825677', 'http://www.wikidata.org/entity/Q111825713', 'http://www.wikidata.org/entity/Q111825832', 'http://www.wikidata.org/entity/Q111826063', 'http://www.wikidata.org/entity/Q111826089', 'http://www.wikidata.org/entity/Q111830034', 'http://www.wikidata.org/entity/Q111830188', 'http://www.wikidata.org/entity/Q111837290', 'http://www.wikidata.org/entity/Q111837438', 'http://www.wikidata.org/entity/Q111837464', 'http://www.wikidata.org/entity/Q111837474', 'http://www.wikidata.org/entity/Q111837785', 'http://www.wikidata.org/entity/Q111837834', 'http://www.wikidata.org/entity/Q111837845', 'http://www.wikidata.org/entity/Q111837855', 'http://www.wikidata.org/entity/Q111837912', 'http://www.wikidata.org/entity/Q111837991', 'http://www.wikidata.org/entity/Q111848069', 'http://www.wikidata.org/entity/Q111848409', 'http://www.wikidata.org/entity/Q111848456', 'http://www.wikidata.org/entity/Q111848558', 'http://www.wikidata.org/entity/Q111848588', 'http://www.wikidata.org/entity/Q111848721', 'http://www.wikidata.org/entity/Q111848749', 'http://www.wikidata.org/entity/Q111848889', 'http://www.wikidata.org/entity/Q111903596', 'http://www.wikidata.org/entity/Q111903847', 'http://www.wikidata.org/entity/Q111903850', 'http://www.wikidata.org/entity/Q111903876', 'http://www.wikidata.org/entity/Q111903878', 'http://www.wikidata.org/entity/Q111903929', 'http://www.wikidata.org/entity/Q111903935', 'http://www.wikidata.org/entity/Q111903958', 'http://www.wikidata.org/entity/Q111904025', 'http://www.wikidata.org/entity/Q111904053', 'http://www.wikidata.org/entity/Q111904059', 'http://www.wikidata.org/entity/Q111904155', 'http://www.wikidata.org/entity/Q111905212', 'http://www.wikidata.org/entity/Q111905225', 'http://www.wikidata.org/entity/Q111905272', 'http://www.wikidata.org/entity/Q111906585', 'http://www.wikidata.org/entity/Q111906632', 'http://www.wikidata.org/entity/Q111906707', 'http://www.wikidata.org/entity/Q111907290', 'http://www.wikidata.org/entity/Q111907317', 'http://www.wikidata.org/entity/Q111908878', 'http://www.wikidata.org/entity/Q111908880', 'http://www.wikidata.org/entity/Q111908884', 'http://www.wikidata.org/entity/Q111908910', 'http://www.wikidata.org/entity/Q111909231', 'http://www.wikidata.org/entity/Q111909314', 'http://www.wikidata.org/entity/Q111909357', 'http://www.wikidata.org/entity/Q111909361', 'http://www.wikidata.org/entity/Q111909369', 'http://www.wikidata.org/entity/Q111909483', 'http://www.wikidata.org/entity/Q111909520', 'http://www.wikidata.org/entity/Q111909557', 'http://www.wikidata.org/entity/Q111909632', 'http://www.wikidata.org/entity/Q111909656', 'http://www.wikidata.org/entity/Q111909659', 'http://www.wikidata.org/entity/Q111909665', 'http://www.wikidata.org/entity/Q111909679', 'http://www.wikidata.org/entity/Q111909683', 'http://www.wikidata.org/entity/Q111909686', 'http://www.wikidata.org/entity/Q111918622', 'http://www.wikidata.org/entity/Q111972328', 'http://www.wikidata.org/entity/Q111972588', 'http://www.wikidata.org/entity/Q111972596', 'http://www.wikidata.org/entity/Q111972626', 'http://www.wikidata.org/entity/Q111972641', 'http://www.wikidata.org/entity/Q111972655', 'http://www.wikidata.org/entity/Q111972667', 'http://www.wikidata.org/entity/Q111972760', 'http://www.wikidata.org/entity/Q111972775', 'http://www.wikidata.org/entity/Q111981575', 'http://www.wikidata.org/entity/Q111981578', 'http://www.wikidata.org/entity/Q111981586', 'http://www.wikidata.org/entity/Q111981600', 'http://www.wikidata.org/entity/Q111981655', 'http://www.wikidata.org/entity/Q111981806', 'http://www.wikidata.org/entity/Q111984435', 'http://www.wikidata.org/entity/Q111993442', 'http://www.wikidata.org/entity/Q111993561', 'http://www.wikidata.org/entity/Q112028016', 'http://www.wikidata.org/entity/Q112028058', 'http://www.wikidata.org/entity/Q112030707', 'http://www.wikidata.org/entity/Q112037464', 'http://www.wikidata.org/entity/Q112038287', 'http://www.wikidata.org/entity/Q112040430', 'http://www.wikidata.org/entity/Q112053302', 'http://www.wikidata.org/entity/Q112059989', 'http://www.wikidata.org/entity/Q112063713', 'http://www.wikidata.org/entity/Q112087493', 'http://www.wikidata.org/entity/Q112127176', 'http://www.wikidata.org/entity/Q112183753', 'http://www.wikidata.org/entity/Q112190885', 'http://www.wikidata.org/entity/Q112263083', 'http://www.wikidata.org/entity/Q112667083', 'http://www.wikidata.org/entity/Q112667550', 'http://www.wikidata.org/entity/Q112669313', 'http://www.wikidata.org/entity/Q112669383', 'http://www.wikidata.org/entity/Q112681996', 'http://www.wikidata.org/entity/Q112746421', 'http://www.wikidata.org/entity/Q112747808', 'http://www.wikidata.org/entity/Q112894949', 'http://www.wikidata.org/entity/Q112894986', 'http://www.wikidata.org/entity/Q113015050', 'http://www.wikidata.org/entity/Q113072738', 'http://www.wikidata.org/entity/Q1131707', 'http://www.wikidata.org/entity/Q113272299', 'http://www.wikidata.org/entity/Q113272409', 'http://www.wikidata.org/entity/Q113272932', 'http://www.wikidata.org/entity/Q113499373', 'http://www.wikidata.org/entity/Q113499494', 'http://www.wikidata.org/entity/Q113650760', 'http://www.wikidata.org/entity/Q11368765', 'http://www.wikidata.org/entity/Q113811579', 'http://www.wikidata.org/entity/Q113813231', 'http://www.wikidata.org/entity/Q113828978', 'http://www.wikidata.org/entity/Q113830063', 'http://www.wikidata.org/entity/Q113841626', 'http://www.wikidata.org/entity/Q113849016', 'http://www.wikidata.org/entity/Q113860611', 'http://www.wikidata.org/entity/Q113860644', 'http://www.wikidata.org/entity/Q113861194', 'http://www.wikidata.org/entity/Q113882354', 'http://www.wikidata.org/entity/Q113884368', 'http://www.wikidata.org/entity/Q113901976', 'http://www.wikidata.org/entity/Q113904662', 'http://www.wikidata.org/entity/Q1139536', 'http://www.wikidata.org/entity/Q113955599', 'http://www.wikidata.org/entity/Q113955616', 'http://www.wikidata.org/entity/Q113955620', 'http://www.wikidata.org/entity/Q113955692', 'http://www.wikidata.org/entity/Q113961851', 'http://www.wikidata.org/entity/Q113961888', 'http://www.wikidata.org/entity/Q113961932', 'http://www.wikidata.org/entity/Q114028189', 'http://www.wikidata.org/entity/Q114046091', 'http://www.wikidata.org/entity/Q114056617', 'http://www.wikidata.org/entity/Q114057278', 'http://www.wikidata.org/entity/Q114059225', 'http://www.wikidata.org/entity/Q114243677', 'http://www.wikidata.org/entity/Q114454471', 'http://www.wikidata.org/entity/Q1145566', 'http://www.wikidata.org/entity/Q1145630', 'http://www.wikidata.org/entity/Q114582556', 'http://www.wikidata.org/entity/Q114588676', 'http://www.wikidata.org/entity/Q114604', 'http://www.wikidata.org/entity/Q114947458', 'http://www.wikidata.org/entity/Q114948159', 'http://www.wikidata.org/entity/Q114996688', 'http://www.wikidata.org/entity/Q114997174', 'http://www.wikidata.org/entity/Q115341348', 'http://www.wikidata.org/entity/Q115367992', 'http://www.wikidata.org/entity/Q115397386', 'http://www.wikidata.org/entity/Q115517924', 'http://www.wikidata.org/entity/Q115764515', 'http://www.wikidata.org/entity/Q115801523', 'http://www.wikidata.org/entity/Q115912774', 'http://www.wikidata.org/entity/Q115990472', 'http://www.wikidata.org/entity/Q116414186', 'http://www.wikidata.org/entity/Q116690653', 'http://www.wikidata.org/entity/Q117421915', 'http://www.wikidata.org/entity/Q117695225', 'http://www.wikidata.org/entity/Q117751349', 'http://www.wikidata.org/entity/Q117795094', 'http://www.wikidata.org/entity/Q11789705', 'http://www.wikidata.org/entity/Q118128483', 'http://www.wikidata.org/entity/Q11921906', 'http://www.wikidata.org/entity/Q11938851', 'http://www.wikidata.org/entity/Q119496586', 'http://www.wikidata.org/entity/Q11993043', 'http://www.wikidata.org/entity/Q1207931', 'http://www.wikidata.org/entity/Q1207932', 'http://www.wikidata.org/entity/Q120837533', 'http://www.wikidata.org/entity/Q121886956', 'http://www.wikidata.org/entity/Q122068698', 'http://www.wikidata.org/entity/Q122188018', 'http://www.wikidata.org/entity/Q12228863', 'http://www.wikidata.org/entity/Q12228866', 'http://www.wikidata.org/entity/Q12228868', 'http://www.wikidata.org/entity/Q12228876', 'http://www.wikidata.org/entity/Q12228884', 'http://www.wikidata.org/entity/Q12252186', 'http://www.wikidata.org/entity/Q12277858', 'http://www.wikidata.org/entity/Q122832546', 'http://www.wikidata.org/entity/Q12314502', 'http://www.wikidata.org/entity/Q123337193', 'http://www.wikidata.org/entity/Q123592992', 'http://www.wikidata.org/entity/Q12361577', 'http://www.wikidata.org/entity/Q123746478', 'http://www.wikidata.org/entity/Q12376028', 'http://www.wikidata.org/entity/Q12378350', 'http://www.wikidata.org/entity/Q124036138', 'http://www.wikidata.org/entity/Q12407929', 'http://www.wikidata.org/entity/Q12411505', 'http://www.wikidata.org/entity/Q124367042', 'http://www.wikidata.org/entity/Q124504910', 'http://www.wikidata.org/entity/Q124564384', 'http://www.wikidata.org/entity/Q124612831', 'http://www.wikidata.org/entity/Q124615758', 'http://www.wikidata.org/entity/Q124619352', 'http://www.wikidata.org/entity/Q124620804', 'http://www.wikidata.org/entity/Q124620822', 'http://www.wikidata.org/entity/Q124707699', 'http://www.wikidata.org/entity/Q124820083', 'http://www.wikidata.org/entity/Q124830280', 'http://www.wikidata.org/entity/Q124857570', 'http://www.wikidata.org/entity/Q124858688', 'http://www.wikidata.org/entity/Q124858953', 'http://www.wikidata.org/entity/Q125149734', 'http://www.wikidata.org/entity/Q125205121', 'http://www.wikidata.org/entity/Q1254268', 'http://www.wikidata.org/entity/Q125510673', 'http://www.wikidata.org/entity/Q125511630', 'http://www.wikidata.org/entity/Q125521675', 'http://www.wikidata.org/entity/Q125521758', 'http://www.wikidata.org/entity/Q125555445', 'http://www.wikidata.org/entity/Q125566609', 'http://www.wikidata.org/entity/Q125577561', 'http://www.wikidata.org/entity/Q125592462', 'http://www.wikidata.org/entity/Q12560060', 'http://www.wikidata.org/entity/Q125688458', 'http://www.wikidata.org/entity/Q125688603', 'http://www.wikidata.org/entity/Q125700972', 'http://www.wikidata.org/entity/Q125704427', 'http://www.wikidata.org/entity/Q125747483', 'http://www.wikidata.org/entity/Q125749644', 'http://www.wikidata.org/entity/Q125758800', 'http://www.wikidata.org/entity/Q125759229', 'http://www.wikidata.org/entity/Q125845551', 'http://www.wikidata.org/entity/Q12584835', 'http://www.wikidata.org/entity/Q125856465', 'http://www.wikidata.org/entity/Q125867175', 'http://www.wikidata.org/entity/Q125867458', 'http://www.wikidata.org/entity/Q125867756', 'http://www.wikidata.org/entity/Q125867888', 'http://www.wikidata.org/entity/Q125869488', 'http://www.wikidata.org/entity/Q125879646', 'http://www.wikidata.org/entity/Q125879891', 'http://www.wikidata.org/entity/Q125883649', 'http://www.wikidata.org/entity/Q125883847', 'http://www.wikidata.org/entity/Q125890530', 'http://www.wikidata.org/entity/Q125890753', 'http://www.wikidata.org/entity/Q125891443', 'http://www.wikidata.org/entity/Q125891720', 'http://www.wikidata.org/entity/Q125895110', 'http://www.wikidata.org/entity/Q125895155', 'http://www.wikidata.org/entity/Q125899181', 'http://www.wikidata.org/entity/Q125899513', 'http://www.wikidata.org/entity/Q125901134', 'http://www.wikidata.org/entity/Q125903138', 'http://www.wikidata.org/entity/Q125910729', 'http://www.wikidata.org/entity/Q125910806', 'http://www.wikidata.org/entity/Q125911055', 'http://www.wikidata.org/entity/Q125911072', 'http://www.wikidata.org/entity/Q125914666', 'http://www.wikidata.org/entity/Q125914885', 'http://www.wikidata.org/entity/Q125921693', 'http://www.wikidata.org/entity/Q125922831', 'http://www.wikidata.org/entity/Q125922882', 'http://www.wikidata.org/entity/Q125926636', 'http://www.wikidata.org/entity/Q125932740', 'http://www.wikidata.org/entity/Q125936101', 'http://www.wikidata.org/entity/Q125936683', 'http://www.wikidata.org/entity/Q125956876', 'http://www.wikidata.org/entity/Q125959131', 'http://www.wikidata.org/entity/Q125965703', 'http://www.wikidata.org/entity/Q125966437', 'http://www.wikidata.org/entity/Q125966992', 'http://www.wikidata.org/entity/Q125968806', 'http://www.wikidata.org/entity/Q125969610', 'http://www.wikidata.org/entity/Q125970539', 'http://www.wikidata.org/entity/Q125984409', 'http://www.wikidata.org/entity/Q125984492', 'http://www.wikidata.org/entity/Q125994583', 'http://www.wikidata.org/entity/Q125997034', 'http://www.wikidata.org/entity/Q125998688', 'http://www.wikidata.org/entity/Q125998803', 'http://www.wikidata.org/entity/Q125998897', 'http://www.wikidata.org/entity/Q125999072', 'http://www.wikidata.org/entity/Q12599950', 'http://www.wikidata.org/entity/Q126010095', 'http://www.wikidata.org/entity/Q126010128', 'http://www.wikidata.org/entity/Q126028447', 'http://www.wikidata.org/entity/Q126028546', 'http://www.wikidata.org/entity/Q126032653', 'http://www.wikidata.org/entity/Q126126323', 'http://www.wikidata.org/entity/Q126126778', 'http://www.wikidata.org/entity/Q12613371', 'http://www.wikidata.org/entity/Q12629515', 'http://www.wikidata.org/entity/Q126325524', 'http://www.wikidata.org/entity/Q126361854', 'http://www.wikidata.org/entity/Q126362969', 'http://www.wikidata.org/entity/Q126371412', 'http://www.wikidata.org/entity/Q126371457', 'http://www.wikidata.org/entity/Q126371864', 'http://www.wikidata.org/entity/Q126371886', 'http://www.wikidata.org/entity/Q126372368', 'http://www.wikidata.org/entity/Q126372458', 'http://www.wikidata.org/entity/Q126372576', 'http://www.wikidata.org/entity/Q126415038', 'http://www.wikidata.org/entity/Q126456102', 'http://www.wikidata.org/entity/Q126477003', 'http://www.wikidata.org/entity/Q126477086', 'http://www.wikidata.org/entity/Q126477151', 'http://www.wikidata.org/entity/Q126477162', 'http://www.wikidata.org/entity/Q126478091', 'http://www.wikidata.org/entity/Q126478228', 'http://www.wikidata.org/entity/Q126511431', 'http://www.wikidata.org/entity/Q126513767', 'http://www.wikidata.org/entity/Q126593634', 'http://www.wikidata.org/entity/Q12663413', 'http://www.wikidata.org/entity/Q126666887', 'http://www.wikidata.org/entity/Q126709387', 'http://www.wikidata.org/entity/Q126721902', 'http://www.wikidata.org/entity/Q126726117', 'http://www.wikidata.org/entity/Q126811008', 'http://www.wikidata.org/e</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q100329955', 'http://www.wikidata.org/entity/Q100597341', 'http://www.wikidata.org/entity/Q100860934', 'http://www.wikidata.org/entity/Q101026979', 'http://www.wikidata.org/entity/Q101545880', 'http://www.wikidata.org/entity/Q101627559', 'http://www.wikidata.org/entity/Q1016833', 'http://www.wikidata.org/entity/Q101706322', 'http://www.wikidata.org/entity/Q102276948', 'http://www.wikidata.org/entity/Q102398478', 'http://www.wikidata.org/entity/Q10244', 'http://www.wikidata.org/entity/Q10253', 'http://www.wikidata.org/entity/Q1025481', 'http://www.wikidata.org/entity/Q10259922', 'http://www.wikidata.org/entity/Q10265947', 'http://www.wikidata.org/entity/Q10281787', 'http://www.wikidata.org/entity/Q10329424', 'http://www.wikidata.org/entity/Q103821550', 'http://www.wikidata.org/entity/Q1038328', 'http://www.wikidata.org/entity/Q103956800', 'http://www.wikidata.org/entity/Q10398273', 'http://www.wikidata.org/entity/Q104051143', 'http://www.wikidata.org/entity/Q10412386', 'http://www.wikidata.org/entity/Q10416096', 'http://www.wikidata.org/entity/Q10418897', 'http://www.wikidata.org/entity/Q104224166', 'http://www.wikidata.org/entity/Q1043596', 'http://www.wikidata.org/entity/Q104601590', 'http://www.wikidata.org/entity/Q104625773', 'http://www.wikidata.org/entity/Q104758920', 'http://www.wikidata.org/entity/Q10481350', 'http://www.wikidata.org/entity/Q104920297', 'http://www.wikidata.org/entity/Q10494624', 'http://www.wikidata.org/entity/Q10495964', 'http://www.wikidata.org/entity/Q10496086', 'http://www.wikidata.org/entity/Q10501512', 'http://www.wikidata.org/entity/Q1050292', 'http://www.wikidata.org/entity/Q105043914', 'http://www.wikidata.org/entity/Q105121443', 'http://www.wikidata.org/entity/Q105360445', 'http://www.wikidata.org/entity/Q105393711', 'http://www.wikidata.org/entity/Q105394069', 'http://www.wikidata.org/entity/Q10541207', 'http://www.wikidata.org/entity/Q1054558', 'http://www.wikidata.org/entity/Q105663779', 'http://www.wikidata.org/entity/Q10586365', 'http://www.wikidata.org/entity/Q10601007', 'http://www.wikidata.org/entity/Q10601355', 'http://www.wikidata.org/entity/Q106019359', 'http://www.wikidata.org/entity/Q106043577', 'http://www.wikidata.org/entity/Q106078232', 'http://www.wikidata.org/entity/Q106200291', 'http://www.wikidata.org/entity/Q106240773', 'http://www.wikidata.org/entity/Q106290028', 'http://www.wikidata.org/entity/Q106307776', 'http://www.wikidata.org/entity/Q10631904', 'http://www.wikidata.org/entity/Q106331005', 'http://www.wikidata.org/entity/Q106349026', 'http://www.wikidata.org/entity/Q106369745', 'http://www.wikidata.org/entity/Q106436015', 'http://www.wikidata.org/entity/Q106505905', 'http://www.wikidata.org/entity/Q10666884', 'http://www.wikidata.org/entity/Q106675733', 'http://www.wikidata.org/entity/Q106689897', 'http://www.wikidata.org/entity/Q10669318', 'http://www.wikidata.org/entity/Q10669370', 'http://www.wikidata.org/entity/Q10669371', 'http://www.wikidata.org/entity/Q10685840', 'http://www.wikidata.org/entity/Q10689144', 'http://www.wikidata.org/entity/Q10689145', 'http://www.wikidata.org/entity/Q10689146', 'http://www.wikidata.org/entity/Q106899527', 'http://www.wikidata.org/entity/Q10698576', 'http://www.wikidata.org/entity/Q10698931', 'http://www.wikidata.org/entity/Q10698932', 'http://www.wikidata.org/entity/Q10698935', 'http://www.wikidata.org/entity/Q10698936', 'http://www.wikidata.org/entity/Q10698937', 'http://www.wikidata.org/entity/Q10699347', 'http://www.wikidata.org/entity/Q107015910', 'http://www.wikidata.org/entity/Q10701677', 'http://www.wikidata.org/entity/Q10701968', 'http://www.wikidata.org/entity/Q1070318', 'http://www.wikidata.org/entity/Q10714715', 'http://www.wikidata.org/entity/Q10726998', 'http://www.wikidata.org/entity/Q107309593', 'http://www.wikidata.org/entity/Q107718805', 'http://www.wikidata.org/entity/Q107739995', 'http://www.wikidata.org/entity/Q108010714', 'http://www.wikidata.org/entity/Q108101493', 'http://www.wikidata.org/entity/Q108131371', 'http://www.wikidata.org/entity/Q108219988', 'http://www.wikidata.org/entity/Q108315106', 'http://www.wikidata.org/entity/Q108392466', 'http://www.wikidata.org/entity/Q108424805', 'http://www.wikidata.org/entity/Q10854401', 'http://www.wikidata.org/entity/Q10855559', 'http://www.wikidata.org/entity/Q108660772', 'http://www.wikidata.org/entity/Q10868404', 'http://www.wikidata.org/entity/Q108730127', 'http://www.wikidata.org/entity/Q108749396', 'http://www.wikidata.org/entity/Q108749484', 'http://www.wikidata.org/entity/Q108814176', 'http://www.wikidata.org/entity/Q108936669', 'http://www.wikidata.org/entity/Q10909572', 'http://www.wikidata.org/entity/Q109121006', 'http://www.wikidata.org/entity/Q1091428', 'http://www.wikidata.org/entity/Q10921477', 'http://www.wikidata.org/entity/Q109285268', 'http://www.wikidata.org/entity/Q109329448', 'http://www.wikidata.org/entity/Q109329455', 'http://www.wikidata.org/entity/Q109356066', 'http://www.wikidata.org/entity/Q109381834', 'http://www.wikidata.org/entity/Q109381883', 'http://www.wikidata.org/entity/Q109440429', 'http://www.wikidata.org/entity/Q109455204', 'http://www.wikidata.org/entity/Q10955171', 'http://www.wikidata.org/entity/Q109558468', 'http://www.wikidata.org/entity/Q109609391', 'http://www.wikidata.org/entity/Q10964022', 'http://www.wikidata.org/entity/Q109827527', 'http://www.wikidata.org/entity/Q109838056', 'http://www.wikidata.org/entity/Q109908577', 'http://www.wikidata.org/entity/Q11002663', 'http://www.wikidata.org/entity/Q110091424', 'http://www.wikidata.org/entity/Q110128398', 'http://www.wikidata.org/entity/Q110206440', 'http://www.wikidata.org/entity/Q110239836', 'http://www.wikidata.org/entity/Q110639888', 'http://www.wikidata.org/entity/Q110962934', 'http://www.wikidata.org/entity/Q111149458', 'http://www.wikidata.org/entity/Q111202983', 'http://www.wikidata.org/entity/Q111333928', 'http://www.wikidata.org/entity/Q111574867', 'http://www.wikidata.org/entity/Q111605537', 'http://www.wikidata.org/entity/Q111649462', 'http://www.wikidata.org/entity/Q111649876', 'http://www.wikidata.org/entity/Q111655654', 'http://www.wikidata.org/entity/Q111711222', 'http://www.wikidata.org/entity/Q111732603', 'http://www.wikidata.org/entity/Q111811564', 'http://www.wikidata.org/entity/Q111846538', 'http://www.wikidata.org/entity/Q111914764', 'http://www.wikidata.org/entity/Q112055', 'http://www.wikidata.org/entity/Q112059989', 'http://www.wikidata.org/entity/Q112075710', 'http://www.wikidata.org/entity/Q11219195', 'http://www.wikidata.org/entity/Q112292803', 'http://www.wikidata.org/entity/Q11237670', 'http://www.wikidata.org/entity/Q11244589', 'http://www.wikidata.org/entity/Q112613424', 'http://www.wikidata.org/entity/Q11269', 'http://www.wikidata.org/entity/Q112748137', 'http://www.wikidata.org/entity/Q11277431', 'http://www.wikidata.org/entity/Q112971391', 'http://www.wikidata.org/entity/Q112971396', 'http://www.wikidata.org/entity/Q112971410', 'http://www.wikidata.org/entity/Q112971413', 'http://www.wikidata.org/entity/Q113040064', 'http://www.wikidata.org/entity/Q113114857', 'http://www.wikidata.org/entity/Q113232600', 'http://www.wikidata.org/entity/Q113383597', 'http://www.wikidata.org/entity/Q113470219', 'http://www.wikidata.org/entity/Q113470532', 'http://www.wikidata.org/entity/Q113485231', 'http://www.wikidata.org/entity/Q113499420', 'http://www.wikidata.org/entity/Q113499458', 'http://www.wikidata.org/entity/Q1135034', 'http://www.wikidata.org/entity/Q11354348', 'http://www.wikidata.org/entity/Q113549137', 'http://www.wikidata.org/entity/Q113576165', 'http://www.wikidata.org/entity/Q113581609', 'http://www.wikidata.org/entity/Q113627236', 'http://www.wikidata.org/entity/Q113631347', 'http://www.wikidata.org/entity/Q113631375', 'http://www.wikidata.org/entity/Q113631508', 'http://www.wikidata.org/entity/Q113631563', 'http://www.wikidata.org/entity/Q113631569', 'http://www.wikidata.org/entity/Q113674106', 'http://www.wikidata.org/entity/Q11371391', 'http://www.wikidata.org/entity/Q113714633', 'http://www.wikidata.org/entity/Q11387117', 'http://www.wikidata.org/entity/Q113903854', 'http://www.wikidata.org/entity/Q11391277', 'http://www.wikidata.org/entity/Q1139591', 'http://www.wikidata.org/entity/Q11409712', 'http://www.wikidata.org/entity/Q114315605', 'http://www.wikidata.org/entity/Q114658295', 'http://www.wikidata.org/entity/Q1147008', 'http://www.wikidata.org/entity/Q114779611', 'http://www.wikidata.org/entity/Q114780741', 'http://www.wikidata.org/entity/Q114781351', 'http://www.wikidata.org/entity/Q114840373', 'http://www.wikidata.org/entity/Q114863314', 'http://www.wikidata.org/entity/Q115152362', 'http://www.wikidata.org/entity/Q115209188', 'http://www.wikidata.org/entity/Q115214299', 'http://www.wikidata.org/entity/Q115259173', 'http://www.wikidata.org/entity/Q115294651', 'http://www.wikidata.org/entity/Q115327380', 'http://www.wikidata.org/entity/Q1153848', 'http://www.wikidata.org/entity/Q11545488', 'http://www.wikidata.org/entity/Q115516436', 'http://www.wikidata.org/entity/Q115526578', 'http://www.wikidata.org/entity/Q115624997', 'http://www.wikidata.org/entity/Q115628690', 'http://www.wikidata.org/entity/Q11567159', 'http://www.wikidata.org/entity/Q11590237', 'http://www.wikidata.org/entity/Q115937074', 'http://www.wikidata.org/entity/Q11606287', 'http://www.wikidata.org/entity/Q116113833', 'http://www.wikidata.org/entity/Q116349234', 'http://www.wikidata.org/entity/Q116767714', 'http://www.wikidata.org/entity/Q116790237', 'http://www.wikidata.org/entity/Q116846825', 'http://www.wikidata.org/entity/Q116858640', 'http://www.wikidata.org/entity/Q116938985', 'http://www.wikidata.org/entity/Q11695705', 'http://www.wikidata.org/entity/Q11695707', 'http://www.wikidata.org/entity/Q11695708', 'http://www.wikidata.org/entity/Q11695711', 'http://www.wikidata.org/entity/Q11695713', 'http://www.wikidata.org/entity/Q11695714', 'http://www.wikidata.org/entity/Q11695716', 'http://www.wikidata.org/entity/Q11695717', 'http://www.wikidata.org/entity/Q11695718', 'http://www.wikidata.org/entity/Q11695721', 'http://www.wikidata.org/entity/Q11695722', 'http://www.wikidata.org/entity/Q11695723', 'http://www.wikidata.org/entity/Q116973585', 'http://www.wikidata.org/entity/Q116980492', 'http://www.wikidata.org/entity/Q117035968', 'http://www.wikidata.org/entity/Q11703716', 'http://www.wikidata.org/entity/Q117040282', 'http://www.wikidata.org/entity/Q11706236', 'http://www.wikidata.org/entity/Q1170632', 'http://www.wikidata.org/entity/Q117361394', 'http://www.wikidata.org/entity/Q117421915', 'http://www.wikidata.org/entity/Q117455751', 'http://www.wikidata.org/entity/Q117587270', 'http://www.wikidata.org/entity/Q117711867', 'http://www.wikidata.org/entity/Q11783773', 'http://www.wikidata.org/entity/Q11783808', 'http://www.wikidata.org/entity/Q117844480', 'http://www.wikidata.org/entity/Q11789695', 'http://www.wikidata.org/entity/Q11789705', 'http://www.wikidata.org/entity/Q11789707', 'http://www.wikidata.org/entity/Q11802972', 'http://www.wikidata.org/entity/Q118224784', 'http://www.wikidata.org/entity/Q118288532', 'http://www.wikidata.org/entity/Q118314773', 'http://www.wikidata.org/entity/Q118330188', 'http://www.wikidata.org/entity/Q118369207', 'http://www.wikidata.org/entity/Q118744251', 'http://www.wikidata.org/entity/Q118842681', 'http://www.wikidata.org/entity/Q118849459', 'http://www.wikidata.org/entity/Q118947258', 'http://www.wikidata.org/entity/Q119105010', 'http://www.wikidata.org/entity/Q11919090', 'http://www.wikidata.org/entity/Q119241124', 'http://www.wikidata.org/entity/Q119243817', 'http://www.wikidata.org/entity/Q119285617', 'http://www.wikidata.org/entity/Q119348301', 'http://www.wikidata.org/entity/Q119397277', 'http://www.wikidata.org/entity/Q1194059', 'http://www.wikidata.org/entity/Q11977920', 'http://www.wikidata.org/entity/Q119806244', 'http://www.wikidata.org/entity/Q119853995', 'http://www.wikidata.org/entity/Q120068971', 'http://www.wikidata.org/entity/Q120146391', 'http://www.wikidata.org/entity/Q120403912', 'http://www.wikidata.org/entity/Q120486552', 'http://www.wikidata.org/entity/Q12060958', 'http://www.wikidata.org/entity/Q120823815', 'http://www.wikidata.org/entity/Q120837533', 'http://www.wikidata.org/entity/Q12090941', 'http://www.wikidata.org/entity/Q1209940', 'http://www.wikidata.org/entity/Q12100125', 'http://www.wikidata.org/entity/Q12100126', 'http://www.wikidata.org/entity/Q12100128', 'http://www.wikidata.org/entity/Q12100132', 'http://www.wikidata.org/entity/Q12100138', 'http://www.wikidata.org/entity/Q12100141', 'http://www.wikidata.org/entity/Q12100152', 'http://www.wikidata.org/entity/Q12100160', 'http://www.wikidata.org/entity/Q12131090', 'http://www.wikidata.org/entity/Q121322780', 'http://www.wikidata.org/entity/Q121393', 'http://www.wikidata.org/entity/Q12149731', 'http://www.wikidata.org/entity/Q12174361', 'http://www.wikidata.org/entity/Q121759535', 'http://www.wikidata.org/entity/Q121852183', 'http://www.wikidata.org/entity/Q121864546', 'http://www.wikidata.org/entity/Q121991381', 'http://www.wikidata.org/entity/Q122057715', 'http://www.wikidata.org/entity/Q122058042', 'http://www.wikidata.org/entity/Q122144115', 'http://www.wikidata.org/entity/Q122199376', 'http://www.wikidata.org/entity/Q122341064', 'http://www.wikidata.org/entity/Q122460010', 'http://www.wikidata.org/entity/Q122495885', 'http://www.wikidata.org/entity/Q1226845', 'http://www.wikidata.org/entity/Q122767100', 'http://www.wikidata.org/entity/Q12284238', 'http://www.wikidata.org/entity/Q12286265', 'http://www.wikidata.org/entity/Q12286390', 'http://www.wikidata.org/entity/Q12289674', 'http://www.wikidata.org/entity/Q12292151', 'http://www.wikidata.org/entity/Q12293119', 'http://www.wikidata.org/entity/Q12293243', 'http://www.wikidata.org/entity/Q12299913', 'http://www.wikidata.org/entity/Q123111964', 'http://www.wikidata.org/entity/Q1231872', 'http://www.wikidata.org/entity/Q123253535', 'http://www.wikidata.org/entity/Q123265528', 'http://www.wikidata.org/entity/Q123450314', 'http://www.wikidata.org/entity/Q123515600', 'http://www.wikidata.org/entity/Q12353618', 'http://www.wikidata.org/entity/Q123746478', 'http://www.wikidata.org/entity/Q123757853', 'http://www.wikidata.org/entity/Q1239437', 'http://www.wikidata.org/entity/Q12407917', 'http://www.wikidata.org/entity/Q12407923', 'http://www.wikidata.org/entity/Q1241858', 'http://www.wikidata.org/entity/Q12422844', 'http://www.wikidata.org/entity/Q124250314', 'http://www.wikidata.org/entity/Q124250951', 'http://www.wikidata.org/entity/Q124255532', 'http://www.wikidata.org/entity/Q124318023', 'http://www.wikidata.org/entity/Q124352953', 'http://www.wikidata.org/entity/Q124367000', 'http://www.wikidata.org/entity/Q12438967', 'http://www.wikidata.org/entity/Q124408550', 'http://www.wikidata.org/entity/Q12441237', 'http://www.wikidata.org/entity/Q124498473', 'http://www.wikidata.org/entity/Q124498859', 'http://www.wikidata.org/entity/Q124568688', 'http://www.wikidata.org/entity/Q124747000', 'http://www.wikidata.org/entity/Q124799998', 'http://www.wikidata.org/entity/Q124830290', 'http://www.wikidata.org/entity/Q124854084', 'http://www.wikidata.org/entity/Q12513670', 'http://www.wikidata.org/entity/Q12525597', 'http://www.wikidata.org/entity/Q1252585', 'http://www.wikidata.org/entity/Q1252596', 'http://www.wikidata.org/entity/Q125505711', 'http://www.wikidata.org/entity/Q1255099', 'http://www.wikidata.org/entity/Q125524227', 'http://www.wikidata.org/entity/Q125613295', 'http://www.wikidata.org/entity/Q125912847', 'http://www.wikidata.org/entity/Q125928736', 'http://www.wikidata.org/entity/Q12601109', 'http://www.wikidata.org/entity/Q12602481', 'http://www.wikidata.org/entity/Q126083299', 'http://www.wikidata.org/entity/Q126083373', 'http://www.wikidata.org/entity/Q126113071', 'http://www.wikidata.org/entity/Q12614307', 'http://www.wikidata.org/entity/Q12614875', 'http://www.wikidata.org/entity/Q126192995', 'http://www.wikidata.org/entity/Q126260200', 'http://www.wikidata.org/entity/Q12650252', 'http://www.wikidata.org/entity/Q12663498', 'http://www.wikidata.org/entity/Q126708915', 'http://www.wikidata.org/entity/Q126902823', 'http://www.wikidata.org/entity/Q126903060', 'http://www.wikidata.org/entity/Q126910647', 'http://www.wikidata.org/entity/Q126948133', 'http://www.wikidata.org/entity/Q126949840', 'http://www.wikidata.org/entity/Q1270782', 'http://www.wikidata.org/entity/Q12713841', 'http://www.wikidata.org/entity/Q12716026', 'http://www.wikidata.org/entity/Q12719109', 'http://www.wikidata.org/entity/Q127393146', 'http://www.wikidata.org/entity/Q127502506', 'http://www.wikidata.org/entity/Q12750635', 'http://www.wikidata.org/entity/Q127597840', 'http://www.wikidata.org/entity/Q127798249', 'http://www.wikidata.org/entity/Q12787253', 'http://www.wikidata.org/entity/Q12787255', 'http://www.wikidata.org/entity/Q127922454', 'http://www.wikidata.org/entity/Q12803843', 'http://www.wikidata.org/entity/Q12836659', 'http://www.wikidata.org/entity/Q12859165', 'http://www.wikidata.org/entity/Q12864158', 'http://www.wikidata.org/entity/Q1290276', 'http://www.wikidata.org/entity/Q12927731', 'http://www.wikidata.org/entity/Q129726', 'http://www.wikidata.org/entity/Q12986877', 'http://www.wikidata.org/entity/Q129876847', 'http://www.wikidata.org/entity/Q129876849', 'http://www.wikidata.org/entity/Q129876851', 'http://www.wikidata.org/entity/Q129876853', 'http://www.wikidata.org/entity/Q129876855', 'http://www.wikidata.org/entity/Q129876857', 'http://www.wikidata.org/entity/Q12989464', 'http://www.wikidata.org/entity/Q13020973', 'http://www.wikidata.org/entity/Q130215597', 'http://www.wikidata.org/entity/Q130237269', 'http://www.wikidata.org/entity/Q130237270', 'http://www.wikidata.org/entity/Q130237271', 'http://www.wikidata.org/entity/Q130237272', 'http://www.wikidata.org/entity/Q130237273', 'http://www.wikidata.org/entity/Q130237274', 'http://www.wikidata.org/entity/Q130237276', 'http://www.wikidata.org/entity/Q130237277', 'http://www.wikidata.org/entity/Q130237278', 'http://www.wikidata.org/entity/Q130237279', 'http://www.wikidata.org/entity/Q130237280', 'http://www.wikidata.org/entity/Q130237281', 'http://www.wikidata.org/entity/Q130237282', 'http://www.wikidata.org/entity/Q130237283', 'http://www.wikidata.org/entity/Q130237284', 'http://www.wikidata.org/entity/Q130237285', 'http://www.wikidata.org/entity/Q130237286', 'http://www.wikidata.org/entity/Q130237287', 'http://www.wikidata.org/entity/Q130237288', 'http://www.wikidata.org/entity/Q130237289', 'http://www.wikidata.org/entity/Q130237290', 'http://www.wikidata.org/entity/Q130237291', 'http://www.wikidata.org/entity/Q130237292', 'http://www.wikidata.org/entity/Q130237293', 'http://www.wikidata.org/entity/Q130237294', 'http://www.wikidata.org/entity/Q130237295', 'http://www.wikidata.org/entity/Q130237296', 'http://www.wikidata.org/entity/Q130237297', 'http://www.wikidata.org/entity/Q130237298', 'http://www.wikidata.org/entity/Q130237299', 'http://www.wikidata.org/entity/Q130237300', 'http://www.wikidata.org/entity/Q130237301', 'http://www.wikidata.org/entity/Q130237302', 'http://www.wikidata.org/entity/Q130237303', 'http://www.wikidata.org/entity/Q130237304', 'http://www.wikidata.org/entity/Q130237305', 'http://www.wikidata.org/entity/Q130237306', 'http://www.wikidata.org/entity/Q130237307', 'http://www.wikidata.org/entity/Q130237308', 'http://www.wikidata.org/entity/Q130237309', 'http://www.wikidata.org/entity/Q130237310', 'http://www.wikidata.org/entity/Q130237311', 'http://www.wikidata.org/entity/Q130237312', 'http://www.wikidata.org/entity/Q130237314', 'http://www.wikidata.org/entity/Q130237315', 'http://www.wikidata.org/entity/Q130237316', 'http://www.wikidata.org/entity/Q130237317', 'http://www.wikidata.org/entity/Q130237318', 'http://www.wikidata.org/entity/Q130237319', 'http://www.wikidata.org/entity/Q130237320', 'http://www.wikidata.org/entity/Q130237321', 'http://www.wikidata.org/entity/Q130237322', 'http://www.wikidata.org/entity/Q130237323', 'http://www.wikidata.org/entity/Q130237324', 'http://www.wikidata.org/entity/Q130237325', 'http://www.wikidata.org/entity/Q130237326', 'http://www.wikidata.org/entity/Q130237327', 'http://www.wikidata.org/entity/Q130237328', 'http://www.wikidata.org/entity/Q130237329', 'http://www.wikidata.org/entity/Q130237330', 'http://www.wikidata.org/entity/Q130237331', 'http://www.wikidata.org/entity/Q130237332', 'http://www.wikidata.org/entity/Q130237333', 'http://www.wikidata.org/entity/Q130237334', 'http://www.wikidata.org/entity/Q130237335', 'http://www.wikidata.org/entity/Q130237336', 'http://www.wikidata.org/entity/Q130237337', 'http://www.wikidata.org/entity/Q130237338', 'http://www.wikidata.org/entity/Q130237339', 'http://www.wikidata.org/entity/Q130237340', 'http://www.wikidata.org/entity/Q130237341', 'http://www.wikidata.org/entity/Q130237342', 'http://www.wikidata.org/entity/Q130237343', 'http://www.wikidata.org/entity/Q130237344', 'http://www.wikidata.org/entity/Q130237345', 'http://www.wikidata.org/entity/Q130237346', 'http://www.wikidata.org/entity/Q130237347', 'http://www.wikidata.org/entity/Q130237348', 'http://www.wikidata.org/entity/Q130237349', 'http://www.wikidata.org/entity/Q130237350', 'http://www.wikidata.org/entity/Q130237351', 'http://www.wikidata.org/entity/Q130237353', 'http://www.wikidata.org/entity/Q130237354', 'http://www.wikidata.org/entity/Q130237355', 'http://www.wikidata.org/entity/Q130237356', 'http://www.wikidata.org/entity/Q130237357', 'http://www.wikidata.org/entity/Q130237358', 'http://www.wikidata.org/entity/Q130237359', 'http://www.wikidata.org/entity/Q130237360', 'http://www.wikidata.org/entity/Q130237361', 'http://www.wikidata.org/entity/Q130237362', 'http://www.wikidata.org/entity/Q130237363', 'http://www.wikidata.org/entity/Q130237364', 'http://www.wikidata.org/entity/Q130237365', 'http://www.wikidata.org/entity/Q130237366', 'http://www.wikidata.org/entity/Q130237367', 'http://www.wikidata.org/entity/Q130237368', 'http://www.wikidata.org/entity/Q130237369', 'http://www.wikidata.org/entity/Q130237370', 'http://www.wikidata.org/entity/Q130237371', 'http://www.wikidata.org/entity/Q130237372', 'http://www.wikidata.org/entity/Q130237373', 'http://www.wikidata.org/entity/Q130237374', 'http://www.wikidata.org/entity/Q130237375', 'http://www.wikidata.org/entity/Q130237376', 'http://www.wikidata.org/entity/Q130237377', 'http://www.wikidata.org/entity/Q130237378', 'http://www.wikidata.org/entity/Q130237379', 'http://www.wikidata.org/entity/Q130237380', 'http://www.wikidata.org/entity/Q130237381', 'http://www.wikidata.org/entity/Q130237382', 'http://www.wikidata.org/entity/Q130237383', 'http://www.wikidata.org/entity/Q130237384', 'http://www.wikidata.org/entity/Q130237385', 'http://www.wikidata.org/entity/Q130237386', 'http://www.wikidata.org/entity/Q130237387', 'http://www.wikidata.org/entity/Q130237388', 'http://www.wikidata.org/entity/Q130237389', 'http://www.wikidata.org/entity/Q130237390', 'http://www.wikidata.org/entity/Q130237391', 'http://www.wikidata.org/entity/Q130237392', 'http://www.wikidata.org/entity/Q130237393', 'http://www.wikidata.org/entity/Q130237394', 'http://www.wikidata.org/entity/Q130237395', 'http://www.wikidata.org/entity/Q130237396', 'http://www.wikidata.org/entity/Q130237397', 'http://www.wikidata.org/entity/Q130237398', 'http://www.wikidata.org/entity/Q130237399', 'http://www.wikidata.org/entity/Q130237400', 'http://www.wikidata.org/entity/Q130237402', 'http://www.wikidata.org/entity/Q130237403', 'http://www.wikidata.org/entity/Q130237404', 'http://www.wikidata.org/entity/Q130237405', 'http://www.wikidata.org/entity/Q130237406', 'http://www.wikidata.org/entity/Q130237407', 'http://www.wikidata.org/entity/Q130237408', 'http://www.wikidata.org/entity/Q130237409', 'http://www.wikidata.org/entity/Q130237410', 'http://www.wikidata.org/entity/Q130237411', 'http://www.wikidata.org/entity/Q130237412', 'http://www.wikidata.org/entity/Q130237413', 'http://www.wikidata.org/entity/Q130237414', 'http://www.wikidata.org/entity/Q130237415', 'http://www.wikidata.org/entity/Q130237416', 'http://www.wikidata.org/entity/Q130237417', 'http://www.wikidata.org/entity/Q130237419', 'http://www.wikidata.org/entity/Q130237420', 'http://www.wikidata.org/entity/Q130237421', 'http://www.wikidata.org/entity/Q130237422', 'http://www.wikidata.org/entity/Q130237423', 'http://www.wikidata.org/entity/Q130237424', 'http://www.wikidata.org/entity/Q130237425', 'http://www.wikidata.org/entity/Q130237426', 'http://www.wikidata.org/entity/Q130237427', 'http://www.wikidata.org/entity/Q130237428', 'http://www.wikidata.org/entity/Q130237429', 'http://www.wikidata.org/entity/Q130237430', 'http://www.wikidata.org/entity/Q130237431', 'http://www.wikidata.org/entity/Q130237432', 'http://www.wikidata.org/entity/Q130237433', 'http://www.wikidata.org/entity/Q130237434', 'http://www.wikidata.org/entity/Q130237435', 'http://www.wikidata.org/entity/Q130237436', 'http://www.wikidata.org/entity/Q130237437', 'http://www.wikidata.org/entity/Q130237438', 'http://www.wikidata.org/entity/Q130237439', 'http://www.wikidata.org/entity/Q130237440', 'http://www.wikidata.org/entity/Q130237441', 'http://www.wikidata.org/entity/Q130237442', 'http://www.wikidata.org/entity/Q130237443', 'http://www.wikidata.org/entity/Q130237444', 'http://www.wikidata.org/entity/Q130237445', 'http://www.wikidata.org/entity/Q130237446', 'http://www.wikidata.org/entity/Q130237447', 'http://www.wikidata.org/entity/Q130237448', 'http://www.wikidata.org/entity/Q130237449', 'http://www.wikidata.org/entity/Q130237450', 'http://www.wikidata.org/entity/Q130237451', 'http://www.wikidata.org/entity/Q130237452', 'http://www.wikidata.org/entity/Q130237453', 'http://www.wikidata.org/entity/Q130237454', 'http://www.wikidata.org/entity/Q130237455', 'http://www.wikidata.org/entity/Q130237456', 'http://www.wikidata.org/entity/Q130237457', 'http://www.wikidata.org/entity/Q130237458', 'http://www.wikidata.org/entity/Q130237459', 'http://www.wikidata.org/entity/Q130237460', 'http://www.wikidata.org/entity/Q130237461', 'http://www.wikidata.org/entity/Q130237462', 'http://www.wikidata.org/entity/Q130237463', 'http://www.wikidata.org/entity/Q130237464', 'http://www.wikidata.org/entity/Q130237465', 'http://www.wikidata.org/entity/Q130237466', 'http://www.wikidata.org/entity/Q130237467', 'http://www.wikidata.org/entity/Q130237468', 'http://www.wikidata.org/entity/Q130237469', 'http://www.wikidata.org/entity/Q130237471', 'http://www.wikidata.org/entity/Q130237472', 'http://www.wikidata.org/entity/Q130237473', 'http://www.wikidata.org/entity/Q130237474', 'http://www.wikidata.org/entity/Q130237475', 'http://www.wikidata.org/entity/Q130237476', 'http://www.wikidata.org/entity/Q130237477', 'http://www.wikidata.org/entity/Q130237478', 'http://www.wikidata.org/entity/Q130237479', 'http://www.wikidata.org/entity/Q130237480', 'http://www.wikidata.org/entity/Q130237481', 'http://www.wikidata.org/entity/Q130237482', 'http://www.wikidata.org/entity/Q130237484', 'http://www.wikidata.org/entity/Q130237485', 'http://www.wikidata.org/entity/Q130237487', 'http://www.wikidata.org/entity/Q130237488', 'http://www.wikidata.org/entity/Q130237489', 'http://www.wikidata.org/entity/Q130237490', 'http://www.wikidata.org/entity/Q130237491', 'http://www.wikidata.org/entity/Q130237492', 'http://www.wikidata.org/entity/Q130237493', 'http://www.wikidata.org/entity/Q130237494', 'http://www.wikidata.org/entity/Q130237495', 'http://www.wikidata.org/entity/Q130237496', 'http://www.wikidata.org/entity/Q130237497', 'http://www.wikidata.org/entity/Q130237498', 'http://www.wikidata.org/entity/Q130237499', 'http://www.wikidata.org/entity/Q130237500', 'http://www.wikidata.org/entity/Q130237501', 'http://www.wikidata.org/entity/Q130237502', 'http://www.wikidata.org/entity/Q130237503', 'http://www.wikidata.org/entity/Q130237504', 'http://www.wikidata.org/entity/Q130237505', 'http://www.wikidata.org/entity/Q130237506', 'http://www.wikidata.org/entity/Q130237507', 'http://www.wikidata.org/entity/Q130237508', 'http://www.wikidata.org/entity/Q130237509', 'http://www.wikidata.org/entity/Q130237510', 'http://www.wikidata.org/entity/Q130237511', 'http://www.wikidata.org/entity/Q130237513', 'http://www.wikidata.org/entity/Q130237514', 'http://www.wikidata.org/entity/Q130237515', 'http://www.wikidata.org/entity/Q130237516', 'http://www.wikidata.org/entity/Q130237517', 'http://www.wikidata.org/entity/Q130237518', 'http://www.wikidata.org/entity/Q130237520', 'http://www.wikidata.org/entity/Q130237521', 'http://www.wikidata.org/entity/Q130237522', 'http://www.wikidata.org/entity/Q130237524', 'http://www.wikidata.org/entity/Q130237525', 'http://www.wikidata.org/entity/Q130237526', 'http://www.wikidata.org/entity/Q130237527', 'http://www.wikidata.org/entity/Q130237529', 'http://www.wikidata.org/entity/Q130237530', 'http://www.wikidata.org/entity/Q130237531', 'http://www.wikidata.org/entity/Q130237532', 'http://www.wikidata.org/entity/Q130237534', 'http://www.wikidata.org/entity/Q130237535', 'http://www.wikidata.org/entity/Q130237536', 'http://www.wikidata.org/entity/Q130237537', 'http://www.wikidata.org/entity/Q130237538', 'http://www.wikidata.org/entity/Q130237539', 'http://www.wikidata.org/entity/Q130237540', 'http://www.wikidata.org/entity/Q130237541', 'http://www.wikidata.org/entity/Q130237542', 'http://www.wikidata.org/entity/Q130237543', 'http://www.wikidata.org/entity/Q130237544', 'http://www.wikidata.org/entity/Q130237545', 'http://www.wikidata.org/entity/Q130237546', 'http://www.wikidata.org/entity/Q130237547', 'http://www.wikidata.org/entity/Q130237548', 'http://www.wikidata.org/entity/Q130237549', 'http://www.wikidata.org/entity/Q130237550', 'http://www.wikidata.org/entity/Q130237552', 'http://www.wikidata.org/entity/Q130237553', 'http://www.wikidata.org/entity/Q130237554', 'http://www.wikidata.org/entity/Q130237555', 'http://www.wikidata.org/entity/Q130237556', 'http://www.wikidata.org/entity/Q130237557', 'http://www.wikidata.org/entity/Q130237558', 'http://www.wikidata.org/entity/Q130237559', 'http://www.wikidata.org/entity/Q130237560', 'http://www.wikidata.org/entity/Q130237561', 'http://www.wikidata.org/entity/Q130237562', 'http://www.wikidata.org/entity/Q130237563', 'http://www.wikidata.org/entity/Q130237564', 'http://www.wikidata.org/entity/Q130237565', 'http://www.wikidata.org/entity/Q130237566', 'http://www.wikidata.org/entity/Q130237567', 'http://www.wikidata.org/entity/Q130237570', 'http://www.wikidata.org/entity/Q130237571', 'http://www.wikidata.org/entity/Q130237572', 'http://www.wikidata.org/entity/Q130237573', 'http://www.wikidata.org/entity/Q130237574', 'http://www.wikidata.org/entity/Q130237575', 'http://www.wikidata.org/entity/Q130237576', 'http://www.wikidata.org/entity/Q130237577', 'http://www.wikidata.org/entity/Q130237578', 'http://www.wikidata.org/entity/Q130237579', 'http://www.wikidata.org/entity/Q130237581', 'http://www.wikidata.org/entity/Q130237582', 'http://www.wikidata.org/entity/Q130237584', 'http://www.wikidata.org/entity/Q130237585', 'http://www.wikidata.org/entity/Q130237587', 'http://www.wikidata.org/entity/Q130237588', 'http://www.wikidata.org/entity/Q130237589', 'http://www.wikidata.org/entity/Q130237591', 'http://www.wikidata.org/entity/Q130237592', 'http://www.wikidata.org/entity/Q130237593', 'http://www.wikidata.org/entity/Q130237594', 'http://www.wikidata.org/entity/Q130237597', 'http://www.wikidata.org/entity/Q130237598', 'http://www.wikidata.org/entity/Q130237599', 'http://www.wikidata.org/entity/Q130237601', 'http://www.wikidata.org/entity/Q130237602', 'http://www.wikidata.org/entity/Q130237603', 'http://www.wikidata.org/entity/Q130237604', 'http://www.wikidata.org/entity/Q130237605', 'http://www.wikidata.org/entity/Q130237607', 'http://www.wikidata.org/entity/Q130237608', 'http://www.wikidata.org/entity/Q130237609', 'http://www.wikidata.org/entity/Q130237611', 'http://www.wikidata.org/entity/Q130237612', 'http://www.wikidata.org/entity/Q130237613', 'http://www.wikidata.org/entity/Q130237615', 'http://www.wikidata.org/entity/Q130237616', 'http://www.wikidata.org/entity/Q130237617', 'http://www.wikidata.org/entity/Q130237618', 'http://www.wikidata.org/entity/Q130237619', 'http://www.wikidata.org/entity/Q130237620', 'http://www.wikidata.org/entity/Q130237621', 'http://www.wikidata.org/entity/Q130237623', 'http://www.wikidata.org/entity/Q130237624', 'http://www.wikidata.org/entity/Q130237625', 'http://www.wikidata.org/entity/Q130237626', 'http://www.wikidata.org/entity/Q130237627', 'http://www.wikidata.org/entity/Q130237628', 'http://www.wikidata.org/entity/Q130237629', 'http://www.wikidata.org/entity/Q130237630', 'http://www.wikidata.org</t>
+        </is>
+      </c>
+      <c r="D30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Who wrote the Game of Thrones theme?</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q57577']</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q57577']</t>
+        </is>
+      </c>
+      <c r="D31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Give me all people that were born in Vienna and died in Berlin.</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q95199838', 'http://www.wikidata.org/entity/Q55451835', 'http://www.wikidata.org/entity/Q19966956', 'http://www.wikidata.org/entity/Q125207247', 'http://www.wikidata.org/entity/Q11764172', 'http://www.wikidata.org/entity/Q105047314', 'http://www.wikidata.org/entity/Q124369289', 'http://www.wikidata.org/entity/Q114245296', 'http://www.wikidata.org/entity/Q129847804', 'http://www.wikidata.org/entity/Q106689415', 'http://www.wikidata.org/entity/Q125168660', 'http://www.wikidata.org/entity/Q125134505', 'http://www.wikidata.org/entity/Q125141527', 'http://www.wikidata.org/entity/Q13578778', 'http://www.wikidata.org/entity/Q12271681', 'http://www.wikidata.org/entity/Q105953781', 'http://www.wikidata.org/entity/Q1234160', 'http://www.wikidata.org/entity/Q100706635', 'http://www.wikidata.org/entity/Q123474414', 'http://www.wikidata.org/entity/Q126418132', 'http://www.wikidata.org/entity/Q128222132', 'http://www.wikidata.org/entity/Q1360278', 'http://www.wikidata.org/entity/Q128209458', 'http://www.wikidata.org/entity/Q125224535', 'http://www.wikidata.org/entity/Q125207322', 'http://www.wikidata.org/entity/Q113027456', 'http://www.wikidata.org/entity/Q128255861', 'http://www.wikidata.org/entity/Q105953', 'http://www.wikidata.org/entity/Q1246642', 'http://www.wikidata.org/entity/Q109745', 'http://www.wikidata.org/entity/Q114557', 'http://www.wikidata.org/entity/Q124365519', 'http://www.wikidata.org/entity/Q125381657', 'http://www.wikidata.org/entity/Q11923016', 'http://www.wikidata.org/entity/Q124821984', 'http://www.wikidata.org/entity/Q124823586', 'http://www.wikidata.org/entity/Q1289012', 'http://www.wikidata.org/entity/Q110162770', 'http://www.wikidata.org/entity/Q124823640', 'http://www.wikidata.org/entity/Q1338621', 'http://www.wikidata.org/entity/Q124825392', 'http://www.wikidata.org/entity/Q112057', 'http://www.wikidata.org/entity/Q124826025', 'http://www.wikidata.org/entity/Q124821935', 'http://www.wikidata.org/entity/Q124826477', 'http://www.wikidata.org/entity/Q124827127', 'http://www.wikidata.org/entity/Q124834393', 'http://www.wikidata.org/entity/Q124835415', 'http://www.wikidata.org/entity/Q1036737', 'http://www.wikidata.org/entity/Q1336307', 'http://www.wikidata.org/entity/Q112376', 'http://www.wikidata.org/entity/Q124959174', 'http://www.wikidata.org/entity/Q124798509', 'http://www.wikidata.org/entity/Q124848868', 'http://www.wikidata.org/entity/Q1336841', 'http://www.wikidata.org/entity/Q111241', 'http://www.wikidata.org/entity/Q124747852', 'http://www.wikidata.org/entity/Q1604844', 'http://www.wikidata.org/entity/Q1558906', 'http://www.wikidata.org/entity/Q1510986', 'http://www.wikidata.org/entity/Q16029991', 'http://www.wikidata.org/entity/Q1449083', 'http://www.wikidata.org/entity/Q1735870', 'http://www.wikidata.org/entity/Q1449370', 'http://www.wikidata.org/entity/Q18508198', 'http://www.wikidata.org/entity/Q1379473', 'http://www.wikidata.org/entity/Q15439910', 'http://www.wikidata.org/entity/Q1546037', 'http://www.wikidata.org/entity/Q1555666', 'http://www.wikidata.org/entity/Q1707482', 'http://www.wikidata.org/entity/Q18508531', 'http://www.wikidata.org/entity/Q1465742', 'http://www.wikidata.org/entity/Q1379309', 'http://www.wikidata.org/entity/Q18029152', 'http://www.wikidata.org/entity/Q1708747', 'http://www.wikidata.org/entity/Q1705540', 'http://www.wikidata.org/entity/Q14842646', 'http://www.wikidata.org/entity/Q1484506', 'http://www.wikidata.org/entity/Q1501097', 'http://www.wikidata.org/entity/Q1691423', 'http://www.wikidata.org/entity/Q1500209', 'http://www.wikidata.org/entity/Q1614614', 'http://www.wikidata.org/entity/Q1732733', 'http://www.wikidata.org/entity/Q16663352', 'http://www.wikidata.org/entity/Q1527091', 'http://www.wikidata.org/entity/Q18027381', 'http://www.wikidata.org/entity/Q1579455', 'http://www.wikidata.org/entity/Q15430458', 'http://www.wikidata.org/entity/Q15810299', 'http://www.wikidata.org/entity/Q1581174', 'http://www.wikidata.org/entity/Q1505019', 'http://www.wikidata.org/entity/Q1446365', 'http://www.wikidata.org/entity/Q18223339', 'http://www.wikidata.org/entity/Q1414628', 'http://www.wikidata.org/entity/Q1701554', 'http://www.wikidata.org/entity/Q15979728', 'http://www.wikidata.org/entity/Q1707099', 'http://www.wikidata.org/entity/Q1570857', 'http://www.wikidata.org/entity/Q1781063', 'http://www.wikidata.org/entity/Q1368561', 'http://www.wikidata.org/entity/Q15734397', 'http://www.wikidata.org/entity/Q1511264', 'http://www.wikidata.org/entity/Q15452195', 'http://www.wikidata.org/entity/Q1819735', 'http://www.wikidata.org/entity/Q1903438', 'http://www.wikidata.org/entity/Q22249925', 'http://www.wikidata.org/entity/Q22482410', 'http://www.wikidata.org/entity/Q19288504', 'http://www.wikidata.org/entity/Q55675291', 'http://www.wikidata.org/entity/Q55676433', 'http://www.wikidata.org/entity/Q2588636', 'http://www.wikidata.org/entity/Q2517436', 'http://www.wikidata.org/entity/Q550639', 'http://www.wikidata.org/entity/Q4058928', 'http://www.wikidata.org/entity/Q20801784', 'http://www.wikidata.org/entity/Q2077276', 'http://www.wikidata.org/entity/Q475749', 'http://www.wikidata.org/entity/Q28999', 'http://www.wikidata.org/entity/Q2581891', 'http://www.wikidata.org/entity/Q2040666', 'http://www.wikidata.org/entity/Q19273686', 'http://www.wikidata.org/entity/Q194563', 'http://www.wikidata.org/entity/Q4191716', 'http://www.wikidata.org/entity/Q551155', 'http://www.wikidata.org/entity/Q493058', 'http://www.wikidata.org/entity/Q27672503', 'http://www.wikidata.org/entity/Q54862358', 'http://www.wikidata.org/entity/Q43378651', 'http://www.wikidata.org/entity/Q2645934', 'http://www.wikidata.org/entity/Q326252', 'http://www.wikidata.org/entity/Q27670830', 'http://www.wikidata.org/entity/Q36668532', 'http://www.wikidata.org/entity/Q362952', 'http://www.wikidata.org/entity/Q2338888', 'http://www.wikidata.org/entity/Q354466', 'http://www.wikidata.org/entity/Q347559', 'http://www.wikidata.org/entity/Q21168969', 'http://www.wikidata.org/entity/Q20056905', 'http://www.wikidata.org/entity/Q33011834', 'http://www.wikidata.org/entity/Q23928916', 'http://www.wikidata.org/entity/Q51886108', 'http://www.wikidata.org/entity/Q55674501', 'http://www.wikidata.org/entity/Q2020596', 'http://www.wikidata.org/entity/Q51844316', 'http://www.wikidata.org/entity/Q51844339', 'http://www.wikidata.org/entity/Q45927183', 'http://www.wikidata.org/entity/Q1908687', 'http://www.wikidata.org/entity/Q86323', 'http://www.wikidata.org/entity/Q62076483', 'http://www.wikidata.org/entity/Q650151', 'http://www.wikidata.org/entity/Q7782918', 'http://www.wikidata.org/entity/Q94938005', 'http://www.wikidata.org/entity/Q77736', 'http://www.wikidata.org/entity/Q86293', 'http://www.wikidata.org/entity/Q56487519', 'http://www.wikidata.org/entity/Q6373188', 'http://www.wikidata.org/entity/Q94906393', 'http://www.wikidata.org/entity/Q71198', 'http://www.wikidata.org/entity/Q7983614', 'http://www.wikidata.org/entity/Q94753105', 'http://www.wikidata.org/entity/Q94922778', 'http://www.wikidata.org/entity/Q78614', 'http://www.wikidata.org/entity/Q90462', 'http://www.wikidata.org/entity/Q94761001', 'http://www.wikidata.org/entity/Q63485351', 'http://www.wikidata.org/entity/Q85448', 'http://www.wikidata.org/entity/Q94887584', 'http://www.wikidata.org/entity/Q85692', 'http://www.wikidata.org/entity/Q61971231', 'http://www.wikidata.org/entity/Q94040', 'http://www.wikidata.org/entity/Q710106', 'http://www.wikidata.org/entity/Q61930459', 'http://www.wikidata.org/entity/Q94872174', 'http://www.wikidata.org/entity/Q55885976', 'http://www.wikidata.org/entity/Q87698', 'http://www.wikidata.org/entity/Q87595', 'http://www.wikidata.org/entity/Q87593', 'http://www.wikidata.org/entity/Q87498', 'http://www.wikidata.org/entity/Q60820294', 'http://www.wikidata.org/entity/Q60822973', 'http://www.wikidata.org/entity/Q96452', 'http://www.wikidata.org/entity/Q95227952', 'http://www.wikidata.org/entity/Q88140', 'http://www.wikidata.org/entity/Q95249180', 'http://www.wikidata.org/entity/Q911548', 'http://www.wikidata.org/entity/Q89164', 'http://www.wikidata.org/entity/Q55681103', 'http://www.wikidata.org/entity/Q872165', 'http://www.wikidata.org/entity/Q94731605', 'http://www.wikidata.org/entity/Q95805826', 'http://www.wikidata.org/entity/Q60528', 'http://www.wikidata.org/entity/Q76143', 'http://www.wikidata.org/entity/Q95389052', 'http://www.wikidata.org/entity/Q88627', 'http://www.wikidata.org/entity/Q86718', 'http://www.wikidata.org/entity/Q88835', 'http://www.wikidata.org/entity/Q86516', 'http://www.wikidata.org/entity/Q94777816', 'http://www.wikidata.org/entity/Q90014', 'http://www.wikidata.org/entity/Q94577', 'http://www.wikidata.org/entity/Q57385917', 'http://www.wikidata.org/entity/Q24078', 'http://www.wikidata.org/entity/Q1441046', 'http://www.wikidata.org/entity/Q16563052', 'http://www.wikidata.org/entity/Q87735', 'http://www.wikidata.org/entity/Q111031308', 'http://www.wikidata.org/entity/Q125347249', 'http://www.wikidata.org/entity/Q112469746', 'http://www.wikidata.org/entity/Q15436531', 'http://www.wikidata.org/entity/Q1468949', 'http://www.wikidata.org/entity/Q1604844', 'http://www.wikidata.org/entity/Q5946570', 'http://www.wikidata.org/entity/Q43382717', 'http://www.wikidata.org/entity/Q85051', 'http://www.wikidata.org/entity/Q78934', 'http://www.wikidata.org/entity/Q697055', 'http://www.wikidata.org/entity/Q113027456', 'http://www.wikidata.org/entity/Q124369289', 'http://www.wikidata.org/entity/Q111241', 'http://www.wikidata.org/entity/Q105047314', 'http://www.wikidata.org/entity/Q11923016', 'http://www.wikidata.org/entity/Q114245296', 'http://www.wikidata.org/entity/Q114557', 'http://www.wikidata.org/entity/Q112057', 'http://www.wikidata.org/entity/Q109745', 'http://www.wikidata.org/entity/Q124365519', 'http://www.wikidata.org/entity/Q1234160', 'http://www.wikidata.org/entity/Q11764172', 'http://www.wikidata.org/entity/Q105953', 'http://www.wikidata.org/entity/Q12271681', 'http://www.wikidata.org/entity/Q105953781', 'http://www.wikidata.org/entity/Q112376', 'http://www.wikidata.org/entity/Q1246642', 'http://www.wikidata.org/entity/Q106689415', 'http://www.wikidata.org/entity/Q123474414', 'http://www.wikidata.org/entity/Q100706635', 'http://www.wikidata.org/entity/Q110162770', 'http://www.wikidata.org/entity/Q1036737', 'http://www.wikidata.org/entity/Q21168969', 'http://www.wikidata.org/entity/Q2020596', 'http://www.wikidata.org/entity/Q128255861', 'http://www.wikidata.org/entity/Q125207322', 'http://www.wikidata.org/entity/Q124823640', 'http://www.wikidata.org/entity/Q124827127', 'http://www.wikidata.org/entity/Q124798509', 'http://www.wikidata.org/entity/Q2040666', 'http://www.wikidata.org/entity/Q128222132', 'http://www.wikidata.org/entity/Q124825392', 'http://www.wikidata.org/entity/Q20056905', 'http://www.wikidata.org/entity/Q128209458', 'http://www.wikidata.org/entity/Q124826025', 'http://www.wikidata.org/entity/Q125141527', 'http://www.wikidata.org/entity/Q124821935', 'http://www.wikidata.org/entity/Q124821984', 'http://www.wikidata.org/entity/Q125381657', 'http://www.wikidata.org/entity/Q125224535', 'http://www.wikidata.org/entity/Q126418132', 'http://www.wikidata.org/entity/Q125134505', 'http://www.wikidata.org/entity/Q124747852', 'http://www.wikidata.org/entity/Q124848868', 'http://www.wikidata.org/entity/Q124835415', 'http://www.wikidata.org/entity/Q125207247', 'http://www.wikidata.org/entity/Q124834393', 'http://www.wikidata.org/entity/Q20801784', 'http://www.wikidata.org/entity/Q124823586', 'http://www.wikidata.org/entity/Q125168660', 'http://www.wikidata.org/entity/Q2077276', 'http://www.wikidata.org/entity/Q124959174', 'http://www.wikidata.org/entity/Q124826477', 'http://www.wikidata.org/entity/Q1379309', 'http://www.wikidata.org/entity/Q16029991', 'http://www.wikidata.org/entity/Q1707099', 'http://www.wikidata.org/entity/Q18508531', 'http://www.wikidata.org/entity/Q19273686', 'http://www.wikidata.org/entity/Q1449083', 'http://www.wikidata.org/entity/Q1449370', 'http://www.wikidata.org/entity/Q1705540', 'http://www.wikidata.org/entity/Q15979728', 'http://www.wikidata.org/entity/Q1701554', 'http://www.wikidata.org/entity/Q15439910', 'http://www.wikidata.org/entity/Q1338621', 'http://www.wikidata.org/entity/Q1465742', 'http://www.wikidata.org/entity/Q1691423', 'http://www.wikidata.org/entity/Q1336841', 'http://www.wikidata.org/entity/Q15430458', 'http://www.wikidata.org/entity/Q18508198', 'http://www.wikidata.org/entity/Q14842646', 'http://www.wikidata.org/entity/Q1908687', 'http://www.wikidata.org/entity/Q1484506', 'http://www.wikidata.org/entity/Q1903438', 'http://www.wikidata.org/entity/Q1604844', 'http://www.wikidata.org/entity/Q1527091', 'http://www.wikidata.org/entity/Q1336307', 'http://www.wikidata.org/entity/Q16663352', 'http://www.wikidata.org/entity/Q1500209', 'http://www.wikidata.org/entity/Q1614614', 'http://www.wikidata.org/entity/Q1501097', 'http://www.wikidata.org/entity/Q1511264', 'http://www.wikidata.org/entity/Q1510986', 'http://www.wikidata.org/entity/Q1505019', 'http://www.wikidata.org/entity/Q13578778', 'http://www.wikidata.org/entity/Q1570857', 'http://www.wikidata.org/entity/Q1360278', 'http://www.wikidata.org/entity/Q15734397', 'http://www.wikidata.org/entity/Q18027381', 'http://www.wikidata.org/entity/Q1368561', 'http://www.wikidata.org/entity/Q1579455', 'http://www.wikidata.org/entity/Q1558906', 'http://www.wikidata.org/entity/Q1781063', 'http://www.wikidata.org/entity/Q15810299', 'http://www.wikidata.org/entity/Q1819735', 'http://www.wikidata.org/entity/Q1379473', 'http://www.wikidata.org/entity/Q1289012', 'http://www.wikidata.org/entity/Q1581174', 'http://www.wikidata.org/entity/Q19288504', 'http://www.wikidata.org/entity/Q1735870', 'http://www.wikidata.org/entity/Q194563', 'http://www.wikidata.org/entity/Q1414628', 'http://www.wikidata.org/entity/Q1555666', 'http://www.wikidata.org/entity/Q1732733', 'http://www.wikidata.org/entity/Q129847804', 'http://www.wikidata.org/entity/Q18223339', 'http://www.wikidata.org/entity/Q1546037', 'http://www.wikidata.org/entity/Q1446365', 'http://www.wikidata.org/entity/Q1708747', 'http://www.wikidata.org/entity/Q1707482', 'http://www.wikidata.org/entity/Q15452195', 'http://www.wikidata.org/entity/Q18029152', 'http://www.wikidata.org/entity/Q493058', 'http://www.wikidata.org/entity/Q55681103', 'http://www.wikidata.org/entity/Q2581891', 'http://www.wikidata.org/entity/Q33011834', 'http://www.wikidata.org/entity/Q22249925', 'http://www.wikidata.org/entity/Q2338888', 'http://www.wikidata.org/entity/Q36668532', 'http://www.wikidata.org/entity/Q51886108', 'http://www.wikidata.org/entity/Q22482410', 'http://www.wikidata.org/entity/Q2588636', 'http://www.wikidata.org/entity/Q475749', 'http://www.wikidata.org/entity/Q43378651', 'http://www.wikidata.org/entity/Q51844339', 'http://www.wikidata.org/entity/Q362952', 'http://www.wikidata.org/entity/Q51844316', 'http://www.wikidata.org/entity/Q354466', 'http://www.wikidata.org/entity/Q60528', 'http://www.wikidata.org/entity/Q2645934', 'http://www.wikidata.org/entity/Q45927183', 'http://www.wikidata.org/entity/Q347559', 'http://www.wikidata.org/entity/Q4058928', 'http://www.wikidata.org/entity/Q2517436', 'http://www.wikidata.org/entity/Q28999', 'http://www.wikidata.org/entity/Q55676433', 'http://www.wikidata.org/entity/Q57385917', 'http://www.wikidata.org/entity/Q27672503', 'http://www.wikidata.org/entity/Q27670830', 'http://www.wikidata.org/entity/Q54862358', 'http://www.wikidata.org/entity/Q23928916', 'http://www.wikidata.org/entity/Q55674501', 'http://www.wikidata.org/entity/Q550639', 'http://www.wikidata.org/entity/Q326252', 'http://www.wikidata.org/entity/Q56487519', 'http://www.wikidata.org/entity/Q551155', 'http://www.wikidata.org/entity/Q55675291', 'http://www.wikidata.org/entity/Q4191716', 'http://www.wikidata.org/entity/Q55885976', 'http://www.wikidata.org/entity/Q911548', 'http://www.wikidata.org/entity/Q71198', 'http://www.wikidata.org/entity/Q94761001', 'http://www.wikidata.org/entity/Q78614', 'http://www.wikidata.org/entity/Q94906393', 'http://www.wikidata.org/entity/Q61930459', 'http://www.wikidata.org/entity/Q90014', 'http://www.wikidata.org/entity/Q94777816', 'http://www.wikidata.org/entity/Q63485351', 'http://www.wikidata.org/entity/Q88835', 'http://www.wikidata.org/entity/Q94938005', 'http://www.wikidata.org/entity/Q87698', 'http://www.wikidata.org/entity/Q88627', 'http://www.wikidata.org/entity/Q94577', 'http://www.wikidata.org/entity/Q60822973', 'http://www.wikidata.org/entity/Q95249180', 'http://www.wikidata.org/entity/Q85692', 'http://www.wikidata.org/entity/Q94872174', 'http://www.wikidata.org/entity/Q76143', 'http://www.wikidata.org/entity/Q94887584', 'http://www.wikidata.org/entity/Q85448', 'http://www.wikidata.org/entity/Q60820294', 'http://www.wikidata.org/entity/Q77736', 'http://www.wikidata.org/entity/Q6373188', 'http://www.wikidata.org/entity/Q88140', 'http://www.wikidata.org/entity/Q95389052', 'http://www.wikidata.org/entity/Q94731605', 'http://www.wikidata.org/entity/Q7782918', 'http://www.wikidata.org/entity/Q710106', 'http://www.wikidata.org/entity/Q86293', 'http://www.wikidata.org/entity/Q96452', 'http://www.wikidata.org/entity/Q86718', 'http://www.wikidata.org/entity/Q7983614', 'http://www.wikidata.org/entity/Q86516', 'http://www.wikidata.org/entity/Q90462', 'http://www.wikidata.org/entity/Q94922778', 'http://www.wikidata.org/entity/Q61971231', 'http://www.wikidata.org/entity/Q872165', 'http://www.wikidata.org/entity/Q86323', 'http://www.wikidata.org/entity/Q89164', 'http://www.wikidata.org/entity/Q62076483', 'http://www.wikidata.org/entity/Q94040', 'http://www.wikidata.org/entity/Q650151', 'http://www.wikidata.org/entity/Q87498', 'http://www.wikidata.org/entity/Q95805826', 'http://www.wikidata.org/entity/Q95227952', 'http://www.wikidata.org/entity/Q94753105', 'http://www.wikidata.org/entity/Q87593', 'http://www.wikidata.org/entity/Q87595', 'http://www.wikidata.org/entity/Q33011834', 'http://www.wikidata.org/entity/Q55682962', 'http://www.wikidata.org/entity/Q12028148', 'http://www.wikidata.org/entity/Q19309506', 'http://www.wikidata.org/entity/Q78793', 'http://www.wikidata.org/entity/Q2173626', 'http://www.wikidata.org/entity/Q51844338', 'http://www.wikidata.org/entity/Q61199008', 'http://www.wikidata.org/entity/Q94743563']</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q100706635', 'http://www.wikidata.org/entity/Q1036737', 'http://www.wikidata.org/entity/Q105047314', 'http://www.wikidata.org/entity/Q105953', 'http://www.wikidata.org/entity/Q105953781', 'http://www.wikidata.org/entity/Q106689415', 'http://www.wikidata.org/entity/Q109745', 'http://www.wikidata.org/entity/Q110162770', 'http://www.wikidata.org/entity/Q111241', 'http://www.wikidata.org/entity/Q112057', 'http://www.wikidata.org/entity/Q112376', 'http://www.wikidata.org/entity/Q113027456', 'http://www.wikidata.org/entity/Q114245296', 'http://www.wikidata.org/entity/Q114557', 'http://www.wikidata.org/entity/Q11764172', 'http://www.wikidata.org/entity/Q11923016', 'http://www.wikidata.org/entity/Q12271681', 'http://www.wikidata.org/entity/Q1234160', 'http://www.wikidata.org/entity/Q123474414', 'http://www.wikidata.org/entity/Q124365519', 'http://www.wikidata.org/entity/Q124369289', 'http://www.wikidata.org/entity/Q1246642', 'http://www.wikidata.org/entity/Q124747852', 'http://www.wikidata.org/entity/Q124798509', 'http://www.wikidata.org/entity/Q124821935', 'http://www.wikidata.org/entity/Q124821984', 'http://www.wikidata.org/entity/Q124823586', 'http://www.wikidata.org/entity/Q124823640', 'http://www.wikidata.org/entity/Q124825392', 'http://www.wikidata.org/entity/Q124826025', 'http://www.wikidata.org/entity/Q124826477', 'http://www.wikidata.org/entity/Q124827127', 'http://www.wikidata.org/entity/Q124834393', 'http://www.wikidata.org/entity/Q124835415', 'http://www.wikidata.org/entity/Q124848868', 'http://www.wikidata.org/entity/Q124959174', 'http://www.wikidata.org/entity/Q125134505', 'http://www.wikidata.org/entity/Q125141527', 'http://www.wikidata.org/entity/Q125168660', 'http://www.wikidata.org/entity/Q125207247', 'http://www.wikidata.org/entity/Q125207322', 'http://www.wikidata.org/entity/Q125224535', 'http://www.wikidata.org/entity/Q125381657', 'http://www.wikidata.org/entity/Q126418132', 'http://www.wikidata.org/entity/Q128209458', 'http://www.wikidata.org/entity/Q128222132', 'http://www.wikidata.org/entity/Q128255861', 'http://www.wikidata.org/entity/Q1289012', 'http://www.wikidata.org/entity/Q129847804', 'http://www.wikidata.org/entity/Q1336307', 'http://www.wikidata.org/entity/Q1336841', 'http://www.wikidata.org/entity/Q1338621', 'http://www.wikidata.org/entity/Q13578778', 'http://www.wikidata.org/entity/Q1360278', 'http://www.wikidata.org/entity/Q1368561', 'http://www.wikidata.org/entity/Q1379309', 'http://www.wikidata.org/entity/Q1379473', 'http://www.wikidata.org/entity/Q1414628', 'http://www.wikidata.org/entity/Q1446365', 'http://www.wikidata.org/entity/Q1449083', 'http://www.wikidata.org/entity/Q1449370', 'http://www.wikidata.org/entity/Q1465742', 'http://www.wikidata.org/entity/Q14842646', 'http://www.wikidata.org/entity/Q1484506', 'http://www.wikidata.org/entity/Q1500209', 'http://www.wikidata.org/entity/Q1501097', 'http://www.wikidata.org/entity/Q1505019', 'http://www.wikidata.org/entity/Q1510986', 'http://www.wikidata.org/entity/Q1511264', 'http://www.wikidata.org/entity/Q1527091', 'http://www.wikidata.org/entity/Q15430458', 'http://www.wikidata.org/entity/Q15439910', 'http://www.wikidata.org/entity/Q15452195', 'http://www.wikidata.org/entity/Q1546037', 'http://www.wikidata.org/entity/Q1555666', 'http://www.wikidata.org/entity/Q1558906', 'http://www.wikidata.org/entity/Q1570857', 'http://www.wikidata.org/entity/Q15734397', 'http://www.wikidata.org/entity/Q1579455', 'http://www.wikidata.org/entity/Q15810299', 'http://www.wikidata.org/entity/Q1581174', 'http://www.wikidata.org/entity/Q15979728', 'http://www.wikidata.org/entity/Q16029991', 'http://www.wikidata.org/entity/Q1604844', 'http://www.wikidata.org/entity/Q1614614', 'http://www.wikidata.org/entity/Q16663352', 'http://www.wikidata.org/entity/Q1691423', 'http://www.wikidata.org/entity/Q1701554', 'http://www.wikidata.org/entity/Q1705540', 'http://www.wikidata.org/entity/Q1707099', 'http://www.wikidata.org/entity/Q1707482', 'http://www.wikidata.org/entity/Q1708747', 'http://www.wikidata.org/entity/Q1732733', 'http://www.wikidata.org/entity/Q1735870', 'http://www.wikidata.org/entity/Q1781063', 'http://www.wikidata.org/entity/Q18027381', 'http://www.wikidata.org/entity/Q18029152', 'http://www.wikidata.org/entity/Q1819735', 'http://www.wikidata.org/entity/Q18223339', 'http://www.wikidata.org/entity/Q18508198', 'http://www.wikidata.org/entity/Q18508531', 'http://www.wikidata.org/entity/Q1903438', 'http://www.wikidata.org/entity/Q1908687', 'http://www.wikidata.org/entity/Q19273686', 'http://www.wikidata.org/entity/Q19288504', 'http://www.wikidata.org/entity/Q194563', 'http://www.wikidata.org/entity/Q20056905', 'http://www.wikidata.org/entity/Q2020596', 'http://www.wikidata.org/entity/Q2040666', 'http://www.wikidata.org/entity/Q2077276', 'http://www.wikidata.org/entity/Q20801784', 'http://www.wikidata.org/entity/Q21168969', 'http://www.wikidata.org/entity/Q22249925', 'http://www.wikidata.org/entity/Q22482410', 'http://www.wikidata.org/entity/Q2338888', 'http://www.wikidata.org/entity/Q23928916', 'http://www.wikidata.org/entity/Q2517436', 'http://www.wikidata.org/entity/Q2581891', 'http://www.wikidata.org/entity/Q2588636', 'http://www.wikidata.org/entity/Q2645934', 'http://www.wikidata.org/entity/Q27670830', 'http://www.wikidata.org/entity/Q27672503', 'http://www.wikidata.org/entity/Q28999', 'http://www.wikidata.org/entity/Q326252', 'http://www.wikidata.org/entity/Q33011834', 'http://www.wikidata.org/entity/Q347559', 'http://www.wikidata.org/entity/Q354466', 'http://www.wikidata.org/entity/Q362952', 'http://www.wikidata.org/entity/Q36668532', 'http://www.wikidata.org/entity/Q4058928', 'http://www.wikidata.org/entity/Q4191716', 'http://www.wikidata.org/entity/Q43378651', 'http://www.wikidata.org/entity/Q45927183', 'http://www.wikidata.org/entity/Q475749', 'http://www.wikidata.org/entity/Q493058', 'http://www.wikidata.org/entity/Q51844316', 'http://www.wikidata.org/entity/Q51844339', 'http://www.wikidata.org/entity/Q51886108', 'http://www.wikidata.org/entity/Q54862358', 'http://www.wikidata.org/entity/Q550639', 'http://www.wikidata.org/entity/Q551155', 'http://www.wikidata.org/entity/Q55674501', 'http://www.wikidata.org/entity/Q55675291', 'http://www.wikidata.org/entity/Q55676433', 'http://www.wikidata.org/entity/Q55681103', 'http://www.wikidata.org/entity/Q55885976', 'http://www.wikidata.org/entity/Q56487519', 'http://www.wikidata.org/entity/Q57385917', 'http://www.wikidata.org/entity/Q60528', 'http://www.wikidata.org/entity/Q60820294', 'http://www.wikidata.org/entity/Q60822973', 'http://www.wikidata.org/entity/Q61930459', 'http://www.wikidata.org/entity/Q61971231', 'http://www.wikidata.org/entity/Q62076483', 'http://www.wikidata.org/entity/Q63485351', 'http://www.wikidata.org/entity/Q6373188', 'http://www.wikidata.org/entity/Q650151', 'http://www.wikidata.org/entity/Q710106', 'http://www.wikidata.org/entity/Q71198', 'http://www.wikidata.org/entity/Q76143', 'http://www.wikidata.org/entity/Q77736', 'http://www.wikidata.org/entity/Q7782918', 'http://www.wikidata.org/entity/Q78614', 'http://www.wikidata.org/entity/Q7983614', 'http://www.wikidata.org/entity/Q85448', 'http://www.wikidata.org/entity/Q85692', 'http://www.wikidata.org/entity/Q86293', 'http://www.wikidata.org/entity/Q86323', 'http://www.wikidata.org/entity/Q86516', 'http://www.wikidata.org/entity/Q86718', 'http://www.wikidata.org/entity/Q872165', 'http://www.wikidata.org/entity/Q87498', 'http://www.wikidata.org/entity/Q87593', 'http://www.wikidata.org/entity/Q87595', 'http://www.wikidata.org/entity/Q87698', 'http://www.wikidata.org/entity/Q88140', 'http://www.wikidata.org/entity/Q88627', 'http://www.wikidata.org/entity/Q88835', 'http://www.wikidata.org/entity/Q89164', 'http://www.wikidata.org/entity/Q90014', 'http://www.wikidata.org/entity/Q90462', 'http://www.wikidata.org/entity/Q911548', 'http://www.wikidata.org/entity/Q94040', 'http://www.wikidata.org/entity/Q94577', 'http://www.wikidata.org/entity/Q94731605', 'http://www.wikidata.org/entity/Q94753105', 'http://www.wikidata.org/entity/Q94761001', 'http://www.wikidata.org/entity/Q94777816', 'http://www.wikidata.org/entity/Q94872174', 'http://www.wikidata.org/entity/Q94887584', 'http://www.wikidata.org/entity/Q94906393', 'http://www.wikidata.org/entity/Q94922778', 'http://www.wikidata.org/entity/Q94938005', 'http://www.wikidata.org/entity/Q95227952', 'http://www.wikidata.org/entity/Q95249180', 'http://www.wikidata.org/entity/Q95389052', 'http://www.wikidata.org/entity/Q95805826', 'http://www.wikidata.org/entity/Q96452']</t>
+        </is>
+      </c>
+      <c r="D32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Who discovered Ceres?</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q14280']</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q14280']</t>
+        </is>
+      </c>
+      <c r="D33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Give me a list of all bandleaders that play trumpet.</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q100249671', 'http://www.wikidata.org/entity/Q1026959', 'http://www.wikidata.org/entity/Q1027629', 'http://www.wikidata.org/entity/Q1036753', 'http://www.wikidata.org/entity/Q1039172', 'http://www.wikidata.org/entity/Q1050088', 'http://www.wikidata.org/entity/Q106959617', 'http://www.wikidata.org/entity/Q109094', 'http://www.wikidata.org/entity/Q110182609', 'http://www.wikidata.org/entity/Q1103685', 'http://www.wikidata.org/entity/Q11290964', 'http://www.wikidata.org/entity/Q1138796', 'http://www.wikidata.org/entity/Q11409656', 'http://www.wikidata.org/entity/Q11473196', 'http://www.wikidata.org/entity/Q116745984', 'http://www.wikidata.org/entity/Q1173729', 'http://www.wikidata.org/entity/Q1238872', 'http://www.wikidata.org/entity/Q124042030', 'http://www.wikidata.org/entity/Q12469951', 'http://www.wikidata.org/entity/Q1248972', 'http://www.wikidata.org/entity/Q1266275', 'http://www.wikidata.org/entity/Q1282429', 'http://www.wikidata.org/entity/Q1282945', 'http://www.wikidata.org/entity/Q1282967', 'http://www.wikidata.org/entity/Q130324694', 'http://www.wikidata.org/entity/Q1308870', 'http://www.wikidata.org/entity/Q1311188', 'http://www.wikidata.org/entity/Q1318323', 'http://www.wikidata.org/entity/Q1347472', 'http://www.wikidata.org/entity/Q13571046', 'http://www.wikidata.org/entity/Q13571677', 'http://www.wikidata.org/entity/Q1364120', 'http://www.wikidata.org/entity/Q1412239', 'http://www.wikidata.org/entity/Q144622', 'http://www.wikidata.org/entity/Q1452661', 'http://www.wikidata.org/entity/Q1453118', 'http://www.wikidata.org/entity/Q14545268', 'http://www.wikidata.org/entity/Q1454645', 'http://www.wikidata.org/entity/Q1535887', 'http://www.wikidata.org/entity/Q15453836', 'http://www.wikidata.org/entity/Q15485363', 'http://www.wikidata.org/entity/Q1557440', 'http://www.wikidata.org/entity/Q15815145', 'http://www.wikidata.org/entity/Q1583816', 'http://www.wikidata.org/entity/Q15840407', 'http://www.wikidata.org/entity/Q15851160', 'http://www.wikidata.org/entity/Q16017359', 'http://www.wikidata.org/entity/Q1607887', 'http://www.wikidata.org/entity/Q16090563', 'http://www.wikidata.org/entity/Q161753', 'http://www.wikidata.org/entity/Q1622068', 'http://www.wikidata.org/entity/Q1631802', 'http://www.wikidata.org/entity/Q163861', 'http://www.wikidata.org/entity/Q1675549', 'http://www.wikidata.org/entity/Q1678838', 'http://www.wikidata.org/entity/Q1687893', 'http://www.wikidata.org/entity/Q1689131', 'http://www.wikidata.org/entity/Q1689347', 'http://www.wikidata.org/entity/Q1691548', 'http://www.wikidata.org/entity/Q1701204', 'http://www.wikidata.org/entity/Q1701748', 'http://www.wikidata.org/entity/Q1702274', 'http://www.wikidata.org/entity/Q1703633', 'http://www.wikidata.org/entity/Q17306038', 'http://www.wikidata.org/entity/Q17352853', 'http://www.wikidata.org/entity/Q1738588', 'http://www.wikidata.org/entity/Q1738949', 'http://www.wikidata.org/entity/Q1740093', 'http://www.wikidata.org/entity/Q1745395', 'http://www.wikidata.org/entity/Q177824', 'http://www.wikidata.org/entity/Q1779', 'http://www.wikidata.org/entity/Q1791341', 'http://www.wikidata.org/entity/Q1806037', 'http://www.wikidata.org/entity/Q1820504', 'http://www.wikidata.org/entity/Q18410973', 'http://www.wikidata.org/entity/Q1872759', 'http://www.wikidata.org/entity/Q188046', 'http://www.wikidata.org/entity/Q1902146', 'http://www.wikidata.org/entity/Q1903353', 'http://www.wikidata.org/entity/Q1912807', 'http://www.wikidata.org/entity/Q1917393', 'http://www.wikidata.org/entity/Q19275122', 'http://www.wikidata.org/entity/Q1935815', 'http://www.wikidata.org/entity/Q193645', 'http://www.wikidata.org/entity/Q19561422', 'http://www.wikidata.org/entity/Q19629147', 'http://www.wikidata.org/entity/Q1971146', 'http://www.wikidata.org/entity/Q19832476', 'http://www.wikidata.org/entity/Q199406', 'http://www.wikidata.org/entity/Q19960682', 'http://www.wikidata.org/entity/Q19962541', 'http://www.wikidata.org/entity/Q19968522', 'http://www.wikidata.org/entity/Q201500', 'http://www.wikidata.org/entity/Q2041252', 'http://www.wikidata.org/entity/Q204943', 'http://www.wikidata.org/entity/Q2061143', 'http://www.wikidata.org/entity/Q2075755', 'http://www.wikidata.org/entity/Q210173', 'http://www.wikidata.org/entity/Q210289', 'http://www.wikidata.org/entity/Q2216444', 'http://www.wikidata.org/entity/Q222798', 'http://www.wikidata.org/entity/Q22670541', 'http://www.wikidata.org/entity/Q22958430', 'http://www.wikidata.org/entity/Q2302261', 'http://www.wikidata.org/entity/Q2347504', 'http://www.wikidata.org/entity/Q23874600', 'http://www.wikidata.org/entity/Q2396601', 'http://www.wikidata.org/entity/Q2401961', 'http://www.wikidata.org/entity/Q2405288', 'http://www.wikidata.org/entity/Q2478090', 'http://www.wikidata.org/entity/Q2544934', 'http://www.wikidata.org/entity/Q26196818', 'http://www.wikidata.org/entity/Q2645829', 'http://www.wikidata.org/entity/Q2686238', 'http://www.wikidata.org/entity/Q273076', 'http://www.wikidata.org/entity/Q276068', 'http://www.wikidata.org/entity/Q27916182', 'http://www.wikidata.org/entity/Q313368', 'http://www.wikidata.org/entity/Q313529', 'http://www.wikidata.org/entity/Q313868', 'http://www.wikidata.org/entity/Q3196381', 'http://www.wikidata.org/entity/Q322210', 'http://www.wikidata.org/entity/Q329362', 'http://www.wikidata.org/entity/Q344822', 'http://www.wikidata.org/entity/Q355481', 'http://www.wikidata.org/entity/Q356715', 'http://www.wikidata.org/entity/Q376146', 'http://www.wikidata.org/entity/Q432924', 'http://www.wikidata.org/entity/Q436176', 'http://www.wikidata.org/entity/Q465105', 'http://www.wikidata.org/entity/Q4760598', 'http://www.wikidata.org/entity/Q4767267', 'http://www.wikidata.org/entity/Q4797599', 'http://www.wikidata.org/entity/Q4833896', 'http://www.wikidata.org/entity/Q491100', 'http://www.wikidata.org/entity/Q4911881', 'http://www.wikidata.org/entity/Q492677', 'http://www.wikidata.org/entity/Q495464', 'http://www.wikidata.org/entity/Q49575', 'http://www.wikidata.org/entity/Q4998586', 'http://www.wikidata.org/entity/Q510651', 'http://www.wikidata.org/entity/Q5214487', 'http://www.wikidata.org/entity/Q5220273', 'http://www.wikidata.org/entity/Q523899', 'http://www.wikidata.org/entity/Q5263018', 'http://www.wikidata.org/entity/Q528340', 'http://www.wikidata.org/entity/Q5290919', 'http://www.wikidata.org/entity/Q539159', 'http://www.wikidata.org/entity/Q5392650', 'http://www.wikidata.org/entity/Q5394010', 'http://www.wikidata.org/entity/Q539883', 'http://www.wikidata.org/entity/Q545464', 'http://www.wikidata.org/entity/Q54957569', 'http://www.wikidata.org/entity/Q5508594', 'http://www.wikidata.org/entity/Q5525190', 'http://www.wikidata.org/entity/Q5531061', 'http://www.wikidata.org/entity/Q558118', 'http://www.wikidata.org/entity/Q562871', 'http://www.wikidata.org/entity/Q5736141', 'http://www.wikidata.org/entity/Q590792', 'http://www.wikidata.org/entity/Q600700', 'http://www.wikidata.org/entity/Q6074256', 'http://www.wikidata.org/entity/Q612855', 'http://www.wikidata.org/entity/Q6175185', 'http://www.wikidata.org/entity/Q6208919', 'http://www.wikidata.org/entity/Q6221178', 'http://www.wikidata.org/entity/Q6224104', 'http://www.wikidata.org/entity/Q6240203', 'http://www.wikidata.org/entity/Q6309190', 'http://www.wikidata.org/entity/Q64683137', 'http://www.wikidata.org/entity/Q64985242', 'http://www.wikidata.org/entity/Q65028314', 'http://www.wikidata.org/entity/Q65028506', 'http://www.wikidata.org/entity/Q65032384', 'http://www.wikidata.org/entity/Q65034989', 'http://www.wikidata.org/entity/Q65034994', 'http://www.wikidata.org/entity/Q658636', 'http://www.wikidata.org/entity/Q6687998', 'http://www.wikidata.org/entity/Q668856', 'http://www.wikidata.org/entity/Q675810', 'http://www.wikidata.org/entity/Q6793340', 'http://www.wikidata.org/entity/Q6846424', 'http://www.wikidata.org/entity/Q6849142', 'http://www.wikidata.org/entity/Q7052586', 'http://www.wikidata.org/entity/Q70552207', 'http://www.wikidata.org/entity/Q7087874', 'http://www.wikidata.org/entity/Q708990', 'http://www.wikidata.org/entity/Q711921', 'http://www.wikidata.org/entity/Q713273', 'http://www.wikidata.org/entity/Q727418', 'http://www.wikidata.org/entity/Q7298839', 'http://www.wikidata.org/entity/Q737521', 'http://www.wikidata.org/entity/Q743585', 'http://www.wikidata.org/entity/Q7441108', 'http://www.wikidata.org/entity/Q7524109', 'http://www.wikidata.org/entity/Q7614243', 'http://www.wikidata.org/entity/Q7694080', 'http://www.wikidata.org/entity/Q772645', 'http://www.wikidata.org/entity/Q776453', 'http://www.wikidata.org/entity/Q7781439', 'http://www.wikidata.org/entity/Q7781727', 'http://www.wikidata.org/entity/Q7924906', 'http://www.wikidata.org/entity/Q7982390', 'http://www.wikidata.org/entity/Q8009347', 'http://www.wikidata.org/entity/Q807401', 'http://www.wikidata.org/entity/Q808916', 'http://www.wikidata.org/entity/Q861545', 'http://www.wikidata.org/entity/Q861938', 'http://www.wikidata.org/entity/Q870113', 'http://www.wikidata.org/entity/Q887760', 'http://www.wikidata.org/entity/Q888472', 'http://www.wikidata.org/entity/Q888620', 'http://www.wikidata.org/entity/Q888671', 'http://www.wikidata.org/entity/Q895829', 'http://www.wikidata.org/entity/Q923409', 'http://www.wikidata.org/entity/Q93341', 'http://www.wikidata.org/entity/Q936536', 'http://www.wikidata.org/entity/Q973166', 'http://www.wikidata.org/entity/Q975609', 'http://www.wikidata.org/entity/Q98308750', 'http://www.wikidata.org/entity/Q99438820']</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q100249671', 'http://www.wikidata.org/entity/Q1026959', 'http://www.wikidata.org/entity/Q1027629', 'http://www.wikidata.org/entity/Q1036753', 'http://www.wikidata.org/entity/Q1039172', 'http://www.wikidata.org/entity/Q1050088', 'http://www.wikidata.org/entity/Q106959617', 'http://www.wikidata.org/entity/Q109094', 'http://www.wikidata.org/entity/Q110182609', 'http://www.wikidata.org/entity/Q1103685', 'http://www.wikidata.org/entity/Q11290964', 'http://www.wikidata.org/entity/Q1138796', 'http://www.wikidata.org/entity/Q11409656', 'http://www.wikidata.org/entity/Q11473196', 'http://www.wikidata.org/entity/Q116745984', 'http://www.wikidata.org/entity/Q1173729', 'http://www.wikidata.org/entity/Q1238872', 'http://www.wikidata.org/entity/Q124042030', 'http://www.wikidata.org/entity/Q12469951', 'http://www.wikidata.org/entity/Q1248972', 'http://www.wikidata.org/entity/Q1266275', 'http://www.wikidata.org/entity/Q1282429', 'http://www.wikidata.org/entity/Q1282945', 'http://www.wikidata.org/entity/Q1282967', 'http://www.wikidata.org/entity/Q130324694', 'http://www.wikidata.org/entity/Q1308870', 'http://www.wikidata.org/entity/Q1311188', 'http://www.wikidata.org/entity/Q1318323', 'http://www.wikidata.org/entity/Q1347472', 'http://www.wikidata.org/entity/Q13571046', 'http://www.wikidata.org/entity/Q13571677', 'http://www.wikidata.org/entity/Q1364120', 'http://www.wikidata.org/entity/Q1412239', 'http://www.wikidata.org/entity/Q144622', 'http://www.wikidata.org/entity/Q1452661', 'http://www.wikidata.org/entity/Q1453118', 'http://www.wikidata.org/entity/Q14545268', 'http://www.wikidata.org/entity/Q1454645', 'http://www.wikidata.org/entity/Q1535887', 'http://www.wikidata.org/entity/Q15453836', 'http://www.wikidata.org/entity/Q15485363', 'http://www.wikidata.org/entity/Q1557440', 'http://www.wikidata.org/entity/Q15815145', 'http://www.wikidata.org/entity/Q1583816', 'http://www.wikidata.org/entity/Q15840407', 'http://www.wikidata.org/entity/Q15851160', 'http://www.wikidata.org/entity/Q16017359', 'http://www.wikidata.org/entity/Q1607887', 'http://www.wikidata.org/entity/Q16090563', 'http://www.wikidata.org/entity/Q161753', 'http://www.wikidata.org/entity/Q1622068', 'http://www.wikidata.org/entity/Q1631802', 'http://www.wikidata.org/entity/Q163861', 'http://www.wikidata.org/entity/Q1675549', 'http://www.wikidata.org/entity/Q1678838', 'http://www.wikidata.org/entity/Q1687893', 'http://www.wikidata.org/entity/Q1689131', 'http://www.wikidata.org/entity/Q1689347', 'http://www.wikidata.org/entity/Q1691548', 'http://www.wikidata.org/entity/Q1701204', 'http://www.wikidata.org/entity/Q1701748', 'http://www.wikidata.org/entity/Q1702274', 'http://www.wikidata.org/entity/Q1703633', 'http://www.wikidata.org/entity/Q17306038', 'http://www.wikidata.org/entity/Q17352853', 'http://www.wikidata.org/entity/Q1738588', 'http://www.wikidata.org/entity/Q1738949', 'http://www.wikidata.org/entity/Q1740093', 'http://www.wikidata.org/entity/Q1745395', 'http://www.wikidata.org/entity/Q177824', 'http://www.wikidata.org/entity/Q1779', 'http://www.wikidata.org/entity/Q1791341', 'http://www.wikidata.org/entity/Q1806037', 'http://www.wikidata.org/entity/Q1820504', 'http://www.wikidata.org/entity/Q18410973', 'http://www.wikidata.org/entity/Q1872759', 'http://www.wikidata.org/entity/Q188046', 'http://www.wikidata.org/entity/Q1902146', 'http://www.wikidata.org/entity/Q1903353', 'http://www.wikidata.org/entity/Q1912807', 'http://www.wikidata.org/entity/Q1917393', 'http://www.wikidata.org/entity/Q19275122', 'http://www.wikidata.org/entity/Q1935815', 'http://www.wikidata.org/entity/Q193645', 'http://www.wikidata.org/entity/Q19561422', 'http://www.wikidata.org/entity/Q19629147', 'http://www.wikidata.org/entity/Q1971146', 'http://www.wikidata.org/entity/Q19832476', 'http://www.wikidata.org/entity/Q199406', 'http://www.wikidata.org/entity/Q19960682', 'http://www.wikidata.org/entity/Q19962541', 'http://www.wikidata.org/entity/Q19968522', 'http://www.wikidata.org/entity/Q201500', 'http://www.wikidata.org/entity/Q2041252', 'http://www.wikidata.org/entity/Q204943', 'http://www.wikidata.org/entity/Q2061143', 'http://www.wikidata.org/entity/Q2075755', 'http://www.wikidata.org/entity/Q210173', 'http://www.wikidata.org/entity/Q210289', 'http://www.wikidata.org/entity/Q2216444', 'http://www.wikidata.org/entity/Q222798', 'http://www.wikidata.org/entity/Q22670541', 'http://www.wikidata.org/entity/Q22958430', 'http://www.wikidata.org/entity/Q2302261', 'http://www.wikidata.org/entity/Q2347504', 'http://www.wikidata.org/entity/Q23874600', 'http://www.wikidata.org/entity/Q2396601', 'http://www.wikidata.org/entity/Q2401961', 'http://www.wikidata.org/entity/Q2405288', 'http://www.wikidata.org/entity/Q2478090', 'http://www.wikidata.org/entity/Q2544934', 'http://www.wikidata.org/entity/Q26196818', 'http://www.wikidata.org/entity/Q2645829', 'http://www.wikidata.org/entity/Q2686238', 'http://www.wikidata.org/entity/Q273076', 'http://www.wikidata.org/entity/Q276068', 'http://www.wikidata.org/entity/Q27916182', 'http://www.wikidata.org/entity/Q313368', 'http://www.wikidata.org/entity/Q313529', 'http://www.wikidata.org/entity/Q313868', 'http://www.wikidata.org/entity/Q3196381', 'http://www.wikidata.org/entity/Q322210', 'http://www.wikidata.org/entity/Q329362', 'http://www.wikidata.org/entity/Q344822', 'http://www.wikidata.org/entity/Q355481', 'http://www.wikidata.org/entity/Q356715', 'http://www.wikidata.org/entity/Q376146', 'http://www.wikidata.org/entity/Q432924', 'http://www.wikidata.org/entity/Q436176', 'http://www.wikidata.org/entity/Q465105', 'http://www.wikidata.org/entity/Q4760598', 'http://www.wikidata.org/entity/Q4767267', 'http://www.wikidata.org/entity/Q4797599', 'http://www.wikidata.org/entity/Q4833896', 'http://www.wikidata.org/entity/Q491100', 'http://www.wikidata.org/entity/Q4911881', 'http://www.wikidata.org/entity/Q492677', 'http://www.wikidata.org/entity/Q495464', 'http://www.wikidata.org/entity/Q49575', 'http://www.wikidata.org/entity/Q4998586', 'http://www.wikidata.org/entity/Q510651', 'http://www.wikidata.org/entity/Q5214487', 'http://www.wikidata.org/entity/Q5220273', 'http://www.wikidata.org/entity/Q523899', 'http://www.wikidata.org/entity/Q5263018', 'http://www.wikidata.org/entity/Q528340', 'http://www.wikidata.org/entity/Q5290919', 'http://www.wikidata.org/entity/Q539159', 'http://www.wikidata.org/entity/Q5392650', 'http://www.wikidata.org/entity/Q5394010', 'http://www.wikidata.org/entity/Q539883', 'http://www.wikidata.org/entity/Q545464', 'http://www.wikidata.org/entity/Q54957569', 'http://www.wikidata.org/entity/Q5508594', 'http://www.wikidata.org/entity/Q5525190', 'http://www.wikidata.org/entity/Q5531061', 'http://www.wikidata.org/entity/Q558118', 'http://www.wikidata.org/entity/Q562871', 'http://www.wikidata.org/entity/Q5736141', 'http://www.wikidata.org/entity/Q590792', 'http://www.wikidata.org/entity/Q600700', 'http://www.wikidata.org/entity/Q6074256', 'http://www.wikidata.org/entity/Q612855', 'http://www.wikidata.org/entity/Q6175185', 'http://www.wikidata.org/entity/Q6208919', 'http://www.wikidata.org/entity/Q6221178', 'http://www.wikidata.org/entity/Q6224104', 'http://www.wikidata.org/entity/Q6240203', 'http://www.wikidata.org/entity/Q6309190', 'http://www.wikidata.org/entity/Q64683137', 'http://www.wikidata.org/entity/Q64985242', 'http://www.wikidata.org/entity/Q65028314', 'http://www.wikidata.org/entity/Q65028506', 'http://www.wikidata.org/entity/Q65032384', 'http://www.wikidata.org/entity/Q65034989', 'http://www.wikidata.org/entity/Q65034994', 'http://www.wikidata.org/entity/Q658636', 'http://www.wikidata.org/entity/Q6687998', 'http://www.wikidata.org/entity/Q668856', 'http://www.wikidata.org/entity/Q675810', 'http://www.wikidata.org/entity/Q6793340', 'http://www.wikidata.org/entity/Q6846424', 'http://www.wikidata.org/entity/Q6849142', 'http://www.wikidata.org/entity/Q7052586', 'http://www.wikidata.org/entity/Q70552207', 'http://www.wikidata.org/entity/Q7087874', 'http://www.wikidata.org/entity/Q708990', 'http://www.wikidata.org/entity/Q711921', 'http://www.wikidata.org/entity/Q713273', 'http://www.wikidata.org/entity/Q727418', 'http://www.wikidata.org/entity/Q7298839', 'http://www.wikidata.org/entity/Q737521', 'http://www.wikidata.org/entity/Q743585', 'http://www.wikidata.org/entity/Q7441108', 'http://www.wikidata.org/entity/Q7524109', 'http://www.wikidata.org/entity/Q7614243', 'http://www.wikidata.org/entity/Q7694080', 'http://www.wikidata.org/entity/Q772645', 'http://www.wikidata.org/entity/Q776453', 'http://www.wikidata.org/entity/Q7781439', 'http://www.wikidata.org/entity/Q7781727', 'http://www.wikidata.org/entity/Q7924906', 'http://www.wikidata.org/entity/Q7982390', 'http://www.wikidata.org/entity/Q8009347', 'http://www.wikidata.org/entity/Q807401', 'http://www.wikidata.org/entity/Q808916', 'http://www.wikidata.org/entity/Q861545', 'http://www.wikidata.org/entity/Q861938', 'http://www.wikidata.org/entity/Q870113', 'http://www.wikidata.org/entity/Q887760', 'http://www.wikidata.org/entity/Q888472', 'http://www.wikidata.org/entity/Q888620', 'http://www.wikidata.org/entity/Q888671', 'http://www.wikidata.org/entity/Q895829', 'http://www.wikidata.org/entity/Q923409', 'http://www.wikidata.org/entity/Q93341', 'http://www.wikidata.org/entity/Q936536', 'http://www.wikidata.org/entity/Q973166', 'http://www.wikidata.org/entity/Q975609', 'http://www.wikidata.org/entity/Q98308750', 'http://www.wikidata.org/entity/Q99438820']</t>
+        </is>
+      </c>
+      <c r="D34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>In which films did Julia Roberts as well as Richard Gere play?</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q1160813', 'http://www.wikidata.org/entity/Q207954']</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q1160813', 'http://www.wikidata.org/entity/Q207954']</t>
+        </is>
+      </c>
+      <c r="D35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>What is the capital of Canada?</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q1930']</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q3876']</t>
+        </is>
+      </c>
+      <c r="D36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>How much is the population of mexico city ?</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>['9209944']</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>['9209944']</t>
+        </is>
+      </c>
+      <c r="D37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Who created Batman?</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q313048', 'http://www.wikidata.org/entity/Q464282']</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q313048', 'http://www.wikidata.org/entity/Q464282']</t>
+        </is>
+      </c>
+      <c r="D38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>how big is the total area of North Rhine- Westphalia?</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>['34112.5']</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>['34112.5']</t>
+        </is>
+      </c>
+      <c r="D39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>How many employees does IBM have?</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>['352600']</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>['352600']</t>
+        </is>
+      </c>
+      <c r="D40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>What movies does Jesse Eisenberg play in?</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q100724914', 'http://www.wikidata.org/entity/Q104714221', 'http://www.wikidata.org/entity/Q110060321', 'http://www.wikidata.org/entity/Q110060323', 'http://www.wikidata.org/entity/Q111950685', 'http://www.wikidata.org/entity/Q116314289', 'http://www.wikidata.org/entity/Q1197427', 'http://www.wikidata.org/entity/Q12126557', 'http://www.wikidata.org/entity/Q12133175', 'http://www.wikidata.org/entity/Q123690193', 'http://www.wikidata.org/entity/Q1467522', 'http://www.wikidata.org/entity/Q14772351', 'http://www.wikidata.org/entity/Q1503896', 'http://www.wikidata.org/entity/Q15270846', 'http://www.wikidata.org/entity/Q16250123', 'http://www.wikidata.org/entity/Q16354845', 'http://www.wikidata.org/entity/Q1753498', 'http://www.wikidata.org/entity/Q18151930', 'http://www.wikidata.org/entity/Q185888', 'http://www.wikidata.org/entity/Q18703028', 'http://www.wikidata.org/entity/Q20501835', 'http://www.wikidata.org/entity/Q20950014', 'http://www.wikidata.org/entity/Q219810', 'http://www.wikidata.org/entity/Q224133', 'http://www.wikidata.org/entity/Q261899', 'http://www.wikidata.org/entity/Q29658', 'http://www.wikidata.org/entity/Q3087286', 'http://www.wikidata.org/entity/Q3178485', 'http://www.wikidata.org/entity/Q37909451', 'http://www.wikidata.org/entity/Q379994', 'http://www.wikidata.org/entity/Q3986749', 'http://www.wikidata.org/entity/Q44613088', 'http://www.wikidata.org/entity/Q465227', 'http://www.wikidata.org/entity/Q474246', 'http://www.wikidata.org/entity/Q49001848', 'http://www.wikidata.org/entity/Q499851', 'http://www.wikidata.org/entity/Q58879016', 'http://www.wikidata.org/entity/Q60737594', 'http://www.wikidata.org/entity/Q63352785', 'http://www.wikidata.org/entity/Q769453', 'http://www.wikidata.org/entity/Q7730725', 'http://www.wikidata.org/entity/Q7747903', 'http://www.wikidata.org/entity/Q94998134', 'http://www.wikidata.org/entity/Q978927']</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q100724914', 'http://www.wikidata.org/entity/Q104714221', 'http://www.wikidata.org/entity/Q110060321', 'http://www.wikidata.org/entity/Q110060323', 'http://www.wikidata.org/entity/Q111950685', 'http://www.wikidata.org/entity/Q116314289', 'http://www.wikidata.org/entity/Q1197427', 'http://www.wikidata.org/entity/Q12126557', 'http://www.wikidata.org/entity/Q12133175', 'http://www.wikidata.org/entity/Q123690193', 'http://www.wikidata.org/entity/Q1467522', 'http://www.wikidata.org/entity/Q14772351', 'http://www.wikidata.org/entity/Q1503896', 'http://www.wikidata.org/entity/Q15270846', 'http://www.wikidata.org/entity/Q16250123', 'http://www.wikidata.org/entity/Q16354845', 'http://www.wikidata.org/entity/Q1753498', 'http://www.wikidata.org/entity/Q18151930', 'http://www.wikidata.org/entity/Q185888', 'http://www.wikidata.org/entity/Q18703028', 'http://www.wikidata.org/entity/Q20501835', 'http://www.wikidata.org/entity/Q20950014', 'http://www.wikidata.org/entity/Q219810', 'http://www.wikidata.org/entity/Q224133', 'http://www.wikidata.org/entity/Q261899', 'http://www.wikidata.org/entity/Q29658', 'http://www.wikidata.org/entity/Q3087286', 'http://www.wikidata.org/entity/Q3178485', 'http://www.wikidata.org/entity/Q37909451', 'http://www.wikidata.org/entity/Q379994', 'http://www.wikidata.org/entity/Q3986749', 'http://www.wikidata.org/entity/Q44613088', 'http://www.wikidata.org/entity/Q465227', 'http://www.wikidata.org/entity/Q474246', 'http://www.wikidata.org/entity/Q49001848', 'http://www.wikidata.org/entity/Q499851', 'http://www.wikidata.org/entity/Q58879016', 'http://www.wikidata.org/entity/Q60737594', 'http://www.wikidata.org/entity/Q63352785', 'http://www.wikidata.org/entity/Q769453', 'http://www.wikidata.org/entity/Q7730725', 'http://www.wikidata.org/entity/Q7747903', 'http://www.wikidata.org/entity/Q94998134', 'http://www.wikidata.org/entity/Q978927']</t>
+        </is>
+      </c>
+      <c r="D41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>What is the alma mater of the chancellor of Germany Angela Merkel?</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q154804', 'http://www.wikidata.org/entity/Q154804']</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q154804', 'http://www.wikidata.org/entity/Q49738', 'http://www.wikidata.org/entity/Q56230681', 'http://www.wikidata.org/entity/Q56230686']</t>
+        </is>
+      </c>
+      <c r="D42" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>